<commit_message>
Added functionality for player stats summary excel export
</commit_message>
<xml_diff>
--- a/backend/excels/game_stats_template.xlsx
+++ b/backend/excels/game_stats_template.xlsx
@@ -497,7 +497,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -816,6 +816,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -2332,17 +2336,17 @@
       <c r="A32" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="B32" s="0"/>
-      <c r="C32" s="0"/>
-      <c r="D32" s="0"/>
-      <c r="E32" s="0"/>
-      <c r="F32" s="0"/>
-      <c r="G32" s="0"/>
-      <c r="H32" s="0"/>
-      <c r="I32" s="0"/>
-      <c r="J32" s="0"/>
-      <c r="K32" s="0"/>
-      <c r="L32" s="0"/>
+      <c r="B32" s="80"/>
+      <c r="C32" s="80"/>
+      <c r="D32" s="80"/>
+      <c r="E32" s="80"/>
+      <c r="F32" s="80"/>
+      <c r="G32" s="80"/>
+      <c r="H32" s="80"/>
+      <c r="I32" s="80"/>
+      <c r="J32" s="80"/>
+      <c r="K32" s="80"/>
+      <c r="L32" s="80"/>
       <c r="M32" s="77"/>
       <c r="N32" s="77"/>
       <c r="O32" s="77"/>
@@ -2350,30 +2354,30 @@
       <c r="Q32" s="77"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="80" t="s">
+      <c r="A33" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="B33" s="81" t="s">
+      <c r="B33" s="82" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="81"/>
-      <c r="D33" s="82" t="s">
+      <c r="C33" s="82"/>
+      <c r="D33" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="E33" s="82"/>
-      <c r="F33" s="82" t="s">
+      <c r="E33" s="83"/>
+      <c r="F33" s="83" t="s">
         <v>52</v>
       </c>
-      <c r="G33" s="82"/>
-      <c r="H33" s="83" t="s">
+      <c r="G33" s="83"/>
+      <c r="H33" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="I33" s="83"/>
-      <c r="J33" s="84" t="s">
+      <c r="I33" s="84"/>
+      <c r="J33" s="85" t="s">
         <v>54</v>
       </c>
-      <c r="K33" s="84"/>
-      <c r="L33" s="0"/>
+      <c r="K33" s="85"/>
+      <c r="L33" s="80"/>
       <c r="M33" s="77"/>
       <c r="N33" s="77"/>
       <c r="O33" s="77"/>
@@ -2381,7 +2385,7 @@
       <c r="Q33" s="77"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="85" t="s">
+      <c r="A34" s="86" t="s">
         <v>17</v>
       </c>
       <c r="B34" s="24" t="s">
@@ -2414,10 +2418,10 @@
       <c r="K34" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="L34" s="0"/>
+      <c r="L34" s="80"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="85" t="s">
+      <c r="A35" s="86" t="s">
         <v>20</v>
       </c>
       <c r="B35" s="26" t="n">
@@ -2450,7 +2454,7 @@
       <c r="K35" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="L35" s="0"/>
+      <c r="L35" s="80"/>
       <c r="M35" s="19"/>
       <c r="N35" s="19"/>
       <c r="O35" s="19"/>
@@ -2458,7 +2462,7 @@
       <c r="Q35" s="19"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="85" t="s">
+      <c r="A36" s="86" t="s">
         <v>21</v>
       </c>
       <c r="B36" s="26" t="n">
@@ -2491,57 +2495,57 @@
       <c r="K36" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="L36" s="0"/>
+      <c r="L36" s="80"/>
       <c r="O36" s="41"/>
       <c r="P36" s="41"/>
       <c r="Q36" s="41"/>
-      <c r="R36" s="86"/>
+      <c r="R36" s="87"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="87" t="s">
+      <c r="A37" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="88" t="n">
+      <c r="B37" s="89" t="n">
         <f aca="false">IFERROR(B36 / B35,0)</f>
         <v>0</v>
       </c>
-      <c r="C37" s="89" t="n">
+      <c r="C37" s="90" t="n">
         <f aca="false">IFERROR(C36 / C35,0)</f>
         <v>0</v>
       </c>
-      <c r="D37" s="88" t="n">
+      <c r="D37" s="89" t="n">
         <f aca="false">IFERROR(D36 / D35,0)</f>
         <v>0</v>
       </c>
-      <c r="E37" s="90" t="n">
+      <c r="E37" s="91" t="n">
         <f aca="false">IFERROR(E36 / E35,0)</f>
         <v>0</v>
       </c>
-      <c r="F37" s="89" t="n">
+      <c r="F37" s="90" t="n">
         <f aca="false">IFERROR(F36 / F35,0)</f>
         <v>0</v>
       </c>
-      <c r="G37" s="89" t="n">
+      <c r="G37" s="90" t="n">
         <f aca="false">IFERROR(G36 / G35,0)</f>
         <v>0</v>
       </c>
-      <c r="H37" s="88" t="n">
+      <c r="H37" s="89" t="n">
         <f aca="false">IFERROR(H36 / H35,0)</f>
         <v>0</v>
       </c>
-      <c r="I37" s="90" t="n">
+      <c r="I37" s="91" t="n">
         <f aca="false">IFERROR(I36 / I35,0)</f>
         <v>0</v>
       </c>
-      <c r="J37" s="89" t="n">
+      <c r="J37" s="90" t="n">
         <f aca="false">IFERROR(J36 / J35,0)</f>
         <v>0</v>
       </c>
-      <c r="K37" s="90" t="n">
+      <c r="K37" s="91" t="n">
         <f aca="false">IFERROR(K36 / K35,0)</f>
         <v>0</v>
       </c>
-      <c r="L37" s="0"/>
+      <c r="L37" s="80"/>
       <c r="M37" s="78"/>
       <c r="N37" s="77"/>
       <c r="O37" s="77"/>
@@ -2576,18 +2580,18 @@
       <c r="AR37" s="19"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="80" t="s">
+      <c r="A38" s="81" t="s">
         <v>55</v>
       </c>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
-      <c r="D38" s="91" t="str">
+      <c r="D38" s="92" t="str">
         <f aca="false">O1</f>
         <v>YV Kerrat:</v>
       </c>
       <c r="E38" s="14"/>
       <c r="F38" s="14"/>
-      <c r="G38" s="91" t="str">
+      <c r="G38" s="92" t="str">
         <f aca="false">Q1</f>
         <v>AV Kerrat:</v>
       </c>
@@ -2595,7 +2599,7 @@
       <c r="I38" s="14"/>
       <c r="J38" s="14"/>
       <c r="K38" s="14"/>
-      <c r="L38" s="0"/>
+      <c r="L38" s="80"/>
       <c r="M38" s="77"/>
       <c r="N38" s="77"/>
       <c r="O38" s="77"/>
@@ -2630,24 +2634,24 @@
       <c r="AR38" s="19"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="87" t="s">
+      <c r="A39" s="88" t="s">
         <v>56</v>
       </c>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
-      <c r="D39" s="92" t="n">
+      <c r="D39" s="93" t="n">
         <f aca="false">IFERROR(D35 / D38,0)</f>
         <v>0</v>
       </c>
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
-      <c r="G39" s="92" t="n">
+      <c r="G39" s="93" t="n">
         <f aca="false">IFERROR(G35 / G38,0)</f>
         <v>0</v>
       </c>
       <c r="H39" s="13"/>
-      <c r="I39" s="93"/>
-      <c r="J39" s="93"/>
+      <c r="I39" s="94"/>
+      <c r="J39" s="94"/>
       <c r="K39" s="13"/>
       <c r="M39" s="77"/>
       <c r="N39" s="77"/>
@@ -2718,31 +2722,31 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="S41" s="19"/>
-      <c r="T41" s="94"/>
-      <c r="U41" s="94"/>
-      <c r="V41" s="94"/>
-      <c r="W41" s="94"/>
-      <c r="X41" s="94"/>
-      <c r="Y41" s="94"/>
-      <c r="Z41" s="94"/>
-      <c r="AA41" s="94"/>
-      <c r="AB41" s="94"/>
-      <c r="AC41" s="94"/>
-      <c r="AD41" s="94"/>
-      <c r="AE41" s="94"/>
+      <c r="T41" s="95"/>
+      <c r="U41" s="95"/>
+      <c r="V41" s="95"/>
+      <c r="W41" s="95"/>
+      <c r="X41" s="95"/>
+      <c r="Y41" s="95"/>
+      <c r="Z41" s="95"/>
+      <c r="AA41" s="95"/>
+      <c r="AB41" s="95"/>
+      <c r="AC41" s="95"/>
+      <c r="AD41" s="95"/>
+      <c r="AE41" s="95"/>
       <c r="AF41" s="19"/>
-      <c r="AG41" s="94"/>
-      <c r="AH41" s="94"/>
-      <c r="AI41" s="94"/>
-      <c r="AJ41" s="94"/>
-      <c r="AK41" s="94"/>
-      <c r="AL41" s="94"/>
-      <c r="AM41" s="94"/>
-      <c r="AN41" s="94"/>
-      <c r="AO41" s="94"/>
-      <c r="AP41" s="94"/>
-      <c r="AQ41" s="94"/>
-      <c r="AR41" s="94"/>
+      <c r="AG41" s="95"/>
+      <c r="AH41" s="95"/>
+      <c r="AI41" s="95"/>
+      <c r="AJ41" s="95"/>
+      <c r="AK41" s="95"/>
+      <c r="AL41" s="95"/>
+      <c r="AM41" s="95"/>
+      <c r="AN41" s="95"/>
+      <c r="AO41" s="95"/>
+      <c r="AP41" s="95"/>
+      <c r="AQ41" s="95"/>
+      <c r="AR41" s="95"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="18"/>
@@ -3588,7 +3592,7 @@
       <c r="A66" s="19"/>
       <c r="C66" s="19"/>
       <c r="D66" s="19"/>
-      <c r="E66" s="95" t="str">
+      <c r="E66" s="96" t="str">
         <f aca="false">IFERROR(C66 / D66, "")</f>
         <v/>
       </c>
@@ -3596,7 +3600,7 @@
       <c r="G66" s="19"/>
       <c r="I66" s="19"/>
       <c r="J66" s="19"/>
-      <c r="K66" s="95" t="str">
+      <c r="K66" s="96" t="str">
         <f aca="false">IFERROR(I66 / J66, "")</f>
         <v/>
       </c>
@@ -3604,7 +3608,7 @@
       <c r="M66" s="19"/>
       <c r="O66" s="19"/>
       <c r="P66" s="19"/>
-      <c r="Q66" s="95" t="str">
+      <c r="Q66" s="96" t="str">
         <f aca="false">IFERROR(O66 / P66, "")</f>
         <v/>
       </c>
@@ -3612,35 +3616,35 @@
       <c r="S66" s="19"/>
       <c r="U66" s="19"/>
       <c r="V66" s="19"/>
-      <c r="W66" s="95" t="str">
+      <c r="W66" s="96" t="str">
         <f aca="false">IFERROR(U66 / V66, "")</f>
         <v/>
       </c>
       <c r="X66" s="19"/>
       <c r="Z66" s="19"/>
       <c r="AA66" s="19"/>
-      <c r="AB66" s="95" t="str">
+      <c r="AB66" s="96" t="str">
         <f aca="false">IFERROR(Z66 / AA66, "")</f>
         <v/>
       </c>
       <c r="AC66" s="19"/>
       <c r="AE66" s="19"/>
       <c r="AF66" s="19"/>
-      <c r="AG66" s="95" t="str">
+      <c r="AG66" s="96" t="str">
         <f aca="false">IFERROR(AE66 / AF66, "")</f>
         <v/>
       </c>
       <c r="AH66" s="19"/>
       <c r="AJ66" s="19"/>
       <c r="AK66" s="19"/>
-      <c r="AL66" s="95" t="str">
+      <c r="AL66" s="96" t="str">
         <f aca="false">IFERROR(AJ66 / AK66, "")</f>
         <v/>
       </c>
       <c r="AM66" s="19"/>
       <c r="AO66" s="19"/>
       <c r="AP66" s="19"/>
-      <c r="AQ66" s="95" t="str">
+      <c r="AQ66" s="96" t="str">
         <f aca="false">IFERROR(AO66 / AP66, "")</f>
         <v/>
       </c>
@@ -5121,8 +5125,8 @@
   </sheetPr>
   <dimension ref="A1:AR114"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5142,14 +5146,14 @@
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
       <c r="F1" s="15"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
       <c r="J1" s="42"/>
       <c r="K1" s="42"/>
       <c r="L1" s="42"/>
-      <c r="M1" s="96"/>
-      <c r="N1" s="96"/>
+      <c r="M1" s="97"/>
+      <c r="N1" s="97"/>
       <c r="O1" s="18"/>
       <c r="P1" s="19"/>
       <c r="Q1" s="18"/>
@@ -5950,7 +5954,7 @@
       <c r="A19" s="52"/>
       <c r="B19" s="53"/>
       <c r="C19" s="54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="55" t="n">
         <v>0</v>
@@ -5961,7 +5965,7 @@
       <c r="F19" s="57"/>
       <c r="G19" s="58"/>
       <c r="H19" s="54" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I19" s="55" t="n">
         <v>0</v>
@@ -5973,7 +5977,7 @@
       <c r="L19" s="58"/>
       <c r="M19" s="60" t="n">
         <f aca="false">IFERROR(C19 / H19,0)</f>
-        <v>0</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="N19" s="61" t="n">
         <f aca="false">IFERROR(D19 / I19,0)</f>
@@ -6358,17 +6362,17 @@
       <c r="A32" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="B32" s="0"/>
-      <c r="C32" s="0"/>
-      <c r="D32" s="0"/>
-      <c r="E32" s="0"/>
-      <c r="F32" s="0"/>
-      <c r="G32" s="0"/>
-      <c r="H32" s="0"/>
-      <c r="I32" s="0"/>
-      <c r="J32" s="0"/>
-      <c r="K32" s="0"/>
-      <c r="L32" s="0"/>
+      <c r="B32" s="80"/>
+      <c r="C32" s="80"/>
+      <c r="D32" s="80"/>
+      <c r="E32" s="80"/>
+      <c r="F32" s="80"/>
+      <c r="G32" s="80"/>
+      <c r="H32" s="80"/>
+      <c r="I32" s="80"/>
+      <c r="J32" s="80"/>
+      <c r="K32" s="80"/>
+      <c r="L32" s="80"/>
       <c r="M32" s="77"/>
       <c r="N32" s="77"/>
       <c r="O32" s="77"/>
@@ -6376,30 +6380,30 @@
       <c r="Q32" s="77"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="80" t="s">
+      <c r="A33" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="B33" s="81" t="s">
+      <c r="B33" s="82" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="81"/>
-      <c r="D33" s="82" t="s">
+      <c r="C33" s="82"/>
+      <c r="D33" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="E33" s="82"/>
-      <c r="F33" s="82" t="s">
+      <c r="E33" s="83"/>
+      <c r="F33" s="83" t="s">
         <v>52</v>
       </c>
-      <c r="G33" s="82"/>
-      <c r="H33" s="83" t="s">
+      <c r="G33" s="83"/>
+      <c r="H33" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="I33" s="83"/>
-      <c r="J33" s="84" t="s">
+      <c r="I33" s="84"/>
+      <c r="J33" s="85" t="s">
         <v>54</v>
       </c>
-      <c r="K33" s="84"/>
-      <c r="L33" s="0"/>
+      <c r="K33" s="85"/>
+      <c r="L33" s="80"/>
       <c r="M33" s="77"/>
       <c r="N33" s="77"/>
       <c r="O33" s="77"/>
@@ -6407,7 +6411,7 @@
       <c r="Q33" s="77"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="85" t="s">
+      <c r="A34" s="86" t="s">
         <v>17</v>
       </c>
       <c r="B34" s="24" t="s">
@@ -6440,10 +6444,10 @@
       <c r="K34" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="L34" s="0"/>
+      <c r="L34" s="80"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="85" t="s">
+      <c r="A35" s="86" t="s">
         <v>20</v>
       </c>
       <c r="B35" s="26" t="n">
@@ -6476,7 +6480,7 @@
       <c r="K35" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="L35" s="0"/>
+      <c r="L35" s="80"/>
       <c r="M35" s="19"/>
       <c r="N35" s="19"/>
       <c r="O35" s="19"/>
@@ -6484,7 +6488,7 @@
       <c r="Q35" s="19"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="85" t="s">
+      <c r="A36" s="86" t="s">
         <v>21</v>
       </c>
       <c r="B36" s="26" t="n">
@@ -6517,57 +6521,57 @@
       <c r="K36" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="L36" s="0"/>
+      <c r="L36" s="80"/>
       <c r="O36" s="41"/>
       <c r="P36" s="41"/>
       <c r="Q36" s="41"/>
-      <c r="R36" s="86"/>
+      <c r="R36" s="87"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="87" t="s">
+      <c r="A37" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="88" t="n">
+      <c r="B37" s="89" t="n">
         <f aca="false">IFERROR(B36 / B35,0)</f>
         <v>0</v>
       </c>
-      <c r="C37" s="89" t="n">
+      <c r="C37" s="90" t="n">
         <f aca="false">IFERROR(C36 / C35,0)</f>
         <v>0</v>
       </c>
-      <c r="D37" s="88" t="n">
+      <c r="D37" s="89" t="n">
         <f aca="false">IFERROR(D36 / D35,0)</f>
         <v>0</v>
       </c>
-      <c r="E37" s="90" t="n">
+      <c r="E37" s="91" t="n">
         <f aca="false">IFERROR(E36 / E35,0)</f>
         <v>0</v>
       </c>
-      <c r="F37" s="89" t="n">
+      <c r="F37" s="90" t="n">
         <f aca="false">IFERROR(F36 / F35,0)</f>
         <v>0</v>
       </c>
-      <c r="G37" s="89" t="n">
+      <c r="G37" s="90" t="n">
         <f aca="false">IFERROR(G36 / G35,0)</f>
         <v>0</v>
       </c>
-      <c r="H37" s="88" t="n">
+      <c r="H37" s="89" t="n">
         <f aca="false">IFERROR(H36 / H35,0)</f>
         <v>0</v>
       </c>
-      <c r="I37" s="90" t="n">
+      <c r="I37" s="91" t="n">
         <f aca="false">IFERROR(I36 / I35,0)</f>
         <v>0</v>
       </c>
-      <c r="J37" s="89" t="n">
+      <c r="J37" s="90" t="n">
         <f aca="false">IFERROR(J36 / J35,0)</f>
         <v>0</v>
       </c>
-      <c r="K37" s="90" t="n">
+      <c r="K37" s="91" t="n">
         <f aca="false">IFERROR(K36 / K35,0)</f>
         <v>0</v>
       </c>
-      <c r="L37" s="0"/>
+      <c r="L37" s="80"/>
       <c r="M37" s="78"/>
       <c r="N37" s="77"/>
       <c r="O37" s="77"/>
@@ -6602,18 +6606,18 @@
       <c r="AR37" s="19"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="80" t="s">
+      <c r="A38" s="81" t="s">
         <v>55</v>
       </c>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
-      <c r="D38" s="91" t="n">
+      <c r="D38" s="92" t="n">
         <f aca="false">O1</f>
         <v>0</v>
       </c>
       <c r="E38" s="14"/>
       <c r="F38" s="14"/>
-      <c r="G38" s="91" t="n">
+      <c r="G38" s="92" t="n">
         <f aca="false">Q1</f>
         <v>0</v>
       </c>
@@ -6621,7 +6625,7 @@
       <c r="I38" s="14"/>
       <c r="J38" s="14"/>
       <c r="K38" s="14"/>
-      <c r="L38" s="0"/>
+      <c r="L38" s="80"/>
       <c r="M38" s="77"/>
       <c r="N38" s="77"/>
       <c r="O38" s="77"/>
@@ -6656,24 +6660,24 @@
       <c r="AR38" s="19"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="87" t="s">
+      <c r="A39" s="88" t="s">
         <v>56</v>
       </c>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
-      <c r="D39" s="92" t="n">
+      <c r="D39" s="93" t="n">
         <f aca="false">IFERROR(D35 / D38,0)</f>
         <v>0</v>
       </c>
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
-      <c r="G39" s="92" t="n">
+      <c r="G39" s="93" t="n">
         <f aca="false">IFERROR(G35 / G38,0)</f>
         <v>0</v>
       </c>
       <c r="H39" s="13"/>
-      <c r="I39" s="93"/>
-      <c r="J39" s="93"/>
+      <c r="I39" s="94"/>
+      <c r="J39" s="94"/>
       <c r="K39" s="13"/>
       <c r="M39" s="77"/>
       <c r="N39" s="77"/>
@@ -6744,31 +6748,31 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="S41" s="19"/>
-      <c r="T41" s="94"/>
-      <c r="U41" s="94"/>
-      <c r="V41" s="94"/>
-      <c r="W41" s="94"/>
-      <c r="X41" s="94"/>
-      <c r="Y41" s="94"/>
-      <c r="Z41" s="94"/>
-      <c r="AA41" s="94"/>
-      <c r="AB41" s="94"/>
-      <c r="AC41" s="94"/>
-      <c r="AD41" s="94"/>
-      <c r="AE41" s="94"/>
+      <c r="T41" s="95"/>
+      <c r="U41" s="95"/>
+      <c r="V41" s="95"/>
+      <c r="W41" s="95"/>
+      <c r="X41" s="95"/>
+      <c r="Y41" s="95"/>
+      <c r="Z41" s="95"/>
+      <c r="AA41" s="95"/>
+      <c r="AB41" s="95"/>
+      <c r="AC41" s="95"/>
+      <c r="AD41" s="95"/>
+      <c r="AE41" s="95"/>
       <c r="AF41" s="19"/>
-      <c r="AG41" s="94"/>
-      <c r="AH41" s="94"/>
-      <c r="AI41" s="94"/>
-      <c r="AJ41" s="94"/>
-      <c r="AK41" s="94"/>
-      <c r="AL41" s="94"/>
-      <c r="AM41" s="94"/>
-      <c r="AN41" s="94"/>
-      <c r="AO41" s="94"/>
-      <c r="AP41" s="94"/>
-      <c r="AQ41" s="94"/>
-      <c r="AR41" s="94"/>
+      <c r="AG41" s="95"/>
+      <c r="AH41" s="95"/>
+      <c r="AI41" s="95"/>
+      <c r="AJ41" s="95"/>
+      <c r="AK41" s="95"/>
+      <c r="AL41" s="95"/>
+      <c r="AM41" s="95"/>
+      <c r="AN41" s="95"/>
+      <c r="AO41" s="95"/>
+      <c r="AP41" s="95"/>
+      <c r="AQ41" s="95"/>
+      <c r="AR41" s="95"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="18"/>
@@ -7614,7 +7618,7 @@
       <c r="A66" s="19"/>
       <c r="C66" s="19"/>
       <c r="D66" s="19"/>
-      <c r="E66" s="95" t="str">
+      <c r="E66" s="96" t="str">
         <f aca="false">IFERROR(C66 / D66, "")</f>
         <v/>
       </c>
@@ -7622,7 +7626,7 @@
       <c r="G66" s="19"/>
       <c r="I66" s="19"/>
       <c r="J66" s="19"/>
-      <c r="K66" s="95" t="str">
+      <c r="K66" s="96" t="str">
         <f aca="false">IFERROR(I66 / J66, "")</f>
         <v/>
       </c>
@@ -7630,7 +7634,7 @@
       <c r="M66" s="19"/>
       <c r="O66" s="19"/>
       <c r="P66" s="19"/>
-      <c r="Q66" s="95" t="str">
+      <c r="Q66" s="96" t="str">
         <f aca="false">IFERROR(O66 / P66, "")</f>
         <v/>
       </c>
@@ -7638,35 +7642,35 @@
       <c r="S66" s="19"/>
       <c r="U66" s="19"/>
       <c r="V66" s="19"/>
-      <c r="W66" s="95" t="str">
+      <c r="W66" s="96" t="str">
         <f aca="false">IFERROR(U66 / V66, "")</f>
         <v/>
       </c>
       <c r="X66" s="19"/>
       <c r="Z66" s="19"/>
       <c r="AA66" s="19"/>
-      <c r="AB66" s="95" t="str">
+      <c r="AB66" s="96" t="str">
         <f aca="false">IFERROR(Z66 / AA66, "")</f>
         <v/>
       </c>
       <c r="AC66" s="19"/>
       <c r="AE66" s="19"/>
       <c r="AF66" s="19"/>
-      <c r="AG66" s="95" t="str">
+      <c r="AG66" s="96" t="str">
         <f aca="false">IFERROR(AE66 / AF66, "")</f>
         <v/>
       </c>
       <c r="AH66" s="19"/>
       <c r="AJ66" s="19"/>
       <c r="AK66" s="19"/>
-      <c r="AL66" s="95" t="str">
+      <c r="AL66" s="96" t="str">
         <f aca="false">IFERROR(AJ66 / AK66, "")</f>
         <v/>
       </c>
       <c r="AM66" s="19"/>
       <c r="AO66" s="19"/>
       <c r="AP66" s="19"/>
-      <c r="AQ66" s="95" t="str">
+      <c r="AQ66" s="96" t="str">
         <f aca="false">IFERROR(AO66 / AP66, "")</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
Implement functionality to export player summary excel. Also separated dev/prod db and backend (#11)
* Added support for scoring game excel exporting

* Added functionality for player stats summary excel export

* frontend changes

* BUGFIX: Merge conflict resolution left ExcelExporter.jsx with some duplicate code. Cleaned

* Small bugfixes removing duplicated code
</commit_message>
<xml_diff>
--- a/backend/excels/game_stats_template.xlsx
+++ b/backend/excels/game_stats_template.xlsx
@@ -497,7 +497,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -816,6 +816,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -2332,17 +2336,17 @@
       <c r="A32" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="B32" s="0"/>
-      <c r="C32" s="0"/>
-      <c r="D32" s="0"/>
-      <c r="E32" s="0"/>
-      <c r="F32" s="0"/>
-      <c r="G32" s="0"/>
-      <c r="H32" s="0"/>
-      <c r="I32" s="0"/>
-      <c r="J32" s="0"/>
-      <c r="K32" s="0"/>
-      <c r="L32" s="0"/>
+      <c r="B32" s="80"/>
+      <c r="C32" s="80"/>
+      <c r="D32" s="80"/>
+      <c r="E32" s="80"/>
+      <c r="F32" s="80"/>
+      <c r="G32" s="80"/>
+      <c r="H32" s="80"/>
+      <c r="I32" s="80"/>
+      <c r="J32" s="80"/>
+      <c r="K32" s="80"/>
+      <c r="L32" s="80"/>
       <c r="M32" s="77"/>
       <c r="N32" s="77"/>
       <c r="O32" s="77"/>
@@ -2350,30 +2354,30 @@
       <c r="Q32" s="77"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="80" t="s">
+      <c r="A33" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="B33" s="81" t="s">
+      <c r="B33" s="82" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="81"/>
-      <c r="D33" s="82" t="s">
+      <c r="C33" s="82"/>
+      <c r="D33" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="E33" s="82"/>
-      <c r="F33" s="82" t="s">
+      <c r="E33" s="83"/>
+      <c r="F33" s="83" t="s">
         <v>52</v>
       </c>
-      <c r="G33" s="82"/>
-      <c r="H33" s="83" t="s">
+      <c r="G33" s="83"/>
+      <c r="H33" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="I33" s="83"/>
-      <c r="J33" s="84" t="s">
+      <c r="I33" s="84"/>
+      <c r="J33" s="85" t="s">
         <v>54</v>
       </c>
-      <c r="K33" s="84"/>
-      <c r="L33" s="0"/>
+      <c r="K33" s="85"/>
+      <c r="L33" s="80"/>
       <c r="M33" s="77"/>
       <c r="N33" s="77"/>
       <c r="O33" s="77"/>
@@ -2381,7 +2385,7 @@
       <c r="Q33" s="77"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="85" t="s">
+      <c r="A34" s="86" t="s">
         <v>17</v>
       </c>
       <c r="B34" s="24" t="s">
@@ -2414,10 +2418,10 @@
       <c r="K34" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="L34" s="0"/>
+      <c r="L34" s="80"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="85" t="s">
+      <c r="A35" s="86" t="s">
         <v>20</v>
       </c>
       <c r="B35" s="26" t="n">
@@ -2450,7 +2454,7 @@
       <c r="K35" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="L35" s="0"/>
+      <c r="L35" s="80"/>
       <c r="M35" s="19"/>
       <c r="N35" s="19"/>
       <c r="O35" s="19"/>
@@ -2458,7 +2462,7 @@
       <c r="Q35" s="19"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="85" t="s">
+      <c r="A36" s="86" t="s">
         <v>21</v>
       </c>
       <c r="B36" s="26" t="n">
@@ -2491,57 +2495,57 @@
       <c r="K36" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="L36" s="0"/>
+      <c r="L36" s="80"/>
       <c r="O36" s="41"/>
       <c r="P36" s="41"/>
       <c r="Q36" s="41"/>
-      <c r="R36" s="86"/>
+      <c r="R36" s="87"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="87" t="s">
+      <c r="A37" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="88" t="n">
+      <c r="B37" s="89" t="n">
         <f aca="false">IFERROR(B36 / B35,0)</f>
         <v>0</v>
       </c>
-      <c r="C37" s="89" t="n">
+      <c r="C37" s="90" t="n">
         <f aca="false">IFERROR(C36 / C35,0)</f>
         <v>0</v>
       </c>
-      <c r="D37" s="88" t="n">
+      <c r="D37" s="89" t="n">
         <f aca="false">IFERROR(D36 / D35,0)</f>
         <v>0</v>
       </c>
-      <c r="E37" s="90" t="n">
+      <c r="E37" s="91" t="n">
         <f aca="false">IFERROR(E36 / E35,0)</f>
         <v>0</v>
       </c>
-      <c r="F37" s="89" t="n">
+      <c r="F37" s="90" t="n">
         <f aca="false">IFERROR(F36 / F35,0)</f>
         <v>0</v>
       </c>
-      <c r="G37" s="89" t="n">
+      <c r="G37" s="90" t="n">
         <f aca="false">IFERROR(G36 / G35,0)</f>
         <v>0</v>
       </c>
-      <c r="H37" s="88" t="n">
+      <c r="H37" s="89" t="n">
         <f aca="false">IFERROR(H36 / H35,0)</f>
         <v>0</v>
       </c>
-      <c r="I37" s="90" t="n">
+      <c r="I37" s="91" t="n">
         <f aca="false">IFERROR(I36 / I35,0)</f>
         <v>0</v>
       </c>
-      <c r="J37" s="89" t="n">
+      <c r="J37" s="90" t="n">
         <f aca="false">IFERROR(J36 / J35,0)</f>
         <v>0</v>
       </c>
-      <c r="K37" s="90" t="n">
+      <c r="K37" s="91" t="n">
         <f aca="false">IFERROR(K36 / K35,0)</f>
         <v>0</v>
       </c>
-      <c r="L37" s="0"/>
+      <c r="L37" s="80"/>
       <c r="M37" s="78"/>
       <c r="N37" s="77"/>
       <c r="O37" s="77"/>
@@ -2576,18 +2580,18 @@
       <c r="AR37" s="19"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="80" t="s">
+      <c r="A38" s="81" t="s">
         <v>55</v>
       </c>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
-      <c r="D38" s="91" t="str">
+      <c r="D38" s="92" t="str">
         <f aca="false">O1</f>
         <v>YV Kerrat:</v>
       </c>
       <c r="E38" s="14"/>
       <c r="F38" s="14"/>
-      <c r="G38" s="91" t="str">
+      <c r="G38" s="92" t="str">
         <f aca="false">Q1</f>
         <v>AV Kerrat:</v>
       </c>
@@ -2595,7 +2599,7 @@
       <c r="I38" s="14"/>
       <c r="J38" s="14"/>
       <c r="K38" s="14"/>
-      <c r="L38" s="0"/>
+      <c r="L38" s="80"/>
       <c r="M38" s="77"/>
       <c r="N38" s="77"/>
       <c r="O38" s="77"/>
@@ -2630,24 +2634,24 @@
       <c r="AR38" s="19"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="87" t="s">
+      <c r="A39" s="88" t="s">
         <v>56</v>
       </c>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
-      <c r="D39" s="92" t="n">
+      <c r="D39" s="93" t="n">
         <f aca="false">IFERROR(D35 / D38,0)</f>
         <v>0</v>
       </c>
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
-      <c r="G39" s="92" t="n">
+      <c r="G39" s="93" t="n">
         <f aca="false">IFERROR(G35 / G38,0)</f>
         <v>0</v>
       </c>
       <c r="H39" s="13"/>
-      <c r="I39" s="93"/>
-      <c r="J39" s="93"/>
+      <c r="I39" s="94"/>
+      <c r="J39" s="94"/>
       <c r="K39" s="13"/>
       <c r="M39" s="77"/>
       <c r="N39" s="77"/>
@@ -2718,31 +2722,31 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="S41" s="19"/>
-      <c r="T41" s="94"/>
-      <c r="U41" s="94"/>
-      <c r="V41" s="94"/>
-      <c r="W41" s="94"/>
-      <c r="X41" s="94"/>
-      <c r="Y41" s="94"/>
-      <c r="Z41" s="94"/>
-      <c r="AA41" s="94"/>
-      <c r="AB41" s="94"/>
-      <c r="AC41" s="94"/>
-      <c r="AD41" s="94"/>
-      <c r="AE41" s="94"/>
+      <c r="T41" s="95"/>
+      <c r="U41" s="95"/>
+      <c r="V41" s="95"/>
+      <c r="W41" s="95"/>
+      <c r="X41" s="95"/>
+      <c r="Y41" s="95"/>
+      <c r="Z41" s="95"/>
+      <c r="AA41" s="95"/>
+      <c r="AB41" s="95"/>
+      <c r="AC41" s="95"/>
+      <c r="AD41" s="95"/>
+      <c r="AE41" s="95"/>
       <c r="AF41" s="19"/>
-      <c r="AG41" s="94"/>
-      <c r="AH41" s="94"/>
-      <c r="AI41" s="94"/>
-      <c r="AJ41" s="94"/>
-      <c r="AK41" s="94"/>
-      <c r="AL41" s="94"/>
-      <c r="AM41" s="94"/>
-      <c r="AN41" s="94"/>
-      <c r="AO41" s="94"/>
-      <c r="AP41" s="94"/>
-      <c r="AQ41" s="94"/>
-      <c r="AR41" s="94"/>
+      <c r="AG41" s="95"/>
+      <c r="AH41" s="95"/>
+      <c r="AI41" s="95"/>
+      <c r="AJ41" s="95"/>
+      <c r="AK41" s="95"/>
+      <c r="AL41" s="95"/>
+      <c r="AM41" s="95"/>
+      <c r="AN41" s="95"/>
+      <c r="AO41" s="95"/>
+      <c r="AP41" s="95"/>
+      <c r="AQ41" s="95"/>
+      <c r="AR41" s="95"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="18"/>
@@ -3588,7 +3592,7 @@
       <c r="A66" s="19"/>
       <c r="C66" s="19"/>
       <c r="D66" s="19"/>
-      <c r="E66" s="95" t="str">
+      <c r="E66" s="96" t="str">
         <f aca="false">IFERROR(C66 / D66, "")</f>
         <v/>
       </c>
@@ -3596,7 +3600,7 @@
       <c r="G66" s="19"/>
       <c r="I66" s="19"/>
       <c r="J66" s="19"/>
-      <c r="K66" s="95" t="str">
+      <c r="K66" s="96" t="str">
         <f aca="false">IFERROR(I66 / J66, "")</f>
         <v/>
       </c>
@@ -3604,7 +3608,7 @@
       <c r="M66" s="19"/>
       <c r="O66" s="19"/>
       <c r="P66" s="19"/>
-      <c r="Q66" s="95" t="str">
+      <c r="Q66" s="96" t="str">
         <f aca="false">IFERROR(O66 / P66, "")</f>
         <v/>
       </c>
@@ -3612,35 +3616,35 @@
       <c r="S66" s="19"/>
       <c r="U66" s="19"/>
       <c r="V66" s="19"/>
-      <c r="W66" s="95" t="str">
+      <c r="W66" s="96" t="str">
         <f aca="false">IFERROR(U66 / V66, "")</f>
         <v/>
       </c>
       <c r="X66" s="19"/>
       <c r="Z66" s="19"/>
       <c r="AA66" s="19"/>
-      <c r="AB66" s="95" t="str">
+      <c r="AB66" s="96" t="str">
         <f aca="false">IFERROR(Z66 / AA66, "")</f>
         <v/>
       </c>
       <c r="AC66" s="19"/>
       <c r="AE66" s="19"/>
       <c r="AF66" s="19"/>
-      <c r="AG66" s="95" t="str">
+      <c r="AG66" s="96" t="str">
         <f aca="false">IFERROR(AE66 / AF66, "")</f>
         <v/>
       </c>
       <c r="AH66" s="19"/>
       <c r="AJ66" s="19"/>
       <c r="AK66" s="19"/>
-      <c r="AL66" s="95" t="str">
+      <c r="AL66" s="96" t="str">
         <f aca="false">IFERROR(AJ66 / AK66, "")</f>
         <v/>
       </c>
       <c r="AM66" s="19"/>
       <c r="AO66" s="19"/>
       <c r="AP66" s="19"/>
-      <c r="AQ66" s="95" t="str">
+      <c r="AQ66" s="96" t="str">
         <f aca="false">IFERROR(AO66 / AP66, "")</f>
         <v/>
       </c>
@@ -5121,8 +5125,8 @@
   </sheetPr>
   <dimension ref="A1:AR114"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5142,14 +5146,14 @@
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
       <c r="F1" s="15"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
       <c r="J1" s="42"/>
       <c r="K1" s="42"/>
       <c r="L1" s="42"/>
-      <c r="M1" s="96"/>
-      <c r="N1" s="96"/>
+      <c r="M1" s="97"/>
+      <c r="N1" s="97"/>
       <c r="O1" s="18"/>
       <c r="P1" s="19"/>
       <c r="Q1" s="18"/>
@@ -5950,7 +5954,7 @@
       <c r="A19" s="52"/>
       <c r="B19" s="53"/>
       <c r="C19" s="54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="55" t="n">
         <v>0</v>
@@ -5961,7 +5965,7 @@
       <c r="F19" s="57"/>
       <c r="G19" s="58"/>
       <c r="H19" s="54" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I19" s="55" t="n">
         <v>0</v>
@@ -5973,7 +5977,7 @@
       <c r="L19" s="58"/>
       <c r="M19" s="60" t="n">
         <f aca="false">IFERROR(C19 / H19,0)</f>
-        <v>0</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="N19" s="61" t="n">
         <f aca="false">IFERROR(D19 / I19,0)</f>
@@ -6358,17 +6362,17 @@
       <c r="A32" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="B32" s="0"/>
-      <c r="C32" s="0"/>
-      <c r="D32" s="0"/>
-      <c r="E32" s="0"/>
-      <c r="F32" s="0"/>
-      <c r="G32" s="0"/>
-      <c r="H32" s="0"/>
-      <c r="I32" s="0"/>
-      <c r="J32" s="0"/>
-      <c r="K32" s="0"/>
-      <c r="L32" s="0"/>
+      <c r="B32" s="80"/>
+      <c r="C32" s="80"/>
+      <c r="D32" s="80"/>
+      <c r="E32" s="80"/>
+      <c r="F32" s="80"/>
+      <c r="G32" s="80"/>
+      <c r="H32" s="80"/>
+      <c r="I32" s="80"/>
+      <c r="J32" s="80"/>
+      <c r="K32" s="80"/>
+      <c r="L32" s="80"/>
       <c r="M32" s="77"/>
       <c r="N32" s="77"/>
       <c r="O32" s="77"/>
@@ -6376,30 +6380,30 @@
       <c r="Q32" s="77"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="80" t="s">
+      <c r="A33" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="B33" s="81" t="s">
+      <c r="B33" s="82" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="81"/>
-      <c r="D33" s="82" t="s">
+      <c r="C33" s="82"/>
+      <c r="D33" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="E33" s="82"/>
-      <c r="F33" s="82" t="s">
+      <c r="E33" s="83"/>
+      <c r="F33" s="83" t="s">
         <v>52</v>
       </c>
-      <c r="G33" s="82"/>
-      <c r="H33" s="83" t="s">
+      <c r="G33" s="83"/>
+      <c r="H33" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="I33" s="83"/>
-      <c r="J33" s="84" t="s">
+      <c r="I33" s="84"/>
+      <c r="J33" s="85" t="s">
         <v>54</v>
       </c>
-      <c r="K33" s="84"/>
-      <c r="L33" s="0"/>
+      <c r="K33" s="85"/>
+      <c r="L33" s="80"/>
       <c r="M33" s="77"/>
       <c r="N33" s="77"/>
       <c r="O33" s="77"/>
@@ -6407,7 +6411,7 @@
       <c r="Q33" s="77"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="85" t="s">
+      <c r="A34" s="86" t="s">
         <v>17</v>
       </c>
       <c r="B34" s="24" t="s">
@@ -6440,10 +6444,10 @@
       <c r="K34" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="L34" s="0"/>
+      <c r="L34" s="80"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="85" t="s">
+      <c r="A35" s="86" t="s">
         <v>20</v>
       </c>
       <c r="B35" s="26" t="n">
@@ -6476,7 +6480,7 @@
       <c r="K35" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="L35" s="0"/>
+      <c r="L35" s="80"/>
       <c r="M35" s="19"/>
       <c r="N35" s="19"/>
       <c r="O35" s="19"/>
@@ -6484,7 +6488,7 @@
       <c r="Q35" s="19"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="85" t="s">
+      <c r="A36" s="86" t="s">
         <v>21</v>
       </c>
       <c r="B36" s="26" t="n">
@@ -6517,57 +6521,57 @@
       <c r="K36" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="L36" s="0"/>
+      <c r="L36" s="80"/>
       <c r="O36" s="41"/>
       <c r="P36" s="41"/>
       <c r="Q36" s="41"/>
-      <c r="R36" s="86"/>
+      <c r="R36" s="87"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="87" t="s">
+      <c r="A37" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="88" t="n">
+      <c r="B37" s="89" t="n">
         <f aca="false">IFERROR(B36 / B35,0)</f>
         <v>0</v>
       </c>
-      <c r="C37" s="89" t="n">
+      <c r="C37" s="90" t="n">
         <f aca="false">IFERROR(C36 / C35,0)</f>
         <v>0</v>
       </c>
-      <c r="D37" s="88" t="n">
+      <c r="D37" s="89" t="n">
         <f aca="false">IFERROR(D36 / D35,0)</f>
         <v>0</v>
       </c>
-      <c r="E37" s="90" t="n">
+      <c r="E37" s="91" t="n">
         <f aca="false">IFERROR(E36 / E35,0)</f>
         <v>0</v>
       </c>
-      <c r="F37" s="89" t="n">
+      <c r="F37" s="90" t="n">
         <f aca="false">IFERROR(F36 / F35,0)</f>
         <v>0</v>
       </c>
-      <c r="G37" s="89" t="n">
+      <c r="G37" s="90" t="n">
         <f aca="false">IFERROR(G36 / G35,0)</f>
         <v>0</v>
       </c>
-      <c r="H37" s="88" t="n">
+      <c r="H37" s="89" t="n">
         <f aca="false">IFERROR(H36 / H35,0)</f>
         <v>0</v>
       </c>
-      <c r="I37" s="90" t="n">
+      <c r="I37" s="91" t="n">
         <f aca="false">IFERROR(I36 / I35,0)</f>
         <v>0</v>
       </c>
-      <c r="J37" s="89" t="n">
+      <c r="J37" s="90" t="n">
         <f aca="false">IFERROR(J36 / J35,0)</f>
         <v>0</v>
       </c>
-      <c r="K37" s="90" t="n">
+      <c r="K37" s="91" t="n">
         <f aca="false">IFERROR(K36 / K35,0)</f>
         <v>0</v>
       </c>
-      <c r="L37" s="0"/>
+      <c r="L37" s="80"/>
       <c r="M37" s="78"/>
       <c r="N37" s="77"/>
       <c r="O37" s="77"/>
@@ -6602,18 +6606,18 @@
       <c r="AR37" s="19"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="80" t="s">
+      <c r="A38" s="81" t="s">
         <v>55</v>
       </c>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
-      <c r="D38" s="91" t="n">
+      <c r="D38" s="92" t="n">
         <f aca="false">O1</f>
         <v>0</v>
       </c>
       <c r="E38" s="14"/>
       <c r="F38" s="14"/>
-      <c r="G38" s="91" t="n">
+      <c r="G38" s="92" t="n">
         <f aca="false">Q1</f>
         <v>0</v>
       </c>
@@ -6621,7 +6625,7 @@
       <c r="I38" s="14"/>
       <c r="J38" s="14"/>
       <c r="K38" s="14"/>
-      <c r="L38" s="0"/>
+      <c r="L38" s="80"/>
       <c r="M38" s="77"/>
       <c r="N38" s="77"/>
       <c r="O38" s="77"/>
@@ -6656,24 +6660,24 @@
       <c r="AR38" s="19"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="87" t="s">
+      <c r="A39" s="88" t="s">
         <v>56</v>
       </c>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
-      <c r="D39" s="92" t="n">
+      <c r="D39" s="93" t="n">
         <f aca="false">IFERROR(D35 / D38,0)</f>
         <v>0</v>
       </c>
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
-      <c r="G39" s="92" t="n">
+      <c r="G39" s="93" t="n">
         <f aca="false">IFERROR(G35 / G38,0)</f>
         <v>0</v>
       </c>
       <c r="H39" s="13"/>
-      <c r="I39" s="93"/>
-      <c r="J39" s="93"/>
+      <c r="I39" s="94"/>
+      <c r="J39" s="94"/>
       <c r="K39" s="13"/>
       <c r="M39" s="77"/>
       <c r="N39" s="77"/>
@@ -6744,31 +6748,31 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="S41" s="19"/>
-      <c r="T41" s="94"/>
-      <c r="U41" s="94"/>
-      <c r="V41" s="94"/>
-      <c r="W41" s="94"/>
-      <c r="X41" s="94"/>
-      <c r="Y41" s="94"/>
-      <c r="Z41" s="94"/>
-      <c r="AA41" s="94"/>
-      <c r="AB41" s="94"/>
-      <c r="AC41" s="94"/>
-      <c r="AD41" s="94"/>
-      <c r="AE41" s="94"/>
+      <c r="T41" s="95"/>
+      <c r="U41" s="95"/>
+      <c r="V41" s="95"/>
+      <c r="W41" s="95"/>
+      <c r="X41" s="95"/>
+      <c r="Y41" s="95"/>
+      <c r="Z41" s="95"/>
+      <c r="AA41" s="95"/>
+      <c r="AB41" s="95"/>
+      <c r="AC41" s="95"/>
+      <c r="AD41" s="95"/>
+      <c r="AE41" s="95"/>
       <c r="AF41" s="19"/>
-      <c r="AG41" s="94"/>
-      <c r="AH41" s="94"/>
-      <c r="AI41" s="94"/>
-      <c r="AJ41" s="94"/>
-      <c r="AK41" s="94"/>
-      <c r="AL41" s="94"/>
-      <c r="AM41" s="94"/>
-      <c r="AN41" s="94"/>
-      <c r="AO41" s="94"/>
-      <c r="AP41" s="94"/>
-      <c r="AQ41" s="94"/>
-      <c r="AR41" s="94"/>
+      <c r="AG41" s="95"/>
+      <c r="AH41" s="95"/>
+      <c r="AI41" s="95"/>
+      <c r="AJ41" s="95"/>
+      <c r="AK41" s="95"/>
+      <c r="AL41" s="95"/>
+      <c r="AM41" s="95"/>
+      <c r="AN41" s="95"/>
+      <c r="AO41" s="95"/>
+      <c r="AP41" s="95"/>
+      <c r="AQ41" s="95"/>
+      <c r="AR41" s="95"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="18"/>
@@ -7614,7 +7618,7 @@
       <c r="A66" s="19"/>
       <c r="C66" s="19"/>
       <c r="D66" s="19"/>
-      <c r="E66" s="95" t="str">
+      <c r="E66" s="96" t="str">
         <f aca="false">IFERROR(C66 / D66, "")</f>
         <v/>
       </c>
@@ -7622,7 +7626,7 @@
       <c r="G66" s="19"/>
       <c r="I66" s="19"/>
       <c r="J66" s="19"/>
-      <c r="K66" s="95" t="str">
+      <c r="K66" s="96" t="str">
         <f aca="false">IFERROR(I66 / J66, "")</f>
         <v/>
       </c>
@@ -7630,7 +7634,7 @@
       <c r="M66" s="19"/>
       <c r="O66" s="19"/>
       <c r="P66" s="19"/>
-      <c r="Q66" s="95" t="str">
+      <c r="Q66" s="96" t="str">
         <f aca="false">IFERROR(O66 / P66, "")</f>
         <v/>
       </c>
@@ -7638,35 +7642,35 @@
       <c r="S66" s="19"/>
       <c r="U66" s="19"/>
       <c r="V66" s="19"/>
-      <c r="W66" s="95" t="str">
+      <c r="W66" s="96" t="str">
         <f aca="false">IFERROR(U66 / V66, "")</f>
         <v/>
       </c>
       <c r="X66" s="19"/>
       <c r="Z66" s="19"/>
       <c r="AA66" s="19"/>
-      <c r="AB66" s="95" t="str">
+      <c r="AB66" s="96" t="str">
         <f aca="false">IFERROR(Z66 / AA66, "")</f>
         <v/>
       </c>
       <c r="AC66" s="19"/>
       <c r="AE66" s="19"/>
       <c r="AF66" s="19"/>
-      <c r="AG66" s="95" t="str">
+      <c r="AG66" s="96" t="str">
         <f aca="false">IFERROR(AE66 / AF66, "")</f>
         <v/>
       </c>
       <c r="AH66" s="19"/>
       <c r="AJ66" s="19"/>
       <c r="AK66" s="19"/>
-      <c r="AL66" s="95" t="str">
+      <c r="AL66" s="96" t="str">
         <f aca="false">IFERROR(AJ66 / AK66, "")</f>
         <v/>
       </c>
       <c r="AM66" s="19"/>
       <c r="AO66" s="19"/>
       <c r="AP66" s="19"/>
-      <c r="AQ66" s="95" t="str">
+      <c r="AQ66" s="96" t="str">
         <f aca="false">IFERROR(AO66 / AP66, "")</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
Bug fix to make shot for and against work in +/- player stats
</commit_message>
<xml_diff>
--- a/backend/excels/game_stats_template.xlsx
+++ b/backend/excels/game_stats_template.xlsx
@@ -173,19 +173,19 @@
     <t xml:space="preserve">Tilanne</t>
   </si>
   <si>
-    <t xml:space="preserve">5 on 5</t>
+    <t xml:space="preserve">5 v 5</t>
   </si>
   <si>
-    <t xml:space="preserve">PP</t>
+    <t xml:space="preserve">YV</t>
   </si>
   <si>
-    <t xml:space="preserve">PK</t>
+    <t xml:space="preserve">AV</t>
   </si>
   <si>
-    <t xml:space="preserve">6 on 5</t>
+    <t xml:space="preserve">TM+</t>
   </si>
   <si>
-    <t xml:space="preserve">5 on 6</t>
+    <t xml:space="preserve">TM-</t>
   </si>
   <si>
     <t xml:space="preserve">YV / AV Tilaisuudet</t>
@@ -1081,8 +1081,8 @@
   </sheetPr>
   <dimension ref="A1:AR114"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U26" activeCellId="0" sqref="U26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J33" activeCellId="0" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5126,7 +5126,7 @@
   <dimension ref="A1:AR114"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
+      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
First public beta version (#29)
* Added page for visualizing and analyzing stats

* Bug fix to make shot for and against work in +/- player stats

* Translated roster management alert from english to finnish
</commit_message>
<xml_diff>
--- a/backend/excels/game_stats_template.xlsx
+++ b/backend/excels/game_stats_template.xlsx
@@ -173,19 +173,19 @@
     <t xml:space="preserve">Tilanne</t>
   </si>
   <si>
-    <t xml:space="preserve">5 on 5</t>
+    <t xml:space="preserve">5 v 5</t>
   </si>
   <si>
-    <t xml:space="preserve">PP</t>
+    <t xml:space="preserve">YV</t>
   </si>
   <si>
-    <t xml:space="preserve">PK</t>
+    <t xml:space="preserve">AV</t>
   </si>
   <si>
-    <t xml:space="preserve">6 on 5</t>
+    <t xml:space="preserve">TM+</t>
   </si>
   <si>
-    <t xml:space="preserve">5 on 6</t>
+    <t xml:space="preserve">TM-</t>
   </si>
   <si>
     <t xml:space="preserve">YV / AV Tilaisuudet</t>
@@ -1081,8 +1081,8 @@
   </sheetPr>
   <dimension ref="A1:AR114"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U26" activeCellId="0" sqref="U26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J33" activeCellId="0" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5126,7 +5126,7 @@
   <dimension ref="A1:AR114"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
+      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Implemented shot map rendering to the game stats excel
</commit_message>
<xml_diff>
--- a/backend/excels/game_stats_template.xlsx
+++ b/backend/excels/game_stats_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Game_Template" sheetId="1" state="visible" r:id="rId3"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="59">
   <si>
     <t xml:space="preserve">PVM:</t>
   </si>
@@ -146,6 +146,12 @@
     <t xml:space="preserve">YHTEENSÄ +</t>
   </si>
   <si>
+    <t xml:space="preserve">X = Maali</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O = Maalipaikka</t>
+  </si>
+  <si>
     <t xml:space="preserve">MAALIT</t>
   </si>
   <si>
@@ -206,7 +212,7 @@
     <numFmt numFmtId="168" formatCode="0.0%"/>
     <numFmt numFmtId="169" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,6 +295,28 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="36"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="36"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -423,6 +451,13 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
         <color rgb="FFFF0000"/>
       </left>
@@ -438,13 +473,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
-      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -497,7 +525,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="102">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -654,6 +682,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -706,6 +738,18 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -750,7 +794,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -758,11 +806,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -770,7 +818,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -786,7 +834,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -818,10 +866,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -850,7 +894,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -870,7 +914,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="17" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="15" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1081,8 +1125,8 @@
   </sheetPr>
   <dimension ref="A1:AR114"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X20" activeCellId="0" sqref="X20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1744,6 +1788,14 @@
       <c r="U13" s="27" t="n">
         <v>0</v>
       </c>
+      <c r="V13" s="39"/>
+      <c r="W13" s="39"/>
+      <c r="X13" s="39"/>
+      <c r="Y13" s="39"/>
+      <c r="Z13" s="39"/>
+      <c r="AA13" s="39"/>
+      <c r="AB13" s="39"/>
+      <c r="AC13" s="39"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="33" t="s">
@@ -1757,11 +1809,11 @@
         <f aca="false">IFERROR(C13 / C12,0)</f>
         <v>0</v>
       </c>
-      <c r="D14" s="39" t="n">
+      <c r="D14" s="40" t="n">
         <f aca="false">IFERROR(D13 / D12,0)</f>
         <v>0</v>
       </c>
-      <c r="E14" s="39" t="n">
+      <c r="E14" s="40" t="n">
         <f aca="false">IFERROR(E13 / E12,0)</f>
         <v>0</v>
       </c>
@@ -1773,11 +1825,11 @@
         <f aca="false">IFERROR(G13 / G12,0)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="39" t="n">
+      <c r="H14" s="40" t="n">
         <f aca="false">IFERROR(H13 / H12,0)</f>
         <v>0</v>
       </c>
-      <c r="I14" s="39" t="n">
+      <c r="I14" s="40" t="n">
         <f aca="false">IFERROR(I13 / I12,0)</f>
         <v>0</v>
       </c>
@@ -1789,11 +1841,11 @@
         <f aca="false">IFERROR(K13 / K12,0)</f>
         <v>0</v>
       </c>
-      <c r="L14" s="39" t="n">
+      <c r="L14" s="40" t="n">
         <f aca="false">IFERROR(L13 / L12,0)</f>
         <v>0</v>
       </c>
-      <c r="M14" s="39" t="n">
+      <c r="M14" s="40" t="n">
         <f aca="false">IFERROR(M13 / M12,0)</f>
         <v>0</v>
       </c>
@@ -1805,11 +1857,11 @@
         <f aca="false">IFERROR(O13 / O12,0)</f>
         <v>0</v>
       </c>
-      <c r="P14" s="39" t="n">
+      <c r="P14" s="40" t="n">
         <f aca="false">IFERROR(P13 / P12,0)</f>
         <v>0</v>
       </c>
-      <c r="Q14" s="39" t="n">
+      <c r="Q14" s="40" t="n">
         <f aca="false">IFERROR(Q13 / Q12,0)</f>
         <v>0</v>
       </c>
@@ -1821,7 +1873,7 @@
         <f aca="false">IFERROR(S13 / S12,0)</f>
         <v>0</v>
       </c>
-      <c r="T14" s="39" t="n">
+      <c r="T14" s="40" t="n">
         <f aca="false">IFERROR(T13 / T12,0)</f>
         <v>0</v>
       </c>
@@ -1829,6 +1881,14 @@
         <f aca="false">IFERROR(U13 / U12,0)</f>
         <v>0</v>
       </c>
+      <c r="V14" s="39"/>
+      <c r="W14" s="39"/>
+      <c r="X14" s="39"/>
+      <c r="Y14" s="39"/>
+      <c r="Z14" s="39"/>
+      <c r="AA14" s="39"/>
+      <c r="AB14" s="39"/>
+      <c r="AC14" s="39"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="31"/>
@@ -1867,29 +1927,29 @@
       <c r="U16" s="19"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="41" t="s">
         <v>35</v>
       </c>
       <c r="B17" s="19"/>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
-      <c r="H17" s="42" t="s">
+      <c r="H17" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
       <c r="K17" s="19"/>
       <c r="L17" s="19"/>
-      <c r="M17" s="41" t="s">
+      <c r="M17" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="N17" s="41"/>
-      <c r="O17" s="41"/>
+      <c r="N17" s="42"/>
+      <c r="O17" s="42"/>
       <c r="P17" s="19"/>
       <c r="Q17" s="19"/>
       <c r="R17" s="19"/>
@@ -1898,119 +1958,147 @@
       <c r="U17" s="19"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="44"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="50"/>
-      <c r="L18" s="48"/>
-      <c r="M18" s="49"/>
-      <c r="N18" s="49"/>
-      <c r="O18" s="45"/>
-      <c r="P18" s="50"/>
-      <c r="Q18" s="51" t="s">
+      <c r="B18" s="45"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="51"/>
+      <c r="L18" s="49"/>
+      <c r="M18" s="50"/>
+      <c r="N18" s="50"/>
+      <c r="O18" s="46"/>
+      <c r="P18" s="51"/>
+      <c r="Q18" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="R18" s="51"/>
-      <c r="S18" s="51"/>
-      <c r="T18" s="19"/>
-      <c r="U18" s="19"/>
+      <c r="R18" s="52"/>
+      <c r="S18" s="52"/>
+      <c r="T18" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="U18" s="53"/>
+      <c r="V18" s="53"/>
+      <c r="W18" s="53"/>
+      <c r="X18" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y18" s="54"/>
+      <c r="Z18" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA18" s="55"/>
+      <c r="AB18" s="55"/>
+      <c r="AC18" s="55"/>
+      <c r="AD18" s="39"/>
+      <c r="AE18" s="39"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="52"/>
-      <c r="B19" s="53"/>
-      <c r="C19" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" s="57"/>
-      <c r="G19" s="58"/>
-      <c r="H19" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="J19" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="K19" s="59"/>
-      <c r="L19" s="58"/>
-      <c r="M19" s="60" t="n">
+      <c r="A19" s="56"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="59" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="61"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="59" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" s="63"/>
+      <c r="L19" s="62"/>
+      <c r="M19" s="64" t="n">
         <f aca="false">IFERROR(C19 / H19,0)</f>
         <v>0</v>
       </c>
-      <c r="N19" s="61" t="n">
+      <c r="N19" s="65" t="n">
         <f aca="false">IFERROR(D19 / I19,0)</f>
         <v>0</v>
       </c>
-      <c r="O19" s="62" t="n">
+      <c r="O19" s="66" t="n">
         <f aca="false">IFERROR(E19 / J19,0)</f>
         <v>0</v>
       </c>
-      <c r="P19" s="59"/>
-      <c r="Q19" s="51"/>
-      <c r="R19" s="51"/>
-      <c r="S19" s="51"/>
-      <c r="T19" s="19"/>
-      <c r="U19" s="19"/>
+      <c r="P19" s="63"/>
+      <c r="Q19" s="52"/>
+      <c r="R19" s="52"/>
+      <c r="S19" s="52"/>
+      <c r="T19" s="53"/>
+      <c r="U19" s="53"/>
+      <c r="V19" s="53"/>
+      <c r="W19" s="53"/>
+      <c r="X19" s="67" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y19" s="67"/>
+      <c r="Z19" s="55"/>
+      <c r="AA19" s="55"/>
+      <c r="AB19" s="55"/>
+      <c r="AC19" s="55"/>
+      <c r="AD19" s="39"/>
+      <c r="AE19" s="39"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="52"/>
-      <c r="B20" s="53"/>
-      <c r="C20" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" s="57"/>
-      <c r="G20" s="58"/>
-      <c r="H20" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="J20" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="K20" s="59"/>
-      <c r="L20" s="58"/>
-      <c r="M20" s="66" t="n">
+      <c r="A20" s="56"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="61"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" s="63"/>
+      <c r="L20" s="62"/>
+      <c r="M20" s="71" t="n">
         <f aca="false">IFERROR(C20 / H20,0)</f>
         <v>0</v>
       </c>
-      <c r="N20" s="67" t="n">
+      <c r="N20" s="72" t="n">
         <f aca="false">IFERROR(D20 / I20,0)</f>
         <v>0</v>
       </c>
-      <c r="O20" s="68" t="n">
+      <c r="O20" s="73" t="n">
         <f aca="false">IFERROR(E20 / J20,0)</f>
         <v>0</v>
       </c>
-      <c r="P20" s="59"/>
-      <c r="Q20" s="69" t="s">
-        <v>41</v>
-      </c>
-      <c r="R20" s="69"/>
-      <c r="S20" s="70" t="n">
+      <c r="P20" s="63"/>
+      <c r="Q20" s="74" t="s">
+        <v>43</v>
+      </c>
+      <c r="R20" s="74"/>
+      <c r="S20" s="75" t="n">
         <f aca="false">SUM(B13,D13,F13,H13,J13,L13,N13,P13,R13,T13)</f>
         <v>0</v>
       </c>
@@ -2018,74 +2106,74 @@
       <c r="U20" s="19"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="52"/>
-      <c r="B21" s="53"/>
-      <c r="C21" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" s="71" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" s="57"/>
-      <c r="G21" s="58"/>
-      <c r="H21" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="I21" s="71" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" s="59"/>
-      <c r="L21" s="58"/>
-      <c r="M21" s="66" t="n">
+      <c r="A21" s="56"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="61"/>
+      <c r="G21" s="62"/>
+      <c r="H21" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" s="63"/>
+      <c r="L21" s="62"/>
+      <c r="M21" s="71" t="n">
         <f aca="false">IFERROR(C21 / H21,0)</f>
         <v>0</v>
       </c>
-      <c r="N21" s="67" t="n">
+      <c r="N21" s="72" t="n">
         <f aca="false">IFERROR(D21 / I21,0)</f>
         <v>0</v>
       </c>
-      <c r="O21" s="68" t="n">
+      <c r="O21" s="73" t="n">
         <f aca="false">IFERROR(E21 / J21,0)</f>
         <v>0</v>
       </c>
-      <c r="P21" s="59"/>
-      <c r="Q21" s="69" t="s">
-        <v>42</v>
-      </c>
-      <c r="R21" s="69"/>
-      <c r="S21" s="70" t="n">
+      <c r="P21" s="63"/>
+      <c r="Q21" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="R21" s="74"/>
+      <c r="S21" s="75" t="n">
         <f aca="false">SUM(B12,D12,F12,H12,J12,L12,N12,P12,R12,T12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="72"/>
-      <c r="B22" s="73"/>
-      <c r="C22" s="74"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="74"/>
-      <c r="F22" s="75"/>
-      <c r="G22" s="73"/>
-      <c r="H22" s="74"/>
-      <c r="I22" s="74"/>
-      <c r="J22" s="74"/>
-      <c r="K22" s="75"/>
-      <c r="L22" s="73"/>
-      <c r="M22" s="74"/>
-      <c r="N22" s="74"/>
-      <c r="O22" s="74"/>
-      <c r="P22" s="75"/>
-      <c r="Q22" s="69" t="s">
-        <v>43</v>
-      </c>
-      <c r="R22" s="69"/>
-      <c r="S22" s="76" t="n">
+      <c r="A22" s="77"/>
+      <c r="B22" s="78"/>
+      <c r="C22" s="79"/>
+      <c r="D22" s="79"/>
+      <c r="E22" s="79"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="78"/>
+      <c r="H22" s="79"/>
+      <c r="I22" s="79"/>
+      <c r="J22" s="79"/>
+      <c r="K22" s="80"/>
+      <c r="L22" s="78"/>
+      <c r="M22" s="79"/>
+      <c r="N22" s="79"/>
+      <c r="O22" s="79"/>
+      <c r="P22" s="80"/>
+      <c r="Q22" s="74" t="s">
+        <v>45</v>
+      </c>
+      <c r="R22" s="74"/>
+      <c r="S22" s="81" t="n">
         <f aca="false">IFERROR(S20 / S21,0)</f>
         <v>0</v>
       </c>
@@ -2100,213 +2188,213 @@
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="18"/>
       <c r="B24" s="19"/>
-      <c r="C24" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
+      <c r="C24" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
       <c r="F24" s="19"/>
       <c r="G24" s="18"/>
-      <c r="H24" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
+      <c r="H24" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
       <c r="K24" s="19"/>
       <c r="L24" s="19"/>
-      <c r="M24" s="41" t="s">
+      <c r="M24" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="N24" s="41"/>
-      <c r="O24" s="41"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="42"/>
       <c r="P24" s="19"/>
       <c r="Q24" s="19"/>
       <c r="R24" s="19"/>
       <c r="S24" s="19"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="48"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="45"/>
-      <c r="K25" s="50"/>
-      <c r="L25" s="48"/>
-      <c r="M25" s="49"/>
-      <c r="N25" s="49"/>
-      <c r="O25" s="45"/>
-      <c r="P25" s="50"/>
-      <c r="Q25" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="R25" s="51"/>
-      <c r="S25" s="51"/>
+      <c r="A25" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="49"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="51"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="50"/>
+      <c r="N25" s="50"/>
+      <c r="O25" s="46"/>
+      <c r="P25" s="51"/>
+      <c r="Q25" s="52" t="s">
+        <v>49</v>
+      </c>
+      <c r="R25" s="52"/>
+      <c r="S25" s="52"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="52"/>
-      <c r="B26" s="58"/>
-      <c r="C26" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" s="59"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="I26" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="J26" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="K26" s="59"/>
-      <c r="L26" s="58"/>
-      <c r="M26" s="60" t="n">
+      <c r="A26" s="56"/>
+      <c r="B26" s="62"/>
+      <c r="C26" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="59" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="63"/>
+      <c r="G26" s="62"/>
+      <c r="H26" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" s="59" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" s="63"/>
+      <c r="L26" s="62"/>
+      <c r="M26" s="64" t="n">
         <f aca="false">IFERROR(C26 / H26,0)</f>
         <v>0</v>
       </c>
-      <c r="N26" s="61" t="n">
+      <c r="N26" s="65" t="n">
         <f aca="false">IFERROR(D26 / I26,0)</f>
         <v>0</v>
       </c>
-      <c r="O26" s="62" t="n">
+      <c r="O26" s="66" t="n">
         <f aca="false">IFERROR(E26 / J26,0)</f>
         <v>0</v>
       </c>
-      <c r="P26" s="59"/>
-      <c r="Q26" s="51"/>
-      <c r="R26" s="51"/>
-      <c r="S26" s="51"/>
+      <c r="P26" s="63"/>
+      <c r="Q26" s="52"/>
+      <c r="R26" s="52"/>
+      <c r="S26" s="52"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="52"/>
-      <c r="B27" s="58"/>
-      <c r="C27" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="D27" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="E27" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" s="59"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="I27" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="J27" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="K27" s="59"/>
-      <c r="L27" s="58"/>
-      <c r="M27" s="66" t="n">
+      <c r="A27" s="56"/>
+      <c r="B27" s="62"/>
+      <c r="C27" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="63"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" s="63"/>
+      <c r="L27" s="62"/>
+      <c r="M27" s="71" t="n">
         <f aca="false">IFERROR(C27 / H27,0)</f>
         <v>0</v>
       </c>
-      <c r="N27" s="67" t="n">
+      <c r="N27" s="72" t="n">
         <f aca="false">IFERROR(D27 / I27,0)</f>
         <v>0</v>
       </c>
-      <c r="O27" s="68" t="n">
+      <c r="O27" s="73" t="n">
         <f aca="false">IFERROR(E27 / J27,0)</f>
         <v>0</v>
       </c>
-      <c r="P27" s="59"/>
-      <c r="Q27" s="69" t="s">
-        <v>41</v>
-      </c>
-      <c r="R27" s="69"/>
-      <c r="S27" s="70" t="n">
+      <c r="P27" s="63"/>
+      <c r="Q27" s="74" t="s">
+        <v>43</v>
+      </c>
+      <c r="R27" s="74"/>
+      <c r="S27" s="75" t="n">
         <f aca="false">SUM(C13,E13,G13,I13,K13,M13,O13,Q13,S13,U13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="52"/>
-      <c r="B28" s="58"/>
-      <c r="C28" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="D28" s="71" t="n">
-        <v>0</v>
-      </c>
-      <c r="E28" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="F28" s="59"/>
-      <c r="G28" s="58"/>
-      <c r="H28" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="I28" s="71" t="n">
-        <v>0</v>
-      </c>
-      <c r="J28" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="K28" s="59"/>
-      <c r="L28" s="58"/>
-      <c r="M28" s="66" t="n">
+      <c r="A28" s="56"/>
+      <c r="B28" s="62"/>
+      <c r="C28" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="63"/>
+      <c r="G28" s="62"/>
+      <c r="H28" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" s="63"/>
+      <c r="L28" s="62"/>
+      <c r="M28" s="71" t="n">
         <f aca="false">IFERROR(C28 / H28,0)</f>
         <v>0</v>
       </c>
-      <c r="N28" s="67" t="n">
+      <c r="N28" s="72" t="n">
         <f aca="false">IFERROR(D28 / I28,0)</f>
         <v>0</v>
       </c>
-      <c r="O28" s="68" t="n">
+      <c r="O28" s="73" t="n">
         <f aca="false">IFERROR(E28 / J28,0)</f>
         <v>0</v>
       </c>
-      <c r="P28" s="59"/>
-      <c r="Q28" s="69" t="s">
-        <v>42</v>
-      </c>
-      <c r="R28" s="69"/>
-      <c r="S28" s="70" t="n">
+      <c r="P28" s="63"/>
+      <c r="Q28" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="R28" s="74"/>
+      <c r="S28" s="75" t="n">
         <f aca="false">SUM(C12,E12,G12,I12,K12,M12,O12,Q12,S12,U12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="72"/>
-      <c r="B29" s="73"/>
-      <c r="C29" s="74"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="75"/>
-      <c r="G29" s="73"/>
-      <c r="H29" s="74"/>
-      <c r="I29" s="74"/>
-      <c r="J29" s="74"/>
-      <c r="K29" s="75"/>
-      <c r="L29" s="73"/>
-      <c r="M29" s="74"/>
-      <c r="N29" s="74"/>
-      <c r="O29" s="74"/>
-      <c r="P29" s="75"/>
-      <c r="Q29" s="69" t="s">
-        <v>43</v>
-      </c>
-      <c r="R29" s="69"/>
-      <c r="S29" s="76" t="n">
+      <c r="A29" s="77"/>
+      <c r="B29" s="78"/>
+      <c r="C29" s="79"/>
+      <c r="D29" s="79"/>
+      <c r="E29" s="79"/>
+      <c r="F29" s="80"/>
+      <c r="G29" s="78"/>
+      <c r="H29" s="79"/>
+      <c r="I29" s="79"/>
+      <c r="J29" s="79"/>
+      <c r="K29" s="80"/>
+      <c r="L29" s="78"/>
+      <c r="M29" s="79"/>
+      <c r="N29" s="79"/>
+      <c r="O29" s="79"/>
+      <c r="P29" s="80"/>
+      <c r="Q29" s="74" t="s">
+        <v>45</v>
+      </c>
+      <c r="R29" s="74"/>
+      <c r="S29" s="81" t="n">
         <f aca="false">IFERROR(S27 / S28,0)</f>
         <v>0</v>
       </c>
@@ -2316,76 +2404,76 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="31"/>
-      <c r="C31" s="77"/>
-      <c r="D31" s="78"/>
-      <c r="E31" s="77"/>
-      <c r="F31" s="77"/>
-      <c r="G31" s="78"/>
-      <c r="H31" s="77"/>
-      <c r="I31" s="77"/>
-      <c r="J31" s="78"/>
-      <c r="K31" s="77"/>
-      <c r="L31" s="77"/>
-      <c r="M31" s="78"/>
-      <c r="N31" s="77"/>
-      <c r="O31" s="77"/>
-      <c r="P31" s="78"/>
-      <c r="Q31" s="77"/>
+      <c r="C31" s="82"/>
+      <c r="D31" s="83"/>
+      <c r="E31" s="82"/>
+      <c r="F31" s="82"/>
+      <c r="G31" s="83"/>
+      <c r="H31" s="82"/>
+      <c r="I31" s="82"/>
+      <c r="J31" s="83"/>
+      <c r="K31" s="82"/>
+      <c r="L31" s="82"/>
+      <c r="M31" s="83"/>
+      <c r="N31" s="82"/>
+      <c r="O31" s="82"/>
+      <c r="P31" s="83"/>
+      <c r="Q31" s="82"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="79" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" s="80"/>
-      <c r="C32" s="80"/>
-      <c r="D32" s="80"/>
-      <c r="E32" s="80"/>
-      <c r="F32" s="80"/>
-      <c r="G32" s="80"/>
-      <c r="H32" s="80"/>
-      <c r="I32" s="80"/>
-      <c r="J32" s="80"/>
-      <c r="K32" s="80"/>
-      <c r="L32" s="80"/>
-      <c r="M32" s="77"/>
-      <c r="N32" s="77"/>
-      <c r="O32" s="77"/>
-      <c r="P32" s="77"/>
-      <c r="Q32" s="77"/>
+      <c r="A32" s="84" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" s="39"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="39"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="39"/>
+      <c r="L32" s="39"/>
+      <c r="M32" s="82"/>
+      <c r="N32" s="82"/>
+      <c r="O32" s="82"/>
+      <c r="P32" s="82"/>
+      <c r="Q32" s="82"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="81" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33" s="82" t="s">
-        <v>50</v>
-      </c>
-      <c r="C33" s="82"/>
-      <c r="D33" s="83" t="s">
+      <c r="A33" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="E33" s="83"/>
-      <c r="F33" s="83" t="s">
+      <c r="B33" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="G33" s="83"/>
-      <c r="H33" s="84" t="s">
+      <c r="C33" s="86"/>
+      <c r="D33" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="I33" s="84"/>
-      <c r="J33" s="85" t="s">
+      <c r="E33" s="87"/>
+      <c r="F33" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="K33" s="85"/>
-      <c r="L33" s="80"/>
-      <c r="M33" s="77"/>
-      <c r="N33" s="77"/>
-      <c r="O33" s="77"/>
-      <c r="P33" s="77"/>
-      <c r="Q33" s="77"/>
+      <c r="G33" s="87"/>
+      <c r="H33" s="88" t="s">
+        <v>55</v>
+      </c>
+      <c r="I33" s="88"/>
+      <c r="J33" s="89" t="s">
+        <v>56</v>
+      </c>
+      <c r="K33" s="89"/>
+      <c r="L33" s="39"/>
+      <c r="M33" s="82"/>
+      <c r="N33" s="82"/>
+      <c r="O33" s="82"/>
+      <c r="P33" s="82"/>
+      <c r="Q33" s="82"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="86" t="s">
+      <c r="A34" s="90" t="s">
         <v>17</v>
       </c>
       <c r="B34" s="24" t="s">
@@ -2418,10 +2506,10 @@
       <c r="K34" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="L34" s="80"/>
+      <c r="L34" s="39"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="86" t="s">
+      <c r="A35" s="90" t="s">
         <v>20</v>
       </c>
       <c r="B35" s="26" t="n">
@@ -2454,7 +2542,7 @@
       <c r="K35" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="L35" s="80"/>
+      <c r="L35" s="39"/>
       <c r="M35" s="19"/>
       <c r="N35" s="19"/>
       <c r="O35" s="19"/>
@@ -2462,7 +2550,7 @@
       <c r="Q35" s="19"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="86" t="s">
+      <c r="A36" s="90" t="s">
         <v>21</v>
       </c>
       <c r="B36" s="26" t="n">
@@ -2495,62 +2583,62 @@
       <c r="K36" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="L36" s="80"/>
-      <c r="O36" s="41"/>
-      <c r="P36" s="41"/>
-      <c r="Q36" s="41"/>
-      <c r="R36" s="87"/>
+      <c r="L36" s="39"/>
+      <c r="O36" s="42"/>
+      <c r="P36" s="42"/>
+      <c r="Q36" s="42"/>
+      <c r="R36" s="91"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="88" t="s">
+      <c r="A37" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="89" t="n">
+      <c r="B37" s="93" t="n">
         <f aca="false">IFERROR(B36 / B35,0)</f>
         <v>0</v>
       </c>
-      <c r="C37" s="90" t="n">
+      <c r="C37" s="94" t="n">
         <f aca="false">IFERROR(C36 / C35,0)</f>
         <v>0</v>
       </c>
-      <c r="D37" s="89" t="n">
+      <c r="D37" s="93" t="n">
         <f aca="false">IFERROR(D36 / D35,0)</f>
         <v>0</v>
       </c>
-      <c r="E37" s="91" t="n">
+      <c r="E37" s="95" t="n">
         <f aca="false">IFERROR(E36 / E35,0)</f>
         <v>0</v>
       </c>
-      <c r="F37" s="90" t="n">
+      <c r="F37" s="94" t="n">
         <f aca="false">IFERROR(F36 / F35,0)</f>
         <v>0</v>
       </c>
-      <c r="G37" s="90" t="n">
+      <c r="G37" s="94" t="n">
         <f aca="false">IFERROR(G36 / G35,0)</f>
         <v>0</v>
       </c>
-      <c r="H37" s="89" t="n">
+      <c r="H37" s="93" t="n">
         <f aca="false">IFERROR(H36 / H35,0)</f>
         <v>0</v>
       </c>
-      <c r="I37" s="91" t="n">
+      <c r="I37" s="95" t="n">
         <f aca="false">IFERROR(I36 / I35,0)</f>
         <v>0</v>
       </c>
-      <c r="J37" s="90" t="n">
+      <c r="J37" s="94" t="n">
         <f aca="false">IFERROR(J36 / J35,0)</f>
         <v>0</v>
       </c>
-      <c r="K37" s="91" t="n">
+      <c r="K37" s="95" t="n">
         <f aca="false">IFERROR(K36 / K35,0)</f>
         <v>0</v>
       </c>
-      <c r="L37" s="80"/>
-      <c r="M37" s="78"/>
-      <c r="N37" s="77"/>
-      <c r="O37" s="77"/>
-      <c r="P37" s="78"/>
-      <c r="Q37" s="77"/>
+      <c r="L37" s="39"/>
+      <c r="M37" s="83"/>
+      <c r="N37" s="82"/>
+      <c r="O37" s="82"/>
+      <c r="P37" s="83"/>
+      <c r="Q37" s="82"/>
       <c r="R37" s="19"/>
       <c r="S37" s="19"/>
       <c r="T37" s="19"/>
@@ -2580,18 +2668,18 @@
       <c r="AR37" s="19"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="81" t="s">
-        <v>55</v>
+      <c r="A38" s="85" t="s">
+        <v>57</v>
       </c>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
-      <c r="D38" s="92" t="str">
+      <c r="D38" s="96" t="str">
         <f aca="false">O1</f>
         <v>YV Kerrat:</v>
       </c>
       <c r="E38" s="14"/>
       <c r="F38" s="14"/>
-      <c r="G38" s="92" t="str">
+      <c r="G38" s="96" t="str">
         <f aca="false">Q1</f>
         <v>AV Kerrat:</v>
       </c>
@@ -2599,12 +2687,12 @@
       <c r="I38" s="14"/>
       <c r="J38" s="14"/>
       <c r="K38" s="14"/>
-      <c r="L38" s="80"/>
-      <c r="M38" s="77"/>
-      <c r="N38" s="77"/>
-      <c r="O38" s="77"/>
-      <c r="P38" s="77"/>
-      <c r="Q38" s="77"/>
+      <c r="L38" s="39"/>
+      <c r="M38" s="82"/>
+      <c r="N38" s="82"/>
+      <c r="O38" s="82"/>
+      <c r="P38" s="82"/>
+      <c r="Q38" s="82"/>
       <c r="R38" s="19"/>
       <c r="S38" s="19"/>
       <c r="T38" s="19"/>
@@ -2634,30 +2722,30 @@
       <c r="AR38" s="19"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="88" t="s">
-        <v>56</v>
+      <c r="A39" s="92" t="s">
+        <v>58</v>
       </c>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
-      <c r="D39" s="93" t="n">
+      <c r="D39" s="97" t="n">
         <f aca="false">IFERROR(D35 / D38,0)</f>
         <v>0</v>
       </c>
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
-      <c r="G39" s="93" t="n">
+      <c r="G39" s="97" t="n">
         <f aca="false">IFERROR(G35 / G38,0)</f>
         <v>0</v>
       </c>
       <c r="H39" s="13"/>
-      <c r="I39" s="94"/>
-      <c r="J39" s="94"/>
+      <c r="I39" s="98"/>
+      <c r="J39" s="98"/>
       <c r="K39" s="13"/>
-      <c r="M39" s="77"/>
-      <c r="N39" s="77"/>
-      <c r="O39" s="77"/>
-      <c r="P39" s="77"/>
-      <c r="Q39" s="77"/>
+      <c r="M39" s="82"/>
+      <c r="N39" s="82"/>
+      <c r="O39" s="82"/>
+      <c r="P39" s="82"/>
+      <c r="Q39" s="82"/>
       <c r="R39" s="19"/>
       <c r="S39" s="19"/>
       <c r="T39" s="19"/>
@@ -2722,31 +2810,31 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="S41" s="19"/>
-      <c r="T41" s="95"/>
-      <c r="U41" s="95"/>
-      <c r="V41" s="95"/>
-      <c r="W41" s="95"/>
-      <c r="X41" s="95"/>
-      <c r="Y41" s="95"/>
-      <c r="Z41" s="95"/>
-      <c r="AA41" s="95"/>
-      <c r="AB41" s="95"/>
-      <c r="AC41" s="95"/>
-      <c r="AD41" s="95"/>
-      <c r="AE41" s="95"/>
+      <c r="T41" s="99"/>
+      <c r="U41" s="99"/>
+      <c r="V41" s="99"/>
+      <c r="W41" s="99"/>
+      <c r="X41" s="99"/>
+      <c r="Y41" s="99"/>
+      <c r="Z41" s="99"/>
+      <c r="AA41" s="99"/>
+      <c r="AB41" s="99"/>
+      <c r="AC41" s="99"/>
+      <c r="AD41" s="99"/>
+      <c r="AE41" s="99"/>
       <c r="AF41" s="19"/>
-      <c r="AG41" s="95"/>
-      <c r="AH41" s="95"/>
-      <c r="AI41" s="95"/>
-      <c r="AJ41" s="95"/>
-      <c r="AK41" s="95"/>
-      <c r="AL41" s="95"/>
-      <c r="AM41" s="95"/>
-      <c r="AN41" s="95"/>
-      <c r="AO41" s="95"/>
-      <c r="AP41" s="95"/>
-      <c r="AQ41" s="95"/>
-      <c r="AR41" s="95"/>
+      <c r="AG41" s="99"/>
+      <c r="AH41" s="99"/>
+      <c r="AI41" s="99"/>
+      <c r="AJ41" s="99"/>
+      <c r="AK41" s="99"/>
+      <c r="AL41" s="99"/>
+      <c r="AM41" s="99"/>
+      <c r="AN41" s="99"/>
+      <c r="AO41" s="99"/>
+      <c r="AP41" s="99"/>
+      <c r="AQ41" s="99"/>
+      <c r="AR41" s="99"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="18"/>
@@ -3592,7 +3680,7 @@
       <c r="A66" s="19"/>
       <c r="C66" s="19"/>
       <c r="D66" s="19"/>
-      <c r="E66" s="96" t="str">
+      <c r="E66" s="100" t="str">
         <f aca="false">IFERROR(C66 / D66, "")</f>
         <v/>
       </c>
@@ -3600,7 +3688,7 @@
       <c r="G66" s="19"/>
       <c r="I66" s="19"/>
       <c r="J66" s="19"/>
-      <c r="K66" s="96" t="str">
+      <c r="K66" s="100" t="str">
         <f aca="false">IFERROR(I66 / J66, "")</f>
         <v/>
       </c>
@@ -3608,7 +3696,7 @@
       <c r="M66" s="19"/>
       <c r="O66" s="19"/>
       <c r="P66" s="19"/>
-      <c r="Q66" s="96" t="str">
+      <c r="Q66" s="100" t="str">
         <f aca="false">IFERROR(O66 / P66, "")</f>
         <v/>
       </c>
@@ -3616,35 +3704,35 @@
       <c r="S66" s="19"/>
       <c r="U66" s="19"/>
       <c r="V66" s="19"/>
-      <c r="W66" s="96" t="str">
+      <c r="W66" s="100" t="str">
         <f aca="false">IFERROR(U66 / V66, "")</f>
         <v/>
       </c>
       <c r="X66" s="19"/>
       <c r="Z66" s="19"/>
       <c r="AA66" s="19"/>
-      <c r="AB66" s="96" t="str">
+      <c r="AB66" s="100" t="str">
         <f aca="false">IFERROR(Z66 / AA66, "")</f>
         <v/>
       </c>
       <c r="AC66" s="19"/>
       <c r="AE66" s="19"/>
       <c r="AF66" s="19"/>
-      <c r="AG66" s="96" t="str">
+      <c r="AG66" s="100" t="str">
         <f aca="false">IFERROR(AE66 / AF66, "")</f>
         <v/>
       </c>
       <c r="AH66" s="19"/>
       <c r="AJ66" s="19"/>
       <c r="AK66" s="19"/>
-      <c r="AL66" s="96" t="str">
+      <c r="AL66" s="100" t="str">
         <f aca="false">IFERROR(AJ66 / AK66, "")</f>
         <v/>
       </c>
       <c r="AM66" s="19"/>
       <c r="AO66" s="19"/>
       <c r="AP66" s="19"/>
-      <c r="AQ66" s="96" t="str">
+      <c r="AQ66" s="100" t="str">
         <f aca="false">IFERROR(AO66 / AP66, "")</f>
         <v/>
       </c>
@@ -5060,7 +5148,7 @@
       <c r="E114" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="46">
+  <mergeCells count="50">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="J1:L1"/>
@@ -5089,6 +5177,10 @@
     <mergeCell ref="H17:J17"/>
     <mergeCell ref="M17:O17"/>
     <mergeCell ref="Q18:S19"/>
+    <mergeCell ref="T18:W19"/>
+    <mergeCell ref="X18:Y18"/>
+    <mergeCell ref="Z18:AC19"/>
+    <mergeCell ref="X19:Y19"/>
     <mergeCell ref="Q20:R20"/>
     <mergeCell ref="Q21:R21"/>
     <mergeCell ref="Q22:R22"/>
@@ -5125,8 +5217,8 @@
   </sheetPr>
   <dimension ref="A1:AR114"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X20" activeCellId="0" sqref="X20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5146,14 +5238,14 @@
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
       <c r="F1" s="15"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="97"/>
-      <c r="N1" s="97"/>
+      <c r="G1" s="101"/>
+      <c r="H1" s="101"/>
+      <c r="I1" s="101"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="101"/>
+      <c r="N1" s="101"/>
       <c r="O1" s="18"/>
       <c r="P1" s="19"/>
       <c r="Q1" s="18"/>
@@ -5770,6 +5862,14 @@
       <c r="U13" s="27" t="n">
         <v>0</v>
       </c>
+      <c r="V13" s="39"/>
+      <c r="W13" s="39"/>
+      <c r="X13" s="39"/>
+      <c r="Y13" s="39"/>
+      <c r="Z13" s="39"/>
+      <c r="AA13" s="39"/>
+      <c r="AB13" s="39"/>
+      <c r="AC13" s="39"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="33" t="s">
@@ -5783,11 +5883,11 @@
         <f aca="false">IFERROR(C13 / C12,0)</f>
         <v>0</v>
       </c>
-      <c r="D14" s="39" t="n">
+      <c r="D14" s="40" t="n">
         <f aca="false">IFERROR(D13 / D12,0)</f>
         <v>0</v>
       </c>
-      <c r="E14" s="39" t="n">
+      <c r="E14" s="40" t="n">
         <f aca="false">IFERROR(E13 / E12,0)</f>
         <v>0</v>
       </c>
@@ -5799,11 +5899,11 @@
         <f aca="false">IFERROR(G13 / G12,0)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="39" t="n">
+      <c r="H14" s="40" t="n">
         <f aca="false">IFERROR(H13 / H12,0)</f>
         <v>0</v>
       </c>
-      <c r="I14" s="39" t="n">
+      <c r="I14" s="40" t="n">
         <f aca="false">IFERROR(I13 / I12,0)</f>
         <v>0</v>
       </c>
@@ -5815,11 +5915,11 @@
         <f aca="false">IFERROR(K13 / K12,0)</f>
         <v>0</v>
       </c>
-      <c r="L14" s="39" t="n">
+      <c r="L14" s="40" t="n">
         <f aca="false">IFERROR(L13 / L12,0)</f>
         <v>0</v>
       </c>
-      <c r="M14" s="39" t="n">
+      <c r="M14" s="40" t="n">
         <f aca="false">IFERROR(M13 / M12,0)</f>
         <v>0</v>
       </c>
@@ -5831,11 +5931,11 @@
         <f aca="false">IFERROR(O13 / O12,0)</f>
         <v>0</v>
       </c>
-      <c r="P14" s="39" t="n">
+      <c r="P14" s="40" t="n">
         <f aca="false">IFERROR(P13 / P12,0)</f>
         <v>0</v>
       </c>
-      <c r="Q14" s="39" t="n">
+      <c r="Q14" s="40" t="n">
         <f aca="false">IFERROR(Q13 / Q12,0)</f>
         <v>0</v>
       </c>
@@ -5847,7 +5947,7 @@
         <f aca="false">IFERROR(S13 / S12,0)</f>
         <v>0</v>
       </c>
-      <c r="T14" s="39" t="n">
+      <c r="T14" s="40" t="n">
         <f aca="false">IFERROR(T13 / T12,0)</f>
         <v>0</v>
       </c>
@@ -5855,6 +5955,14 @@
         <f aca="false">IFERROR(U13 / U12,0)</f>
         <v>0</v>
       </c>
+      <c r="V14" s="39"/>
+      <c r="W14" s="39"/>
+      <c r="X14" s="39"/>
+      <c r="Y14" s="39"/>
+      <c r="Z14" s="39"/>
+      <c r="AA14" s="39"/>
+      <c r="AB14" s="39"/>
+      <c r="AC14" s="39"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="31"/>
@@ -5893,29 +6001,29 @@
       <c r="U16" s="19"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="41" t="s">
         <v>35</v>
       </c>
       <c r="B17" s="19"/>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
-      <c r="H17" s="42" t="s">
+      <c r="H17" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
       <c r="K17" s="19"/>
       <c r="L17" s="19"/>
-      <c r="M17" s="41" t="s">
+      <c r="M17" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="N17" s="41"/>
-      <c r="O17" s="41"/>
+      <c r="N17" s="42"/>
+      <c r="O17" s="42"/>
       <c r="P17" s="19"/>
       <c r="Q17" s="19"/>
       <c r="R17" s="19"/>
@@ -5924,119 +6032,151 @@
       <c r="U17" s="19"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="44"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="50"/>
-      <c r="L18" s="48"/>
-      <c r="M18" s="49"/>
-      <c r="N18" s="49"/>
-      <c r="O18" s="45"/>
-      <c r="P18" s="50"/>
-      <c r="Q18" s="51" t="s">
+      <c r="B18" s="45"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="51"/>
+      <c r="L18" s="49"/>
+      <c r="M18" s="50"/>
+      <c r="N18" s="50"/>
+      <c r="O18" s="46"/>
+      <c r="P18" s="51"/>
+      <c r="Q18" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="R18" s="51"/>
-      <c r="S18" s="51"/>
-      <c r="T18" s="19"/>
-      <c r="U18" s="19"/>
+      <c r="R18" s="52"/>
+      <c r="S18" s="52"/>
+      <c r="T18" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="U18" s="53"/>
+      <c r="V18" s="53"/>
+      <c r="W18" s="53"/>
+      <c r="X18" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y18" s="54"/>
+      <c r="Z18" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA18" s="55"/>
+      <c r="AB18" s="55"/>
+      <c r="AC18" s="55"/>
+      <c r="AD18" s="39"/>
+      <c r="AE18" s="39"/>
+      <c r="AF18" s="39"/>
+      <c r="AG18" s="39"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="52"/>
-      <c r="B19" s="53"/>
-      <c r="C19" s="54" t="n">
+      <c r="A19" s="56"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="58" t="n">
         <v>1</v>
       </c>
-      <c r="D19" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" s="57"/>
-      <c r="G19" s="58"/>
-      <c r="H19" s="54" t="n">
+      <c r="D19" s="59" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="61"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="58" t="n">
         <v>3</v>
       </c>
-      <c r="I19" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="J19" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="K19" s="59"/>
-      <c r="L19" s="58"/>
-      <c r="M19" s="60" t="n">
+      <c r="I19" s="59" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" s="63"/>
+      <c r="L19" s="62"/>
+      <c r="M19" s="64" t="n">
         <f aca="false">IFERROR(C19 / H19,0)</f>
         <v>0.333333333333333</v>
       </c>
-      <c r="N19" s="61" t="n">
+      <c r="N19" s="65" t="n">
         <f aca="false">IFERROR(D19 / I19,0)</f>
         <v>0</v>
       </c>
-      <c r="O19" s="62" t="n">
+      <c r="O19" s="66" t="n">
         <f aca="false">IFERROR(E19 / J19,0)</f>
         <v>0</v>
       </c>
-      <c r="P19" s="59"/>
-      <c r="Q19" s="51"/>
-      <c r="R19" s="51"/>
-      <c r="S19" s="51"/>
-      <c r="T19" s="19"/>
-      <c r="U19" s="19"/>
+      <c r="P19" s="63"/>
+      <c r="Q19" s="52"/>
+      <c r="R19" s="52"/>
+      <c r="S19" s="52"/>
+      <c r="T19" s="53"/>
+      <c r="U19" s="53"/>
+      <c r="V19" s="53"/>
+      <c r="W19" s="53"/>
+      <c r="X19" s="67" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y19" s="67"/>
+      <c r="Z19" s="55"/>
+      <c r="AA19" s="55"/>
+      <c r="AB19" s="55"/>
+      <c r="AC19" s="55"/>
+      <c r="AD19" s="39"/>
+      <c r="AE19" s="39"/>
+      <c r="AF19" s="39"/>
+      <c r="AG19" s="39"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="52"/>
-      <c r="B20" s="53"/>
-      <c r="C20" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" s="57"/>
-      <c r="G20" s="58"/>
-      <c r="H20" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="J20" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="K20" s="59"/>
-      <c r="L20" s="58"/>
-      <c r="M20" s="66" t="n">
+      <c r="A20" s="56"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="61"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" s="63"/>
+      <c r="L20" s="62"/>
+      <c r="M20" s="71" t="n">
         <f aca="false">IFERROR(C20 / H20,0)</f>
         <v>0</v>
       </c>
-      <c r="N20" s="67" t="n">
+      <c r="N20" s="72" t="n">
         <f aca="false">IFERROR(D20 / I20,0)</f>
         <v>0</v>
       </c>
-      <c r="O20" s="68" t="n">
+      <c r="O20" s="73" t="n">
         <f aca="false">IFERROR(E20 / J20,0)</f>
         <v>0</v>
       </c>
-      <c r="P20" s="59"/>
-      <c r="Q20" s="69" t="s">
-        <v>41</v>
-      </c>
-      <c r="R20" s="69"/>
-      <c r="S20" s="70" t="n">
+      <c r="P20" s="63"/>
+      <c r="Q20" s="74" t="s">
+        <v>43</v>
+      </c>
+      <c r="R20" s="74"/>
+      <c r="S20" s="75" t="n">
         <f aca="false">SUM(B13,D13,F13,H13,J13,L13,N13,P13,R13,T13)</f>
         <v>0</v>
       </c>
@@ -6044,74 +6184,74 @@
       <c r="U20" s="19"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="52"/>
-      <c r="B21" s="53"/>
-      <c r="C21" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" s="71" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" s="57"/>
-      <c r="G21" s="58"/>
-      <c r="H21" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="I21" s="71" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" s="59"/>
-      <c r="L21" s="58"/>
-      <c r="M21" s="66" t="n">
+      <c r="A21" s="56"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="61"/>
+      <c r="G21" s="62"/>
+      <c r="H21" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" s="63"/>
+      <c r="L21" s="62"/>
+      <c r="M21" s="71" t="n">
         <f aca="false">IFERROR(C21 / H21,0)</f>
         <v>0</v>
       </c>
-      <c r="N21" s="67" t="n">
+      <c r="N21" s="72" t="n">
         <f aca="false">IFERROR(D21 / I21,0)</f>
         <v>0</v>
       </c>
-      <c r="O21" s="68" t="n">
+      <c r="O21" s="73" t="n">
         <f aca="false">IFERROR(E21 / J21,0)</f>
         <v>0</v>
       </c>
-      <c r="P21" s="59"/>
-      <c r="Q21" s="69" t="s">
-        <v>42</v>
-      </c>
-      <c r="R21" s="69"/>
-      <c r="S21" s="70" t="n">
+      <c r="P21" s="63"/>
+      <c r="Q21" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="R21" s="74"/>
+      <c r="S21" s="75" t="n">
         <f aca="false">SUM(B12,D12,F12,H12,J12,L12,N12,P12,R12,T12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="72"/>
-      <c r="B22" s="73"/>
-      <c r="C22" s="74"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="74"/>
-      <c r="F22" s="75"/>
-      <c r="G22" s="73"/>
-      <c r="H22" s="74"/>
-      <c r="I22" s="74"/>
-      <c r="J22" s="74"/>
-      <c r="K22" s="75"/>
-      <c r="L22" s="73"/>
-      <c r="M22" s="74"/>
-      <c r="N22" s="74"/>
-      <c r="O22" s="74"/>
-      <c r="P22" s="75"/>
-      <c r="Q22" s="69" t="s">
-        <v>43</v>
-      </c>
-      <c r="R22" s="69"/>
-      <c r="S22" s="76" t="n">
+      <c r="A22" s="77"/>
+      <c r="B22" s="78"/>
+      <c r="C22" s="79"/>
+      <c r="D22" s="79"/>
+      <c r="E22" s="79"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="78"/>
+      <c r="H22" s="79"/>
+      <c r="I22" s="79"/>
+      <c r="J22" s="79"/>
+      <c r="K22" s="80"/>
+      <c r="L22" s="78"/>
+      <c r="M22" s="79"/>
+      <c r="N22" s="79"/>
+      <c r="O22" s="79"/>
+      <c r="P22" s="80"/>
+      <c r="Q22" s="74" t="s">
+        <v>45</v>
+      </c>
+      <c r="R22" s="74"/>
+      <c r="S22" s="81" t="n">
         <f aca="false">IFERROR(S20 / S21,0)</f>
         <v>0</v>
       </c>
@@ -6126,213 +6266,213 @@
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="18"/>
       <c r="B24" s="19"/>
-      <c r="C24" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
+      <c r="C24" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
       <c r="F24" s="19"/>
       <c r="G24" s="18"/>
-      <c r="H24" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
+      <c r="H24" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
       <c r="K24" s="19"/>
       <c r="L24" s="19"/>
-      <c r="M24" s="41" t="s">
+      <c r="M24" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="N24" s="41"/>
-      <c r="O24" s="41"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="42"/>
       <c r="P24" s="19"/>
       <c r="Q24" s="19"/>
       <c r="R24" s="19"/>
       <c r="S24" s="19"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="48"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="45"/>
-      <c r="K25" s="50"/>
-      <c r="L25" s="48"/>
-      <c r="M25" s="49"/>
-      <c r="N25" s="49"/>
-      <c r="O25" s="45"/>
-      <c r="P25" s="50"/>
-      <c r="Q25" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="R25" s="51"/>
-      <c r="S25" s="51"/>
+      <c r="A25" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="49"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="51"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="50"/>
+      <c r="N25" s="50"/>
+      <c r="O25" s="46"/>
+      <c r="P25" s="51"/>
+      <c r="Q25" s="52" t="s">
+        <v>49</v>
+      </c>
+      <c r="R25" s="52"/>
+      <c r="S25" s="52"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="52"/>
-      <c r="B26" s="58"/>
-      <c r="C26" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" s="59"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="I26" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="J26" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="K26" s="59"/>
-      <c r="L26" s="58"/>
-      <c r="M26" s="60" t="n">
+      <c r="A26" s="56"/>
+      <c r="B26" s="62"/>
+      <c r="C26" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="59" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="63"/>
+      <c r="G26" s="62"/>
+      <c r="H26" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" s="59" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" s="63"/>
+      <c r="L26" s="62"/>
+      <c r="M26" s="64" t="n">
         <f aca="false">IFERROR(C26 / H26,0)</f>
         <v>0</v>
       </c>
-      <c r="N26" s="61" t="n">
+      <c r="N26" s="65" t="n">
         <f aca="false">IFERROR(D26 / I26,0)</f>
         <v>0</v>
       </c>
-      <c r="O26" s="62" t="n">
+      <c r="O26" s="66" t="n">
         <f aca="false">IFERROR(E26 / J26,0)</f>
         <v>0</v>
       </c>
-      <c r="P26" s="59"/>
-      <c r="Q26" s="51"/>
-      <c r="R26" s="51"/>
-      <c r="S26" s="51"/>
+      <c r="P26" s="63"/>
+      <c r="Q26" s="52"/>
+      <c r="R26" s="52"/>
+      <c r="S26" s="52"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="52"/>
-      <c r="B27" s="58"/>
-      <c r="C27" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="D27" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="E27" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" s="59"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="I27" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="J27" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="K27" s="59"/>
-      <c r="L27" s="58"/>
-      <c r="M27" s="66" t="n">
+      <c r="A27" s="56"/>
+      <c r="B27" s="62"/>
+      <c r="C27" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="63"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" s="63"/>
+      <c r="L27" s="62"/>
+      <c r="M27" s="71" t="n">
         <f aca="false">IFERROR(C27 / H27,0)</f>
         <v>0</v>
       </c>
-      <c r="N27" s="67" t="n">
+      <c r="N27" s="72" t="n">
         <f aca="false">IFERROR(D27 / I27,0)</f>
         <v>0</v>
       </c>
-      <c r="O27" s="68" t="n">
+      <c r="O27" s="73" t="n">
         <f aca="false">IFERROR(E27 / J27,0)</f>
         <v>0</v>
       </c>
-      <c r="P27" s="59"/>
-      <c r="Q27" s="69" t="s">
-        <v>41</v>
-      </c>
-      <c r="R27" s="69"/>
-      <c r="S27" s="70" t="n">
+      <c r="P27" s="63"/>
+      <c r="Q27" s="74" t="s">
+        <v>43</v>
+      </c>
+      <c r="R27" s="74"/>
+      <c r="S27" s="75" t="n">
         <f aca="false">SUM(C13,E13,G13,I13,K13,M13,O13,Q13,S13,U13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="52"/>
-      <c r="B28" s="58"/>
-      <c r="C28" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="D28" s="71" t="n">
-        <v>0</v>
-      </c>
-      <c r="E28" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="F28" s="59"/>
-      <c r="G28" s="58"/>
-      <c r="H28" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="I28" s="71" t="n">
-        <v>0</v>
-      </c>
-      <c r="J28" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="K28" s="59"/>
-      <c r="L28" s="58"/>
-      <c r="M28" s="66" t="n">
+      <c r="A28" s="56"/>
+      <c r="B28" s="62"/>
+      <c r="C28" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="63"/>
+      <c r="G28" s="62"/>
+      <c r="H28" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" s="63"/>
+      <c r="L28" s="62"/>
+      <c r="M28" s="71" t="n">
         <f aca="false">IFERROR(C28 / H28,0)</f>
         <v>0</v>
       </c>
-      <c r="N28" s="67" t="n">
+      <c r="N28" s="72" t="n">
         <f aca="false">IFERROR(D28 / I28,0)</f>
         <v>0</v>
       </c>
-      <c r="O28" s="68" t="n">
+      <c r="O28" s="73" t="n">
         <f aca="false">IFERROR(E28 / J28,0)</f>
         <v>0</v>
       </c>
-      <c r="P28" s="59"/>
-      <c r="Q28" s="69" t="s">
-        <v>42</v>
-      </c>
-      <c r="R28" s="69"/>
-      <c r="S28" s="70" t="n">
+      <c r="P28" s="63"/>
+      <c r="Q28" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="R28" s="74"/>
+      <c r="S28" s="75" t="n">
         <f aca="false">SUM(C12,E12,G12,I12,K12,M12,O12,Q12,S12,U12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="72"/>
-      <c r="B29" s="73"/>
-      <c r="C29" s="74"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="75"/>
-      <c r="G29" s="73"/>
-      <c r="H29" s="74"/>
-      <c r="I29" s="74"/>
-      <c r="J29" s="74"/>
-      <c r="K29" s="75"/>
-      <c r="L29" s="73"/>
-      <c r="M29" s="74"/>
-      <c r="N29" s="74"/>
-      <c r="O29" s="74"/>
-      <c r="P29" s="75"/>
-      <c r="Q29" s="69" t="s">
-        <v>43</v>
-      </c>
-      <c r="R29" s="69"/>
-      <c r="S29" s="76" t="n">
+      <c r="A29" s="77"/>
+      <c r="B29" s="78"/>
+      <c r="C29" s="79"/>
+      <c r="D29" s="79"/>
+      <c r="E29" s="79"/>
+      <c r="F29" s="80"/>
+      <c r="G29" s="78"/>
+      <c r="H29" s="79"/>
+      <c r="I29" s="79"/>
+      <c r="J29" s="79"/>
+      <c r="K29" s="80"/>
+      <c r="L29" s="78"/>
+      <c r="M29" s="79"/>
+      <c r="N29" s="79"/>
+      <c r="O29" s="79"/>
+      <c r="P29" s="80"/>
+      <c r="Q29" s="74" t="s">
+        <v>45</v>
+      </c>
+      <c r="R29" s="74"/>
+      <c r="S29" s="81" t="n">
         <f aca="false">IFERROR(S27 / S28,0)</f>
         <v>0</v>
       </c>
@@ -6342,76 +6482,76 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="31"/>
-      <c r="C31" s="77"/>
-      <c r="D31" s="78"/>
-      <c r="E31" s="77"/>
-      <c r="F31" s="77"/>
-      <c r="G31" s="78"/>
-      <c r="H31" s="77"/>
-      <c r="I31" s="77"/>
-      <c r="J31" s="78"/>
-      <c r="K31" s="77"/>
-      <c r="L31" s="77"/>
-      <c r="M31" s="78"/>
-      <c r="N31" s="77"/>
-      <c r="O31" s="77"/>
-      <c r="P31" s="78"/>
-      <c r="Q31" s="77"/>
+      <c r="C31" s="82"/>
+      <c r="D31" s="83"/>
+      <c r="E31" s="82"/>
+      <c r="F31" s="82"/>
+      <c r="G31" s="83"/>
+      <c r="H31" s="82"/>
+      <c r="I31" s="82"/>
+      <c r="J31" s="83"/>
+      <c r="K31" s="82"/>
+      <c r="L31" s="82"/>
+      <c r="M31" s="83"/>
+      <c r="N31" s="82"/>
+      <c r="O31" s="82"/>
+      <c r="P31" s="83"/>
+      <c r="Q31" s="82"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="79" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" s="80"/>
-      <c r="C32" s="80"/>
-      <c r="D32" s="80"/>
-      <c r="E32" s="80"/>
-      <c r="F32" s="80"/>
-      <c r="G32" s="80"/>
-      <c r="H32" s="80"/>
-      <c r="I32" s="80"/>
-      <c r="J32" s="80"/>
-      <c r="K32" s="80"/>
-      <c r="L32" s="80"/>
-      <c r="M32" s="77"/>
-      <c r="N32" s="77"/>
-      <c r="O32" s="77"/>
-      <c r="P32" s="77"/>
-      <c r="Q32" s="77"/>
+      <c r="A32" s="84" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" s="39"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="39"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="39"/>
+      <c r="L32" s="39"/>
+      <c r="M32" s="82"/>
+      <c r="N32" s="82"/>
+      <c r="O32" s="82"/>
+      <c r="P32" s="82"/>
+      <c r="Q32" s="82"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="81" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33" s="82" t="s">
-        <v>50</v>
-      </c>
-      <c r="C33" s="82"/>
-      <c r="D33" s="83" t="s">
+      <c r="A33" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="E33" s="83"/>
-      <c r="F33" s="83" t="s">
+      <c r="B33" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="G33" s="83"/>
-      <c r="H33" s="84" t="s">
+      <c r="C33" s="86"/>
+      <c r="D33" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="I33" s="84"/>
-      <c r="J33" s="85" t="s">
+      <c r="E33" s="87"/>
+      <c r="F33" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="K33" s="85"/>
-      <c r="L33" s="80"/>
-      <c r="M33" s="77"/>
-      <c r="N33" s="77"/>
-      <c r="O33" s="77"/>
-      <c r="P33" s="77"/>
-      <c r="Q33" s="77"/>
+      <c r="G33" s="87"/>
+      <c r="H33" s="88" t="s">
+        <v>55</v>
+      </c>
+      <c r="I33" s="88"/>
+      <c r="J33" s="89" t="s">
+        <v>56</v>
+      </c>
+      <c r="K33" s="89"/>
+      <c r="L33" s="39"/>
+      <c r="M33" s="82"/>
+      <c r="N33" s="82"/>
+      <c r="O33" s="82"/>
+      <c r="P33" s="82"/>
+      <c r="Q33" s="82"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="86" t="s">
+      <c r="A34" s="90" t="s">
         <v>17</v>
       </c>
       <c r="B34" s="24" t="s">
@@ -6444,10 +6584,10 @@
       <c r="K34" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="L34" s="80"/>
+      <c r="L34" s="39"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="86" t="s">
+      <c r="A35" s="90" t="s">
         <v>20</v>
       </c>
       <c r="B35" s="26" t="n">
@@ -6480,7 +6620,7 @@
       <c r="K35" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="L35" s="80"/>
+      <c r="L35" s="39"/>
       <c r="M35" s="19"/>
       <c r="N35" s="19"/>
       <c r="O35" s="19"/>
@@ -6488,7 +6628,7 @@
       <c r="Q35" s="19"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="86" t="s">
+      <c r="A36" s="90" t="s">
         <v>21</v>
       </c>
       <c r="B36" s="26" t="n">
@@ -6521,62 +6661,62 @@
       <c r="K36" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="L36" s="80"/>
-      <c r="O36" s="41"/>
-      <c r="P36" s="41"/>
-      <c r="Q36" s="41"/>
-      <c r="R36" s="87"/>
+      <c r="L36" s="39"/>
+      <c r="O36" s="42"/>
+      <c r="P36" s="42"/>
+      <c r="Q36" s="42"/>
+      <c r="R36" s="91"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="88" t="s">
+      <c r="A37" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="89" t="n">
+      <c r="B37" s="93" t="n">
         <f aca="false">IFERROR(B36 / B35,0)</f>
         <v>0</v>
       </c>
-      <c r="C37" s="90" t="n">
+      <c r="C37" s="94" t="n">
         <f aca="false">IFERROR(C36 / C35,0)</f>
         <v>0</v>
       </c>
-      <c r="D37" s="89" t="n">
+      <c r="D37" s="93" t="n">
         <f aca="false">IFERROR(D36 / D35,0)</f>
         <v>0</v>
       </c>
-      <c r="E37" s="91" t="n">
+      <c r="E37" s="95" t="n">
         <f aca="false">IFERROR(E36 / E35,0)</f>
         <v>0</v>
       </c>
-      <c r="F37" s="90" t="n">
+      <c r="F37" s="94" t="n">
         <f aca="false">IFERROR(F36 / F35,0)</f>
         <v>0</v>
       </c>
-      <c r="G37" s="90" t="n">
+      <c r="G37" s="94" t="n">
         <f aca="false">IFERROR(G36 / G35,0)</f>
         <v>0</v>
       </c>
-      <c r="H37" s="89" t="n">
+      <c r="H37" s="93" t="n">
         <f aca="false">IFERROR(H36 / H35,0)</f>
         <v>0</v>
       </c>
-      <c r="I37" s="91" t="n">
+      <c r="I37" s="95" t="n">
         <f aca="false">IFERROR(I36 / I35,0)</f>
         <v>0</v>
       </c>
-      <c r="J37" s="90" t="n">
+      <c r="J37" s="94" t="n">
         <f aca="false">IFERROR(J36 / J35,0)</f>
         <v>0</v>
       </c>
-      <c r="K37" s="91" t="n">
+      <c r="K37" s="95" t="n">
         <f aca="false">IFERROR(K36 / K35,0)</f>
         <v>0</v>
       </c>
-      <c r="L37" s="80"/>
-      <c r="M37" s="78"/>
-      <c r="N37" s="77"/>
-      <c r="O37" s="77"/>
-      <c r="P37" s="78"/>
-      <c r="Q37" s="77"/>
+      <c r="L37" s="39"/>
+      <c r="M37" s="83"/>
+      <c r="N37" s="82"/>
+      <c r="O37" s="82"/>
+      <c r="P37" s="83"/>
+      <c r="Q37" s="82"/>
       <c r="R37" s="19"/>
       <c r="S37" s="19"/>
       <c r="T37" s="19"/>
@@ -6606,18 +6746,18 @@
       <c r="AR37" s="19"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="81" t="s">
-        <v>55</v>
+      <c r="A38" s="85" t="s">
+        <v>57</v>
       </c>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
-      <c r="D38" s="92" t="n">
+      <c r="D38" s="96" t="n">
         <f aca="false">O1</f>
         <v>0</v>
       </c>
       <c r="E38" s="14"/>
       <c r="F38" s="14"/>
-      <c r="G38" s="92" t="n">
+      <c r="G38" s="96" t="n">
         <f aca="false">Q1</f>
         <v>0</v>
       </c>
@@ -6625,12 +6765,12 @@
       <c r="I38" s="14"/>
       <c r="J38" s="14"/>
       <c r="K38" s="14"/>
-      <c r="L38" s="80"/>
-      <c r="M38" s="77"/>
-      <c r="N38" s="77"/>
-      <c r="O38" s="77"/>
-      <c r="P38" s="77"/>
-      <c r="Q38" s="77"/>
+      <c r="L38" s="39"/>
+      <c r="M38" s="82"/>
+      <c r="N38" s="82"/>
+      <c r="O38" s="82"/>
+      <c r="P38" s="82"/>
+      <c r="Q38" s="82"/>
       <c r="R38" s="19"/>
       <c r="S38" s="19"/>
       <c r="T38" s="19"/>
@@ -6660,30 +6800,30 @@
       <c r="AR38" s="19"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="88" t="s">
-        <v>56</v>
+      <c r="A39" s="92" t="s">
+        <v>58</v>
       </c>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
-      <c r="D39" s="93" t="n">
+      <c r="D39" s="97" t="n">
         <f aca="false">IFERROR(D35 / D38,0)</f>
         <v>0</v>
       </c>
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
-      <c r="G39" s="93" t="n">
+      <c r="G39" s="97" t="n">
         <f aca="false">IFERROR(G35 / G38,0)</f>
         <v>0</v>
       </c>
       <c r="H39" s="13"/>
-      <c r="I39" s="94"/>
-      <c r="J39" s="94"/>
+      <c r="I39" s="98"/>
+      <c r="J39" s="98"/>
       <c r="K39" s="13"/>
-      <c r="M39" s="77"/>
-      <c r="N39" s="77"/>
-      <c r="O39" s="77"/>
-      <c r="P39" s="77"/>
-      <c r="Q39" s="77"/>
+      <c r="M39" s="82"/>
+      <c r="N39" s="82"/>
+      <c r="O39" s="82"/>
+      <c r="P39" s="82"/>
+      <c r="Q39" s="82"/>
       <c r="R39" s="19"/>
       <c r="S39" s="19"/>
       <c r="T39" s="19"/>
@@ -6748,31 +6888,31 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="S41" s="19"/>
-      <c r="T41" s="95"/>
-      <c r="U41" s="95"/>
-      <c r="V41" s="95"/>
-      <c r="W41" s="95"/>
-      <c r="X41" s="95"/>
-      <c r="Y41" s="95"/>
-      <c r="Z41" s="95"/>
-      <c r="AA41" s="95"/>
-      <c r="AB41" s="95"/>
-      <c r="AC41" s="95"/>
-      <c r="AD41" s="95"/>
-      <c r="AE41" s="95"/>
+      <c r="T41" s="99"/>
+      <c r="U41" s="99"/>
+      <c r="V41" s="99"/>
+      <c r="W41" s="99"/>
+      <c r="X41" s="99"/>
+      <c r="Y41" s="99"/>
+      <c r="Z41" s="99"/>
+      <c r="AA41" s="99"/>
+      <c r="AB41" s="99"/>
+      <c r="AC41" s="99"/>
+      <c r="AD41" s="99"/>
+      <c r="AE41" s="99"/>
       <c r="AF41" s="19"/>
-      <c r="AG41" s="95"/>
-      <c r="AH41" s="95"/>
-      <c r="AI41" s="95"/>
-      <c r="AJ41" s="95"/>
-      <c r="AK41" s="95"/>
-      <c r="AL41" s="95"/>
-      <c r="AM41" s="95"/>
-      <c r="AN41" s="95"/>
-      <c r="AO41" s="95"/>
-      <c r="AP41" s="95"/>
-      <c r="AQ41" s="95"/>
-      <c r="AR41" s="95"/>
+      <c r="AG41" s="99"/>
+      <c r="AH41" s="99"/>
+      <c r="AI41" s="99"/>
+      <c r="AJ41" s="99"/>
+      <c r="AK41" s="99"/>
+      <c r="AL41" s="99"/>
+      <c r="AM41" s="99"/>
+      <c r="AN41" s="99"/>
+      <c r="AO41" s="99"/>
+      <c r="AP41" s="99"/>
+      <c r="AQ41" s="99"/>
+      <c r="AR41" s="99"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="18"/>
@@ -7618,7 +7758,7 @@
       <c r="A66" s="19"/>
       <c r="C66" s="19"/>
       <c r="D66" s="19"/>
-      <c r="E66" s="96" t="str">
+      <c r="E66" s="100" t="str">
         <f aca="false">IFERROR(C66 / D66, "")</f>
         <v/>
       </c>
@@ -7626,7 +7766,7 @@
       <c r="G66" s="19"/>
       <c r="I66" s="19"/>
       <c r="J66" s="19"/>
-      <c r="K66" s="96" t="str">
+      <c r="K66" s="100" t="str">
         <f aca="false">IFERROR(I66 / J66, "")</f>
         <v/>
       </c>
@@ -7634,7 +7774,7 @@
       <c r="M66" s="19"/>
       <c r="O66" s="19"/>
       <c r="P66" s="19"/>
-      <c r="Q66" s="96" t="str">
+      <c r="Q66" s="100" t="str">
         <f aca="false">IFERROR(O66 / P66, "")</f>
         <v/>
       </c>
@@ -7642,35 +7782,35 @@
       <c r="S66" s="19"/>
       <c r="U66" s="19"/>
       <c r="V66" s="19"/>
-      <c r="W66" s="96" t="str">
+      <c r="W66" s="100" t="str">
         <f aca="false">IFERROR(U66 / V66, "")</f>
         <v/>
       </c>
       <c r="X66" s="19"/>
       <c r="Z66" s="19"/>
       <c r="AA66" s="19"/>
-      <c r="AB66" s="96" t="str">
+      <c r="AB66" s="100" t="str">
         <f aca="false">IFERROR(Z66 / AA66, "")</f>
         <v/>
       </c>
       <c r="AC66" s="19"/>
       <c r="AE66" s="19"/>
       <c r="AF66" s="19"/>
-      <c r="AG66" s="96" t="str">
+      <c r="AG66" s="100" t="str">
         <f aca="false">IFERROR(AE66 / AF66, "")</f>
         <v/>
       </c>
       <c r="AH66" s="19"/>
       <c r="AJ66" s="19"/>
       <c r="AK66" s="19"/>
-      <c r="AL66" s="96" t="str">
+      <c r="AL66" s="100" t="str">
         <f aca="false">IFERROR(AJ66 / AK66, "")</f>
         <v/>
       </c>
       <c r="AM66" s="19"/>
       <c r="AO66" s="19"/>
       <c r="AP66" s="19"/>
-      <c r="AQ66" s="96" t="str">
+      <c r="AQ66" s="100" t="str">
         <f aca="false">IFERROR(AO66 / AP66, "")</f>
         <v/>
       </c>
@@ -9086,7 +9226,7 @@
       <c r="E114" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="45">
+  <mergeCells count="49">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="J1:L1"/>
@@ -9114,6 +9254,10 @@
     <mergeCell ref="H17:J17"/>
     <mergeCell ref="M17:O17"/>
     <mergeCell ref="Q18:S19"/>
+    <mergeCell ref="T18:W19"/>
+    <mergeCell ref="X18:Y18"/>
+    <mergeCell ref="Z18:AC19"/>
+    <mergeCell ref="X19:Y19"/>
     <mergeCell ref="Q20:R20"/>
     <mergeCell ref="Q21:R21"/>
     <mergeCell ref="Q22:R22"/>

</xml_diff>

<commit_message>
Excel export improvements: 1. Added shot map images to game stats. 2. Refactored the excel router for cleaner and more maintainable structure. (#47)
* Refactored excel exporting route functions to use a cleaner dependency (get_current_user_and_team) to get and validate both the user and team. Replaces previously used current user id to reduce duplicated validation inside the route functions.

* Refactores the routes.excel file to top level excel_router.py and separate submodules for each route. This improves maintainability and readability.

* WIP: Implemented some small abstractions and added Enums for better type representation

* Implemented shot map rendering to the game stats excel

* Updated requirements.txt
</commit_message>
<xml_diff>
--- a/backend/excels/game_stats_template.xlsx
+++ b/backend/excels/game_stats_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Game_Template" sheetId="1" state="visible" r:id="rId3"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="59">
   <si>
     <t xml:space="preserve">PVM:</t>
   </si>
@@ -146,6 +146,12 @@
     <t xml:space="preserve">YHTEENSÄ +</t>
   </si>
   <si>
+    <t xml:space="preserve">X = Maali</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O = Maalipaikka</t>
+  </si>
+  <si>
     <t xml:space="preserve">MAALIT</t>
   </si>
   <si>
@@ -206,7 +212,7 @@
     <numFmt numFmtId="168" formatCode="0.0%"/>
     <numFmt numFmtId="169" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,6 +295,28 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="36"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="36"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -423,6 +451,13 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
         <color rgb="FFFF0000"/>
       </left>
@@ -438,13 +473,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
-      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -497,7 +525,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="102">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -654,6 +682,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -706,6 +738,18 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -750,7 +794,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -758,11 +806,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -770,7 +818,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -786,7 +834,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -818,10 +866,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -850,7 +894,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -870,7 +914,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="17" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="15" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1081,8 +1125,8 @@
   </sheetPr>
   <dimension ref="A1:AR114"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X20" activeCellId="0" sqref="X20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1744,6 +1788,14 @@
       <c r="U13" s="27" t="n">
         <v>0</v>
       </c>
+      <c r="V13" s="39"/>
+      <c r="W13" s="39"/>
+      <c r="X13" s="39"/>
+      <c r="Y13" s="39"/>
+      <c r="Z13" s="39"/>
+      <c r="AA13" s="39"/>
+      <c r="AB13" s="39"/>
+      <c r="AC13" s="39"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="33" t="s">
@@ -1757,11 +1809,11 @@
         <f aca="false">IFERROR(C13 / C12,0)</f>
         <v>0</v>
       </c>
-      <c r="D14" s="39" t="n">
+      <c r="D14" s="40" t="n">
         <f aca="false">IFERROR(D13 / D12,0)</f>
         <v>0</v>
       </c>
-      <c r="E14" s="39" t="n">
+      <c r="E14" s="40" t="n">
         <f aca="false">IFERROR(E13 / E12,0)</f>
         <v>0</v>
       </c>
@@ -1773,11 +1825,11 @@
         <f aca="false">IFERROR(G13 / G12,0)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="39" t="n">
+      <c r="H14" s="40" t="n">
         <f aca="false">IFERROR(H13 / H12,0)</f>
         <v>0</v>
       </c>
-      <c r="I14" s="39" t="n">
+      <c r="I14" s="40" t="n">
         <f aca="false">IFERROR(I13 / I12,0)</f>
         <v>0</v>
       </c>
@@ -1789,11 +1841,11 @@
         <f aca="false">IFERROR(K13 / K12,0)</f>
         <v>0</v>
       </c>
-      <c r="L14" s="39" t="n">
+      <c r="L14" s="40" t="n">
         <f aca="false">IFERROR(L13 / L12,0)</f>
         <v>0</v>
       </c>
-      <c r="M14" s="39" t="n">
+      <c r="M14" s="40" t="n">
         <f aca="false">IFERROR(M13 / M12,0)</f>
         <v>0</v>
       </c>
@@ -1805,11 +1857,11 @@
         <f aca="false">IFERROR(O13 / O12,0)</f>
         <v>0</v>
       </c>
-      <c r="P14" s="39" t="n">
+      <c r="P14" s="40" t="n">
         <f aca="false">IFERROR(P13 / P12,0)</f>
         <v>0</v>
       </c>
-      <c r="Q14" s="39" t="n">
+      <c r="Q14" s="40" t="n">
         <f aca="false">IFERROR(Q13 / Q12,0)</f>
         <v>0</v>
       </c>
@@ -1821,7 +1873,7 @@
         <f aca="false">IFERROR(S13 / S12,0)</f>
         <v>0</v>
       </c>
-      <c r="T14" s="39" t="n">
+      <c r="T14" s="40" t="n">
         <f aca="false">IFERROR(T13 / T12,0)</f>
         <v>0</v>
       </c>
@@ -1829,6 +1881,14 @@
         <f aca="false">IFERROR(U13 / U12,0)</f>
         <v>0</v>
       </c>
+      <c r="V14" s="39"/>
+      <c r="W14" s="39"/>
+      <c r="X14" s="39"/>
+      <c r="Y14" s="39"/>
+      <c r="Z14" s="39"/>
+      <c r="AA14" s="39"/>
+      <c r="AB14" s="39"/>
+      <c r="AC14" s="39"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="31"/>
@@ -1867,29 +1927,29 @@
       <c r="U16" s="19"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="41" t="s">
         <v>35</v>
       </c>
       <c r="B17" s="19"/>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
-      <c r="H17" s="42" t="s">
+      <c r="H17" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
       <c r="K17" s="19"/>
       <c r="L17" s="19"/>
-      <c r="M17" s="41" t="s">
+      <c r="M17" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="N17" s="41"/>
-      <c r="O17" s="41"/>
+      <c r="N17" s="42"/>
+      <c r="O17" s="42"/>
       <c r="P17" s="19"/>
       <c r="Q17" s="19"/>
       <c r="R17" s="19"/>
@@ -1898,119 +1958,147 @@
       <c r="U17" s="19"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="44"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="50"/>
-      <c r="L18" s="48"/>
-      <c r="M18" s="49"/>
-      <c r="N18" s="49"/>
-      <c r="O18" s="45"/>
-      <c r="P18" s="50"/>
-      <c r="Q18" s="51" t="s">
+      <c r="B18" s="45"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="51"/>
+      <c r="L18" s="49"/>
+      <c r="M18" s="50"/>
+      <c r="N18" s="50"/>
+      <c r="O18" s="46"/>
+      <c r="P18" s="51"/>
+      <c r="Q18" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="R18" s="51"/>
-      <c r="S18" s="51"/>
-      <c r="T18" s="19"/>
-      <c r="U18" s="19"/>
+      <c r="R18" s="52"/>
+      <c r="S18" s="52"/>
+      <c r="T18" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="U18" s="53"/>
+      <c r="V18" s="53"/>
+      <c r="W18" s="53"/>
+      <c r="X18" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y18" s="54"/>
+      <c r="Z18" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA18" s="55"/>
+      <c r="AB18" s="55"/>
+      <c r="AC18" s="55"/>
+      <c r="AD18" s="39"/>
+      <c r="AE18" s="39"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="52"/>
-      <c r="B19" s="53"/>
-      <c r="C19" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" s="57"/>
-      <c r="G19" s="58"/>
-      <c r="H19" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="J19" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="K19" s="59"/>
-      <c r="L19" s="58"/>
-      <c r="M19" s="60" t="n">
+      <c r="A19" s="56"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="59" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="61"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="59" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" s="63"/>
+      <c r="L19" s="62"/>
+      <c r="M19" s="64" t="n">
         <f aca="false">IFERROR(C19 / H19,0)</f>
         <v>0</v>
       </c>
-      <c r="N19" s="61" t="n">
+      <c r="N19" s="65" t="n">
         <f aca="false">IFERROR(D19 / I19,0)</f>
         <v>0</v>
       </c>
-      <c r="O19" s="62" t="n">
+      <c r="O19" s="66" t="n">
         <f aca="false">IFERROR(E19 / J19,0)</f>
         <v>0</v>
       </c>
-      <c r="P19" s="59"/>
-      <c r="Q19" s="51"/>
-      <c r="R19" s="51"/>
-      <c r="S19" s="51"/>
-      <c r="T19" s="19"/>
-      <c r="U19" s="19"/>
+      <c r="P19" s="63"/>
+      <c r="Q19" s="52"/>
+      <c r="R19" s="52"/>
+      <c r="S19" s="52"/>
+      <c r="T19" s="53"/>
+      <c r="U19" s="53"/>
+      <c r="V19" s="53"/>
+      <c r="W19" s="53"/>
+      <c r="X19" s="67" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y19" s="67"/>
+      <c r="Z19" s="55"/>
+      <c r="AA19" s="55"/>
+      <c r="AB19" s="55"/>
+      <c r="AC19" s="55"/>
+      <c r="AD19" s="39"/>
+      <c r="AE19" s="39"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="52"/>
-      <c r="B20" s="53"/>
-      <c r="C20" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" s="57"/>
-      <c r="G20" s="58"/>
-      <c r="H20" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="J20" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="K20" s="59"/>
-      <c r="L20" s="58"/>
-      <c r="M20" s="66" t="n">
+      <c r="A20" s="56"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="61"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" s="63"/>
+      <c r="L20" s="62"/>
+      <c r="M20" s="71" t="n">
         <f aca="false">IFERROR(C20 / H20,0)</f>
         <v>0</v>
       </c>
-      <c r="N20" s="67" t="n">
+      <c r="N20" s="72" t="n">
         <f aca="false">IFERROR(D20 / I20,0)</f>
         <v>0</v>
       </c>
-      <c r="O20" s="68" t="n">
+      <c r="O20" s="73" t="n">
         <f aca="false">IFERROR(E20 / J20,0)</f>
         <v>0</v>
       </c>
-      <c r="P20" s="59"/>
-      <c r="Q20" s="69" t="s">
-        <v>41</v>
-      </c>
-      <c r="R20" s="69"/>
-      <c r="S20" s="70" t="n">
+      <c r="P20" s="63"/>
+      <c r="Q20" s="74" t="s">
+        <v>43</v>
+      </c>
+      <c r="R20" s="74"/>
+      <c r="S20" s="75" t="n">
         <f aca="false">SUM(B13,D13,F13,H13,J13,L13,N13,P13,R13,T13)</f>
         <v>0</v>
       </c>
@@ -2018,74 +2106,74 @@
       <c r="U20" s="19"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="52"/>
-      <c r="B21" s="53"/>
-      <c r="C21" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" s="71" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" s="57"/>
-      <c r="G21" s="58"/>
-      <c r="H21" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="I21" s="71" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" s="59"/>
-      <c r="L21" s="58"/>
-      <c r="M21" s="66" t="n">
+      <c r="A21" s="56"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="61"/>
+      <c r="G21" s="62"/>
+      <c r="H21" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" s="63"/>
+      <c r="L21" s="62"/>
+      <c r="M21" s="71" t="n">
         <f aca="false">IFERROR(C21 / H21,0)</f>
         <v>0</v>
       </c>
-      <c r="N21" s="67" t="n">
+      <c r="N21" s="72" t="n">
         <f aca="false">IFERROR(D21 / I21,0)</f>
         <v>0</v>
       </c>
-      <c r="O21" s="68" t="n">
+      <c r="O21" s="73" t="n">
         <f aca="false">IFERROR(E21 / J21,0)</f>
         <v>0</v>
       </c>
-      <c r="P21" s="59"/>
-      <c r="Q21" s="69" t="s">
-        <v>42</v>
-      </c>
-      <c r="R21" s="69"/>
-      <c r="S21" s="70" t="n">
+      <c r="P21" s="63"/>
+      <c r="Q21" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="R21" s="74"/>
+      <c r="S21" s="75" t="n">
         <f aca="false">SUM(B12,D12,F12,H12,J12,L12,N12,P12,R12,T12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="72"/>
-      <c r="B22" s="73"/>
-      <c r="C22" s="74"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="74"/>
-      <c r="F22" s="75"/>
-      <c r="G22" s="73"/>
-      <c r="H22" s="74"/>
-      <c r="I22" s="74"/>
-      <c r="J22" s="74"/>
-      <c r="K22" s="75"/>
-      <c r="L22" s="73"/>
-      <c r="M22" s="74"/>
-      <c r="N22" s="74"/>
-      <c r="O22" s="74"/>
-      <c r="P22" s="75"/>
-      <c r="Q22" s="69" t="s">
-        <v>43</v>
-      </c>
-      <c r="R22" s="69"/>
-      <c r="S22" s="76" t="n">
+      <c r="A22" s="77"/>
+      <c r="B22" s="78"/>
+      <c r="C22" s="79"/>
+      <c r="D22" s="79"/>
+      <c r="E22" s="79"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="78"/>
+      <c r="H22" s="79"/>
+      <c r="I22" s="79"/>
+      <c r="J22" s="79"/>
+      <c r="K22" s="80"/>
+      <c r="L22" s="78"/>
+      <c r="M22" s="79"/>
+      <c r="N22" s="79"/>
+      <c r="O22" s="79"/>
+      <c r="P22" s="80"/>
+      <c r="Q22" s="74" t="s">
+        <v>45</v>
+      </c>
+      <c r="R22" s="74"/>
+      <c r="S22" s="81" t="n">
         <f aca="false">IFERROR(S20 / S21,0)</f>
         <v>0</v>
       </c>
@@ -2100,213 +2188,213 @@
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="18"/>
       <c r="B24" s="19"/>
-      <c r="C24" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
+      <c r="C24" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
       <c r="F24" s="19"/>
       <c r="G24" s="18"/>
-      <c r="H24" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
+      <c r="H24" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
       <c r="K24" s="19"/>
       <c r="L24" s="19"/>
-      <c r="M24" s="41" t="s">
+      <c r="M24" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="N24" s="41"/>
-      <c r="O24" s="41"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="42"/>
       <c r="P24" s="19"/>
       <c r="Q24" s="19"/>
       <c r="R24" s="19"/>
       <c r="S24" s="19"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="48"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="45"/>
-      <c r="K25" s="50"/>
-      <c r="L25" s="48"/>
-      <c r="M25" s="49"/>
-      <c r="N25" s="49"/>
-      <c r="O25" s="45"/>
-      <c r="P25" s="50"/>
-      <c r="Q25" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="R25" s="51"/>
-      <c r="S25" s="51"/>
+      <c r="A25" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="49"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="51"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="50"/>
+      <c r="N25" s="50"/>
+      <c r="O25" s="46"/>
+      <c r="P25" s="51"/>
+      <c r="Q25" s="52" t="s">
+        <v>49</v>
+      </c>
+      <c r="R25" s="52"/>
+      <c r="S25" s="52"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="52"/>
-      <c r="B26" s="58"/>
-      <c r="C26" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" s="59"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="I26" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="J26" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="K26" s="59"/>
-      <c r="L26" s="58"/>
-      <c r="M26" s="60" t="n">
+      <c r="A26" s="56"/>
+      <c r="B26" s="62"/>
+      <c r="C26" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="59" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="63"/>
+      <c r="G26" s="62"/>
+      <c r="H26" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" s="59" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" s="63"/>
+      <c r="L26" s="62"/>
+      <c r="M26" s="64" t="n">
         <f aca="false">IFERROR(C26 / H26,0)</f>
         <v>0</v>
       </c>
-      <c r="N26" s="61" t="n">
+      <c r="N26" s="65" t="n">
         <f aca="false">IFERROR(D26 / I26,0)</f>
         <v>0</v>
       </c>
-      <c r="O26" s="62" t="n">
+      <c r="O26" s="66" t="n">
         <f aca="false">IFERROR(E26 / J26,0)</f>
         <v>0</v>
       </c>
-      <c r="P26" s="59"/>
-      <c r="Q26" s="51"/>
-      <c r="R26" s="51"/>
-      <c r="S26" s="51"/>
+      <c r="P26" s="63"/>
+      <c r="Q26" s="52"/>
+      <c r="R26" s="52"/>
+      <c r="S26" s="52"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="52"/>
-      <c r="B27" s="58"/>
-      <c r="C27" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="D27" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="E27" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" s="59"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="I27" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="J27" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="K27" s="59"/>
-      <c r="L27" s="58"/>
-      <c r="M27" s="66" t="n">
+      <c r="A27" s="56"/>
+      <c r="B27" s="62"/>
+      <c r="C27" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="63"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" s="63"/>
+      <c r="L27" s="62"/>
+      <c r="M27" s="71" t="n">
         <f aca="false">IFERROR(C27 / H27,0)</f>
         <v>0</v>
       </c>
-      <c r="N27" s="67" t="n">
+      <c r="N27" s="72" t="n">
         <f aca="false">IFERROR(D27 / I27,0)</f>
         <v>0</v>
       </c>
-      <c r="O27" s="68" t="n">
+      <c r="O27" s="73" t="n">
         <f aca="false">IFERROR(E27 / J27,0)</f>
         <v>0</v>
       </c>
-      <c r="P27" s="59"/>
-      <c r="Q27" s="69" t="s">
-        <v>41</v>
-      </c>
-      <c r="R27" s="69"/>
-      <c r="S27" s="70" t="n">
+      <c r="P27" s="63"/>
+      <c r="Q27" s="74" t="s">
+        <v>43</v>
+      </c>
+      <c r="R27" s="74"/>
+      <c r="S27" s="75" t="n">
         <f aca="false">SUM(C13,E13,G13,I13,K13,M13,O13,Q13,S13,U13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="52"/>
-      <c r="B28" s="58"/>
-      <c r="C28" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="D28" s="71" t="n">
-        <v>0</v>
-      </c>
-      <c r="E28" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="F28" s="59"/>
-      <c r="G28" s="58"/>
-      <c r="H28" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="I28" s="71" t="n">
-        <v>0</v>
-      </c>
-      <c r="J28" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="K28" s="59"/>
-      <c r="L28" s="58"/>
-      <c r="M28" s="66" t="n">
+      <c r="A28" s="56"/>
+      <c r="B28" s="62"/>
+      <c r="C28" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="63"/>
+      <c r="G28" s="62"/>
+      <c r="H28" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" s="63"/>
+      <c r="L28" s="62"/>
+      <c r="M28" s="71" t="n">
         <f aca="false">IFERROR(C28 / H28,0)</f>
         <v>0</v>
       </c>
-      <c r="N28" s="67" t="n">
+      <c r="N28" s="72" t="n">
         <f aca="false">IFERROR(D28 / I28,0)</f>
         <v>0</v>
       </c>
-      <c r="O28" s="68" t="n">
+      <c r="O28" s="73" t="n">
         <f aca="false">IFERROR(E28 / J28,0)</f>
         <v>0</v>
       </c>
-      <c r="P28" s="59"/>
-      <c r="Q28" s="69" t="s">
-        <v>42</v>
-      </c>
-      <c r="R28" s="69"/>
-      <c r="S28" s="70" t="n">
+      <c r="P28" s="63"/>
+      <c r="Q28" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="R28" s="74"/>
+      <c r="S28" s="75" t="n">
         <f aca="false">SUM(C12,E12,G12,I12,K12,M12,O12,Q12,S12,U12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="72"/>
-      <c r="B29" s="73"/>
-      <c r="C29" s="74"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="75"/>
-      <c r="G29" s="73"/>
-      <c r="H29" s="74"/>
-      <c r="I29" s="74"/>
-      <c r="J29" s="74"/>
-      <c r="K29" s="75"/>
-      <c r="L29" s="73"/>
-      <c r="M29" s="74"/>
-      <c r="N29" s="74"/>
-      <c r="O29" s="74"/>
-      <c r="P29" s="75"/>
-      <c r="Q29" s="69" t="s">
-        <v>43</v>
-      </c>
-      <c r="R29" s="69"/>
-      <c r="S29" s="76" t="n">
+      <c r="A29" s="77"/>
+      <c r="B29" s="78"/>
+      <c r="C29" s="79"/>
+      <c r="D29" s="79"/>
+      <c r="E29" s="79"/>
+      <c r="F29" s="80"/>
+      <c r="G29" s="78"/>
+      <c r="H29" s="79"/>
+      <c r="I29" s="79"/>
+      <c r="J29" s="79"/>
+      <c r="K29" s="80"/>
+      <c r="L29" s="78"/>
+      <c r="M29" s="79"/>
+      <c r="N29" s="79"/>
+      <c r="O29" s="79"/>
+      <c r="P29" s="80"/>
+      <c r="Q29" s="74" t="s">
+        <v>45</v>
+      </c>
+      <c r="R29" s="74"/>
+      <c r="S29" s="81" t="n">
         <f aca="false">IFERROR(S27 / S28,0)</f>
         <v>0</v>
       </c>
@@ -2316,76 +2404,76 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="31"/>
-      <c r="C31" s="77"/>
-      <c r="D31" s="78"/>
-      <c r="E31" s="77"/>
-      <c r="F31" s="77"/>
-      <c r="G31" s="78"/>
-      <c r="H31" s="77"/>
-      <c r="I31" s="77"/>
-      <c r="J31" s="78"/>
-      <c r="K31" s="77"/>
-      <c r="L31" s="77"/>
-      <c r="M31" s="78"/>
-      <c r="N31" s="77"/>
-      <c r="O31" s="77"/>
-      <c r="P31" s="78"/>
-      <c r="Q31" s="77"/>
+      <c r="C31" s="82"/>
+      <c r="D31" s="83"/>
+      <c r="E31" s="82"/>
+      <c r="F31" s="82"/>
+      <c r="G31" s="83"/>
+      <c r="H31" s="82"/>
+      <c r="I31" s="82"/>
+      <c r="J31" s="83"/>
+      <c r="K31" s="82"/>
+      <c r="L31" s="82"/>
+      <c r="M31" s="83"/>
+      <c r="N31" s="82"/>
+      <c r="O31" s="82"/>
+      <c r="P31" s="83"/>
+      <c r="Q31" s="82"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="79" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" s="80"/>
-      <c r="C32" s="80"/>
-      <c r="D32" s="80"/>
-      <c r="E32" s="80"/>
-      <c r="F32" s="80"/>
-      <c r="G32" s="80"/>
-      <c r="H32" s="80"/>
-      <c r="I32" s="80"/>
-      <c r="J32" s="80"/>
-      <c r="K32" s="80"/>
-      <c r="L32" s="80"/>
-      <c r="M32" s="77"/>
-      <c r="N32" s="77"/>
-      <c r="O32" s="77"/>
-      <c r="P32" s="77"/>
-      <c r="Q32" s="77"/>
+      <c r="A32" s="84" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" s="39"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="39"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="39"/>
+      <c r="L32" s="39"/>
+      <c r="M32" s="82"/>
+      <c r="N32" s="82"/>
+      <c r="O32" s="82"/>
+      <c r="P32" s="82"/>
+      <c r="Q32" s="82"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="81" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33" s="82" t="s">
-        <v>50</v>
-      </c>
-      <c r="C33" s="82"/>
-      <c r="D33" s="83" t="s">
+      <c r="A33" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="E33" s="83"/>
-      <c r="F33" s="83" t="s">
+      <c r="B33" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="G33" s="83"/>
-      <c r="H33" s="84" t="s">
+      <c r="C33" s="86"/>
+      <c r="D33" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="I33" s="84"/>
-      <c r="J33" s="85" t="s">
+      <c r="E33" s="87"/>
+      <c r="F33" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="K33" s="85"/>
-      <c r="L33" s="80"/>
-      <c r="M33" s="77"/>
-      <c r="N33" s="77"/>
-      <c r="O33" s="77"/>
-      <c r="P33" s="77"/>
-      <c r="Q33" s="77"/>
+      <c r="G33" s="87"/>
+      <c r="H33" s="88" t="s">
+        <v>55</v>
+      </c>
+      <c r="I33" s="88"/>
+      <c r="J33" s="89" t="s">
+        <v>56</v>
+      </c>
+      <c r="K33" s="89"/>
+      <c r="L33" s="39"/>
+      <c r="M33" s="82"/>
+      <c r="N33" s="82"/>
+      <c r="O33" s="82"/>
+      <c r="P33" s="82"/>
+      <c r="Q33" s="82"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="86" t="s">
+      <c r="A34" s="90" t="s">
         <v>17</v>
       </c>
       <c r="B34" s="24" t="s">
@@ -2418,10 +2506,10 @@
       <c r="K34" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="L34" s="80"/>
+      <c r="L34" s="39"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="86" t="s">
+      <c r="A35" s="90" t="s">
         <v>20</v>
       </c>
       <c r="B35" s="26" t="n">
@@ -2454,7 +2542,7 @@
       <c r="K35" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="L35" s="80"/>
+      <c r="L35" s="39"/>
       <c r="M35" s="19"/>
       <c r="N35" s="19"/>
       <c r="O35" s="19"/>
@@ -2462,7 +2550,7 @@
       <c r="Q35" s="19"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="86" t="s">
+      <c r="A36" s="90" t="s">
         <v>21</v>
       </c>
       <c r="B36" s="26" t="n">
@@ -2495,62 +2583,62 @@
       <c r="K36" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="L36" s="80"/>
-      <c r="O36" s="41"/>
-      <c r="P36" s="41"/>
-      <c r="Q36" s="41"/>
-      <c r="R36" s="87"/>
+      <c r="L36" s="39"/>
+      <c r="O36" s="42"/>
+      <c r="P36" s="42"/>
+      <c r="Q36" s="42"/>
+      <c r="R36" s="91"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="88" t="s">
+      <c r="A37" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="89" t="n">
+      <c r="B37" s="93" t="n">
         <f aca="false">IFERROR(B36 / B35,0)</f>
         <v>0</v>
       </c>
-      <c r="C37" s="90" t="n">
+      <c r="C37" s="94" t="n">
         <f aca="false">IFERROR(C36 / C35,0)</f>
         <v>0</v>
       </c>
-      <c r="D37" s="89" t="n">
+      <c r="D37" s="93" t="n">
         <f aca="false">IFERROR(D36 / D35,0)</f>
         <v>0</v>
       </c>
-      <c r="E37" s="91" t="n">
+      <c r="E37" s="95" t="n">
         <f aca="false">IFERROR(E36 / E35,0)</f>
         <v>0</v>
       </c>
-      <c r="F37" s="90" t="n">
+      <c r="F37" s="94" t="n">
         <f aca="false">IFERROR(F36 / F35,0)</f>
         <v>0</v>
       </c>
-      <c r="G37" s="90" t="n">
+      <c r="G37" s="94" t="n">
         <f aca="false">IFERROR(G36 / G35,0)</f>
         <v>0</v>
       </c>
-      <c r="H37" s="89" t="n">
+      <c r="H37" s="93" t="n">
         <f aca="false">IFERROR(H36 / H35,0)</f>
         <v>0</v>
       </c>
-      <c r="I37" s="91" t="n">
+      <c r="I37" s="95" t="n">
         <f aca="false">IFERROR(I36 / I35,0)</f>
         <v>0</v>
       </c>
-      <c r="J37" s="90" t="n">
+      <c r="J37" s="94" t="n">
         <f aca="false">IFERROR(J36 / J35,0)</f>
         <v>0</v>
       </c>
-      <c r="K37" s="91" t="n">
+      <c r="K37" s="95" t="n">
         <f aca="false">IFERROR(K36 / K35,0)</f>
         <v>0</v>
       </c>
-      <c r="L37" s="80"/>
-      <c r="M37" s="78"/>
-      <c r="N37" s="77"/>
-      <c r="O37" s="77"/>
-      <c r="P37" s="78"/>
-      <c r="Q37" s="77"/>
+      <c r="L37" s="39"/>
+      <c r="M37" s="83"/>
+      <c r="N37" s="82"/>
+      <c r="O37" s="82"/>
+      <c r="P37" s="83"/>
+      <c r="Q37" s="82"/>
       <c r="R37" s="19"/>
       <c r="S37" s="19"/>
       <c r="T37" s="19"/>
@@ -2580,18 +2668,18 @@
       <c r="AR37" s="19"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="81" t="s">
-        <v>55</v>
+      <c r="A38" s="85" t="s">
+        <v>57</v>
       </c>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
-      <c r="D38" s="92" t="str">
+      <c r="D38" s="96" t="str">
         <f aca="false">O1</f>
         <v>YV Kerrat:</v>
       </c>
       <c r="E38" s="14"/>
       <c r="F38" s="14"/>
-      <c r="G38" s="92" t="str">
+      <c r="G38" s="96" t="str">
         <f aca="false">Q1</f>
         <v>AV Kerrat:</v>
       </c>
@@ -2599,12 +2687,12 @@
       <c r="I38" s="14"/>
       <c r="J38" s="14"/>
       <c r="K38" s="14"/>
-      <c r="L38" s="80"/>
-      <c r="M38" s="77"/>
-      <c r="N38" s="77"/>
-      <c r="O38" s="77"/>
-      <c r="P38" s="77"/>
-      <c r="Q38" s="77"/>
+      <c r="L38" s="39"/>
+      <c r="M38" s="82"/>
+      <c r="N38" s="82"/>
+      <c r="O38" s="82"/>
+      <c r="P38" s="82"/>
+      <c r="Q38" s="82"/>
       <c r="R38" s="19"/>
       <c r="S38" s="19"/>
       <c r="T38" s="19"/>
@@ -2634,30 +2722,30 @@
       <c r="AR38" s="19"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="88" t="s">
-        <v>56</v>
+      <c r="A39" s="92" t="s">
+        <v>58</v>
       </c>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
-      <c r="D39" s="93" t="n">
+      <c r="D39" s="97" t="n">
         <f aca="false">IFERROR(D35 / D38,0)</f>
         <v>0</v>
       </c>
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
-      <c r="G39" s="93" t="n">
+      <c r="G39" s="97" t="n">
         <f aca="false">IFERROR(G35 / G38,0)</f>
         <v>0</v>
       </c>
       <c r="H39" s="13"/>
-      <c r="I39" s="94"/>
-      <c r="J39" s="94"/>
+      <c r="I39" s="98"/>
+      <c r="J39" s="98"/>
       <c r="K39" s="13"/>
-      <c r="M39" s="77"/>
-      <c r="N39" s="77"/>
-      <c r="O39" s="77"/>
-      <c r="P39" s="77"/>
-      <c r="Q39" s="77"/>
+      <c r="M39" s="82"/>
+      <c r="N39" s="82"/>
+      <c r="O39" s="82"/>
+      <c r="P39" s="82"/>
+      <c r="Q39" s="82"/>
       <c r="R39" s="19"/>
       <c r="S39" s="19"/>
       <c r="T39" s="19"/>
@@ -2722,31 +2810,31 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="S41" s="19"/>
-      <c r="T41" s="95"/>
-      <c r="U41" s="95"/>
-      <c r="V41" s="95"/>
-      <c r="W41" s="95"/>
-      <c r="X41" s="95"/>
-      <c r="Y41" s="95"/>
-      <c r="Z41" s="95"/>
-      <c r="AA41" s="95"/>
-      <c r="AB41" s="95"/>
-      <c r="AC41" s="95"/>
-      <c r="AD41" s="95"/>
-      <c r="AE41" s="95"/>
+      <c r="T41" s="99"/>
+      <c r="U41" s="99"/>
+      <c r="V41" s="99"/>
+      <c r="W41" s="99"/>
+      <c r="X41" s="99"/>
+      <c r="Y41" s="99"/>
+      <c r="Z41" s="99"/>
+      <c r="AA41" s="99"/>
+      <c r="AB41" s="99"/>
+      <c r="AC41" s="99"/>
+      <c r="AD41" s="99"/>
+      <c r="AE41" s="99"/>
       <c r="AF41" s="19"/>
-      <c r="AG41" s="95"/>
-      <c r="AH41" s="95"/>
-      <c r="AI41" s="95"/>
-      <c r="AJ41" s="95"/>
-      <c r="AK41" s="95"/>
-      <c r="AL41" s="95"/>
-      <c r="AM41" s="95"/>
-      <c r="AN41" s="95"/>
-      <c r="AO41" s="95"/>
-      <c r="AP41" s="95"/>
-      <c r="AQ41" s="95"/>
-      <c r="AR41" s="95"/>
+      <c r="AG41" s="99"/>
+      <c r="AH41" s="99"/>
+      <c r="AI41" s="99"/>
+      <c r="AJ41" s="99"/>
+      <c r="AK41" s="99"/>
+      <c r="AL41" s="99"/>
+      <c r="AM41" s="99"/>
+      <c r="AN41" s="99"/>
+      <c r="AO41" s="99"/>
+      <c r="AP41" s="99"/>
+      <c r="AQ41" s="99"/>
+      <c r="AR41" s="99"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="18"/>
@@ -3592,7 +3680,7 @@
       <c r="A66" s="19"/>
       <c r="C66" s="19"/>
       <c r="D66" s="19"/>
-      <c r="E66" s="96" t="str">
+      <c r="E66" s="100" t="str">
         <f aca="false">IFERROR(C66 / D66, "")</f>
         <v/>
       </c>
@@ -3600,7 +3688,7 @@
       <c r="G66" s="19"/>
       <c r="I66" s="19"/>
       <c r="J66" s="19"/>
-      <c r="K66" s="96" t="str">
+      <c r="K66" s="100" t="str">
         <f aca="false">IFERROR(I66 / J66, "")</f>
         <v/>
       </c>
@@ -3608,7 +3696,7 @@
       <c r="M66" s="19"/>
       <c r="O66" s="19"/>
       <c r="P66" s="19"/>
-      <c r="Q66" s="96" t="str">
+      <c r="Q66" s="100" t="str">
         <f aca="false">IFERROR(O66 / P66, "")</f>
         <v/>
       </c>
@@ -3616,35 +3704,35 @@
       <c r="S66" s="19"/>
       <c r="U66" s="19"/>
       <c r="V66" s="19"/>
-      <c r="W66" s="96" t="str">
+      <c r="W66" s="100" t="str">
         <f aca="false">IFERROR(U66 / V66, "")</f>
         <v/>
       </c>
       <c r="X66" s="19"/>
       <c r="Z66" s="19"/>
       <c r="AA66" s="19"/>
-      <c r="AB66" s="96" t="str">
+      <c r="AB66" s="100" t="str">
         <f aca="false">IFERROR(Z66 / AA66, "")</f>
         <v/>
       </c>
       <c r="AC66" s="19"/>
       <c r="AE66" s="19"/>
       <c r="AF66" s="19"/>
-      <c r="AG66" s="96" t="str">
+      <c r="AG66" s="100" t="str">
         <f aca="false">IFERROR(AE66 / AF66, "")</f>
         <v/>
       </c>
       <c r="AH66" s="19"/>
       <c r="AJ66" s="19"/>
       <c r="AK66" s="19"/>
-      <c r="AL66" s="96" t="str">
+      <c r="AL66" s="100" t="str">
         <f aca="false">IFERROR(AJ66 / AK66, "")</f>
         <v/>
       </c>
       <c r="AM66" s="19"/>
       <c r="AO66" s="19"/>
       <c r="AP66" s="19"/>
-      <c r="AQ66" s="96" t="str">
+      <c r="AQ66" s="100" t="str">
         <f aca="false">IFERROR(AO66 / AP66, "")</f>
         <v/>
       </c>
@@ -5060,7 +5148,7 @@
       <c r="E114" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="46">
+  <mergeCells count="50">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="J1:L1"/>
@@ -5089,6 +5177,10 @@
     <mergeCell ref="H17:J17"/>
     <mergeCell ref="M17:O17"/>
     <mergeCell ref="Q18:S19"/>
+    <mergeCell ref="T18:W19"/>
+    <mergeCell ref="X18:Y18"/>
+    <mergeCell ref="Z18:AC19"/>
+    <mergeCell ref="X19:Y19"/>
     <mergeCell ref="Q20:R20"/>
     <mergeCell ref="Q21:R21"/>
     <mergeCell ref="Q22:R22"/>
@@ -5125,8 +5217,8 @@
   </sheetPr>
   <dimension ref="A1:AR114"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X20" activeCellId="0" sqref="X20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5146,14 +5238,14 @@
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
       <c r="F1" s="15"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="97"/>
-      <c r="N1" s="97"/>
+      <c r="G1" s="101"/>
+      <c r="H1" s="101"/>
+      <c r="I1" s="101"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="101"/>
+      <c r="N1" s="101"/>
       <c r="O1" s="18"/>
       <c r="P1" s="19"/>
       <c r="Q1" s="18"/>
@@ -5770,6 +5862,14 @@
       <c r="U13" s="27" t="n">
         <v>0</v>
       </c>
+      <c r="V13" s="39"/>
+      <c r="W13" s="39"/>
+      <c r="X13" s="39"/>
+      <c r="Y13" s="39"/>
+      <c r="Z13" s="39"/>
+      <c r="AA13" s="39"/>
+      <c r="AB13" s="39"/>
+      <c r="AC13" s="39"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="33" t="s">
@@ -5783,11 +5883,11 @@
         <f aca="false">IFERROR(C13 / C12,0)</f>
         <v>0</v>
       </c>
-      <c r="D14" s="39" t="n">
+      <c r="D14" s="40" t="n">
         <f aca="false">IFERROR(D13 / D12,0)</f>
         <v>0</v>
       </c>
-      <c r="E14" s="39" t="n">
+      <c r="E14" s="40" t="n">
         <f aca="false">IFERROR(E13 / E12,0)</f>
         <v>0</v>
       </c>
@@ -5799,11 +5899,11 @@
         <f aca="false">IFERROR(G13 / G12,0)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="39" t="n">
+      <c r="H14" s="40" t="n">
         <f aca="false">IFERROR(H13 / H12,0)</f>
         <v>0</v>
       </c>
-      <c r="I14" s="39" t="n">
+      <c r="I14" s="40" t="n">
         <f aca="false">IFERROR(I13 / I12,0)</f>
         <v>0</v>
       </c>
@@ -5815,11 +5915,11 @@
         <f aca="false">IFERROR(K13 / K12,0)</f>
         <v>0</v>
       </c>
-      <c r="L14" s="39" t="n">
+      <c r="L14" s="40" t="n">
         <f aca="false">IFERROR(L13 / L12,0)</f>
         <v>0</v>
       </c>
-      <c r="M14" s="39" t="n">
+      <c r="M14" s="40" t="n">
         <f aca="false">IFERROR(M13 / M12,0)</f>
         <v>0</v>
       </c>
@@ -5831,11 +5931,11 @@
         <f aca="false">IFERROR(O13 / O12,0)</f>
         <v>0</v>
       </c>
-      <c r="P14" s="39" t="n">
+      <c r="P14" s="40" t="n">
         <f aca="false">IFERROR(P13 / P12,0)</f>
         <v>0</v>
       </c>
-      <c r="Q14" s="39" t="n">
+      <c r="Q14" s="40" t="n">
         <f aca="false">IFERROR(Q13 / Q12,0)</f>
         <v>0</v>
       </c>
@@ -5847,7 +5947,7 @@
         <f aca="false">IFERROR(S13 / S12,0)</f>
         <v>0</v>
       </c>
-      <c r="T14" s="39" t="n">
+      <c r="T14" s="40" t="n">
         <f aca="false">IFERROR(T13 / T12,0)</f>
         <v>0</v>
       </c>
@@ -5855,6 +5955,14 @@
         <f aca="false">IFERROR(U13 / U12,0)</f>
         <v>0</v>
       </c>
+      <c r="V14" s="39"/>
+      <c r="W14" s="39"/>
+      <c r="X14" s="39"/>
+      <c r="Y14" s="39"/>
+      <c r="Z14" s="39"/>
+      <c r="AA14" s="39"/>
+      <c r="AB14" s="39"/>
+      <c r="AC14" s="39"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="31"/>
@@ -5893,29 +6001,29 @@
       <c r="U16" s="19"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="41" t="s">
         <v>35</v>
       </c>
       <c r="B17" s="19"/>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
-      <c r="H17" s="42" t="s">
+      <c r="H17" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
       <c r="K17" s="19"/>
       <c r="L17" s="19"/>
-      <c r="M17" s="41" t="s">
+      <c r="M17" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="N17" s="41"/>
-      <c r="O17" s="41"/>
+      <c r="N17" s="42"/>
+      <c r="O17" s="42"/>
       <c r="P17" s="19"/>
       <c r="Q17" s="19"/>
       <c r="R17" s="19"/>
@@ -5924,119 +6032,151 @@
       <c r="U17" s="19"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="44"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="50"/>
-      <c r="L18" s="48"/>
-      <c r="M18" s="49"/>
-      <c r="N18" s="49"/>
-      <c r="O18" s="45"/>
-      <c r="P18" s="50"/>
-      <c r="Q18" s="51" t="s">
+      <c r="B18" s="45"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="51"/>
+      <c r="L18" s="49"/>
+      <c r="M18" s="50"/>
+      <c r="N18" s="50"/>
+      <c r="O18" s="46"/>
+      <c r="P18" s="51"/>
+      <c r="Q18" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="R18" s="51"/>
-      <c r="S18" s="51"/>
-      <c r="T18" s="19"/>
-      <c r="U18" s="19"/>
+      <c r="R18" s="52"/>
+      <c r="S18" s="52"/>
+      <c r="T18" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="U18" s="53"/>
+      <c r="V18" s="53"/>
+      <c r="W18" s="53"/>
+      <c r="X18" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y18" s="54"/>
+      <c r="Z18" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA18" s="55"/>
+      <c r="AB18" s="55"/>
+      <c r="AC18" s="55"/>
+      <c r="AD18" s="39"/>
+      <c r="AE18" s="39"/>
+      <c r="AF18" s="39"/>
+      <c r="AG18" s="39"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="52"/>
-      <c r="B19" s="53"/>
-      <c r="C19" s="54" t="n">
+      <c r="A19" s="56"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="58" t="n">
         <v>1</v>
       </c>
-      <c r="D19" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" s="57"/>
-      <c r="G19" s="58"/>
-      <c r="H19" s="54" t="n">
+      <c r="D19" s="59" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="61"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="58" t="n">
         <v>3</v>
       </c>
-      <c r="I19" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="J19" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="K19" s="59"/>
-      <c r="L19" s="58"/>
-      <c r="M19" s="60" t="n">
+      <c r="I19" s="59" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" s="63"/>
+      <c r="L19" s="62"/>
+      <c r="M19" s="64" t="n">
         <f aca="false">IFERROR(C19 / H19,0)</f>
         <v>0.333333333333333</v>
       </c>
-      <c r="N19" s="61" t="n">
+      <c r="N19" s="65" t="n">
         <f aca="false">IFERROR(D19 / I19,0)</f>
         <v>0</v>
       </c>
-      <c r="O19" s="62" t="n">
+      <c r="O19" s="66" t="n">
         <f aca="false">IFERROR(E19 / J19,0)</f>
         <v>0</v>
       </c>
-      <c r="P19" s="59"/>
-      <c r="Q19" s="51"/>
-      <c r="R19" s="51"/>
-      <c r="S19" s="51"/>
-      <c r="T19" s="19"/>
-      <c r="U19" s="19"/>
+      <c r="P19" s="63"/>
+      <c r="Q19" s="52"/>
+      <c r="R19" s="52"/>
+      <c r="S19" s="52"/>
+      <c r="T19" s="53"/>
+      <c r="U19" s="53"/>
+      <c r="V19" s="53"/>
+      <c r="W19" s="53"/>
+      <c r="X19" s="67" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y19" s="67"/>
+      <c r="Z19" s="55"/>
+      <c r="AA19" s="55"/>
+      <c r="AB19" s="55"/>
+      <c r="AC19" s="55"/>
+      <c r="AD19" s="39"/>
+      <c r="AE19" s="39"/>
+      <c r="AF19" s="39"/>
+      <c r="AG19" s="39"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="52"/>
-      <c r="B20" s="53"/>
-      <c r="C20" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" s="57"/>
-      <c r="G20" s="58"/>
-      <c r="H20" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="J20" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="K20" s="59"/>
-      <c r="L20" s="58"/>
-      <c r="M20" s="66" t="n">
+      <c r="A20" s="56"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="61"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" s="63"/>
+      <c r="L20" s="62"/>
+      <c r="M20" s="71" t="n">
         <f aca="false">IFERROR(C20 / H20,0)</f>
         <v>0</v>
       </c>
-      <c r="N20" s="67" t="n">
+      <c r="N20" s="72" t="n">
         <f aca="false">IFERROR(D20 / I20,0)</f>
         <v>0</v>
       </c>
-      <c r="O20" s="68" t="n">
+      <c r="O20" s="73" t="n">
         <f aca="false">IFERROR(E20 / J20,0)</f>
         <v>0</v>
       </c>
-      <c r="P20" s="59"/>
-      <c r="Q20" s="69" t="s">
-        <v>41</v>
-      </c>
-      <c r="R20" s="69"/>
-      <c r="S20" s="70" t="n">
+      <c r="P20" s="63"/>
+      <c r="Q20" s="74" t="s">
+        <v>43</v>
+      </c>
+      <c r="R20" s="74"/>
+      <c r="S20" s="75" t="n">
         <f aca="false">SUM(B13,D13,F13,H13,J13,L13,N13,P13,R13,T13)</f>
         <v>0</v>
       </c>
@@ -6044,74 +6184,74 @@
       <c r="U20" s="19"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="52"/>
-      <c r="B21" s="53"/>
-      <c r="C21" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" s="71" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" s="57"/>
-      <c r="G21" s="58"/>
-      <c r="H21" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="I21" s="71" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" s="59"/>
-      <c r="L21" s="58"/>
-      <c r="M21" s="66" t="n">
+      <c r="A21" s="56"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="61"/>
+      <c r="G21" s="62"/>
+      <c r="H21" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" s="63"/>
+      <c r="L21" s="62"/>
+      <c r="M21" s="71" t="n">
         <f aca="false">IFERROR(C21 / H21,0)</f>
         <v>0</v>
       </c>
-      <c r="N21" s="67" t="n">
+      <c r="N21" s="72" t="n">
         <f aca="false">IFERROR(D21 / I21,0)</f>
         <v>0</v>
       </c>
-      <c r="O21" s="68" t="n">
+      <c r="O21" s="73" t="n">
         <f aca="false">IFERROR(E21 / J21,0)</f>
         <v>0</v>
       </c>
-      <c r="P21" s="59"/>
-      <c r="Q21" s="69" t="s">
-        <v>42</v>
-      </c>
-      <c r="R21" s="69"/>
-      <c r="S21" s="70" t="n">
+      <c r="P21" s="63"/>
+      <c r="Q21" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="R21" s="74"/>
+      <c r="S21" s="75" t="n">
         <f aca="false">SUM(B12,D12,F12,H12,J12,L12,N12,P12,R12,T12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="72"/>
-      <c r="B22" s="73"/>
-      <c r="C22" s="74"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="74"/>
-      <c r="F22" s="75"/>
-      <c r="G22" s="73"/>
-      <c r="H22" s="74"/>
-      <c r="I22" s="74"/>
-      <c r="J22" s="74"/>
-      <c r="K22" s="75"/>
-      <c r="L22" s="73"/>
-      <c r="M22" s="74"/>
-      <c r="N22" s="74"/>
-      <c r="O22" s="74"/>
-      <c r="P22" s="75"/>
-      <c r="Q22" s="69" t="s">
-        <v>43</v>
-      </c>
-      <c r="R22" s="69"/>
-      <c r="S22" s="76" t="n">
+      <c r="A22" s="77"/>
+      <c r="B22" s="78"/>
+      <c r="C22" s="79"/>
+      <c r="D22" s="79"/>
+      <c r="E22" s="79"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="78"/>
+      <c r="H22" s="79"/>
+      <c r="I22" s="79"/>
+      <c r="J22" s="79"/>
+      <c r="K22" s="80"/>
+      <c r="L22" s="78"/>
+      <c r="M22" s="79"/>
+      <c r="N22" s="79"/>
+      <c r="O22" s="79"/>
+      <c r="P22" s="80"/>
+      <c r="Q22" s="74" t="s">
+        <v>45</v>
+      </c>
+      <c r="R22" s="74"/>
+      <c r="S22" s="81" t="n">
         <f aca="false">IFERROR(S20 / S21,0)</f>
         <v>0</v>
       </c>
@@ -6126,213 +6266,213 @@
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="18"/>
       <c r="B24" s="19"/>
-      <c r="C24" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
+      <c r="C24" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
       <c r="F24" s="19"/>
       <c r="G24" s="18"/>
-      <c r="H24" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
+      <c r="H24" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
       <c r="K24" s="19"/>
       <c r="L24" s="19"/>
-      <c r="M24" s="41" t="s">
+      <c r="M24" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="N24" s="41"/>
-      <c r="O24" s="41"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="42"/>
       <c r="P24" s="19"/>
       <c r="Q24" s="19"/>
       <c r="R24" s="19"/>
       <c r="S24" s="19"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="48"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="45"/>
-      <c r="K25" s="50"/>
-      <c r="L25" s="48"/>
-      <c r="M25" s="49"/>
-      <c r="N25" s="49"/>
-      <c r="O25" s="45"/>
-      <c r="P25" s="50"/>
-      <c r="Q25" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="R25" s="51"/>
-      <c r="S25" s="51"/>
+      <c r="A25" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="49"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="51"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="50"/>
+      <c r="N25" s="50"/>
+      <c r="O25" s="46"/>
+      <c r="P25" s="51"/>
+      <c r="Q25" s="52" t="s">
+        <v>49</v>
+      </c>
+      <c r="R25" s="52"/>
+      <c r="S25" s="52"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="52"/>
-      <c r="B26" s="58"/>
-      <c r="C26" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" s="59"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="I26" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="J26" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="K26" s="59"/>
-      <c r="L26" s="58"/>
-      <c r="M26" s="60" t="n">
+      <c r="A26" s="56"/>
+      <c r="B26" s="62"/>
+      <c r="C26" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="59" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="63"/>
+      <c r="G26" s="62"/>
+      <c r="H26" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" s="59" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" s="63"/>
+      <c r="L26" s="62"/>
+      <c r="M26" s="64" t="n">
         <f aca="false">IFERROR(C26 / H26,0)</f>
         <v>0</v>
       </c>
-      <c r="N26" s="61" t="n">
+      <c r="N26" s="65" t="n">
         <f aca="false">IFERROR(D26 / I26,0)</f>
         <v>0</v>
       </c>
-      <c r="O26" s="62" t="n">
+      <c r="O26" s="66" t="n">
         <f aca="false">IFERROR(E26 / J26,0)</f>
         <v>0</v>
       </c>
-      <c r="P26" s="59"/>
-      <c r="Q26" s="51"/>
-      <c r="R26" s="51"/>
-      <c r="S26" s="51"/>
+      <c r="P26" s="63"/>
+      <c r="Q26" s="52"/>
+      <c r="R26" s="52"/>
+      <c r="S26" s="52"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="52"/>
-      <c r="B27" s="58"/>
-      <c r="C27" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="D27" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="E27" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" s="59"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="I27" s="64" t="n">
-        <v>0</v>
-      </c>
-      <c r="J27" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="K27" s="59"/>
-      <c r="L27" s="58"/>
-      <c r="M27" s="66" t="n">
+      <c r="A27" s="56"/>
+      <c r="B27" s="62"/>
+      <c r="C27" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="63"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" s="63"/>
+      <c r="L27" s="62"/>
+      <c r="M27" s="71" t="n">
         <f aca="false">IFERROR(C27 / H27,0)</f>
         <v>0</v>
       </c>
-      <c r="N27" s="67" t="n">
+      <c r="N27" s="72" t="n">
         <f aca="false">IFERROR(D27 / I27,0)</f>
         <v>0</v>
       </c>
-      <c r="O27" s="68" t="n">
+      <c r="O27" s="73" t="n">
         <f aca="false">IFERROR(E27 / J27,0)</f>
         <v>0</v>
       </c>
-      <c r="P27" s="59"/>
-      <c r="Q27" s="69" t="s">
-        <v>41</v>
-      </c>
-      <c r="R27" s="69"/>
-      <c r="S27" s="70" t="n">
+      <c r="P27" s="63"/>
+      <c r="Q27" s="74" t="s">
+        <v>43</v>
+      </c>
+      <c r="R27" s="74"/>
+      <c r="S27" s="75" t="n">
         <f aca="false">SUM(C13,E13,G13,I13,K13,M13,O13,Q13,S13,U13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="52"/>
-      <c r="B28" s="58"/>
-      <c r="C28" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="D28" s="71" t="n">
-        <v>0</v>
-      </c>
-      <c r="E28" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="F28" s="59"/>
-      <c r="G28" s="58"/>
-      <c r="H28" s="63" t="n">
-        <v>0</v>
-      </c>
-      <c r="I28" s="71" t="n">
-        <v>0</v>
-      </c>
-      <c r="J28" s="65" t="n">
-        <v>0</v>
-      </c>
-      <c r="K28" s="59"/>
-      <c r="L28" s="58"/>
-      <c r="M28" s="66" t="n">
+      <c r="A28" s="56"/>
+      <c r="B28" s="62"/>
+      <c r="C28" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="63"/>
+      <c r="G28" s="62"/>
+      <c r="H28" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" s="63"/>
+      <c r="L28" s="62"/>
+      <c r="M28" s="71" t="n">
         <f aca="false">IFERROR(C28 / H28,0)</f>
         <v>0</v>
       </c>
-      <c r="N28" s="67" t="n">
+      <c r="N28" s="72" t="n">
         <f aca="false">IFERROR(D28 / I28,0)</f>
         <v>0</v>
       </c>
-      <c r="O28" s="68" t="n">
+      <c r="O28" s="73" t="n">
         <f aca="false">IFERROR(E28 / J28,0)</f>
         <v>0</v>
       </c>
-      <c r="P28" s="59"/>
-      <c r="Q28" s="69" t="s">
-        <v>42</v>
-      </c>
-      <c r="R28" s="69"/>
-      <c r="S28" s="70" t="n">
+      <c r="P28" s="63"/>
+      <c r="Q28" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="R28" s="74"/>
+      <c r="S28" s="75" t="n">
         <f aca="false">SUM(C12,E12,G12,I12,K12,M12,O12,Q12,S12,U12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="72"/>
-      <c r="B29" s="73"/>
-      <c r="C29" s="74"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="75"/>
-      <c r="G29" s="73"/>
-      <c r="H29" s="74"/>
-      <c r="I29" s="74"/>
-      <c r="J29" s="74"/>
-      <c r="K29" s="75"/>
-      <c r="L29" s="73"/>
-      <c r="M29" s="74"/>
-      <c r="N29" s="74"/>
-      <c r="O29" s="74"/>
-      <c r="P29" s="75"/>
-      <c r="Q29" s="69" t="s">
-        <v>43</v>
-      </c>
-      <c r="R29" s="69"/>
-      <c r="S29" s="76" t="n">
+      <c r="A29" s="77"/>
+      <c r="B29" s="78"/>
+      <c r="C29" s="79"/>
+      <c r="D29" s="79"/>
+      <c r="E29" s="79"/>
+      <c r="F29" s="80"/>
+      <c r="G29" s="78"/>
+      <c r="H29" s="79"/>
+      <c r="I29" s="79"/>
+      <c r="J29" s="79"/>
+      <c r="K29" s="80"/>
+      <c r="L29" s="78"/>
+      <c r="M29" s="79"/>
+      <c r="N29" s="79"/>
+      <c r="O29" s="79"/>
+      <c r="P29" s="80"/>
+      <c r="Q29" s="74" t="s">
+        <v>45</v>
+      </c>
+      <c r="R29" s="74"/>
+      <c r="S29" s="81" t="n">
         <f aca="false">IFERROR(S27 / S28,0)</f>
         <v>0</v>
       </c>
@@ -6342,76 +6482,76 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="31"/>
-      <c r="C31" s="77"/>
-      <c r="D31" s="78"/>
-      <c r="E31" s="77"/>
-      <c r="F31" s="77"/>
-      <c r="G31" s="78"/>
-      <c r="H31" s="77"/>
-      <c r="I31" s="77"/>
-      <c r="J31" s="78"/>
-      <c r="K31" s="77"/>
-      <c r="L31" s="77"/>
-      <c r="M31" s="78"/>
-      <c r="N31" s="77"/>
-      <c r="O31" s="77"/>
-      <c r="P31" s="78"/>
-      <c r="Q31" s="77"/>
+      <c r="C31" s="82"/>
+      <c r="D31" s="83"/>
+      <c r="E31" s="82"/>
+      <c r="F31" s="82"/>
+      <c r="G31" s="83"/>
+      <c r="H31" s="82"/>
+      <c r="I31" s="82"/>
+      <c r="J31" s="83"/>
+      <c r="K31" s="82"/>
+      <c r="L31" s="82"/>
+      <c r="M31" s="83"/>
+      <c r="N31" s="82"/>
+      <c r="O31" s="82"/>
+      <c r="P31" s="83"/>
+      <c r="Q31" s="82"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="79" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" s="80"/>
-      <c r="C32" s="80"/>
-      <c r="D32" s="80"/>
-      <c r="E32" s="80"/>
-      <c r="F32" s="80"/>
-      <c r="G32" s="80"/>
-      <c r="H32" s="80"/>
-      <c r="I32" s="80"/>
-      <c r="J32" s="80"/>
-      <c r="K32" s="80"/>
-      <c r="L32" s="80"/>
-      <c r="M32" s="77"/>
-      <c r="N32" s="77"/>
-      <c r="O32" s="77"/>
-      <c r="P32" s="77"/>
-      <c r="Q32" s="77"/>
+      <c r="A32" s="84" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" s="39"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="39"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="39"/>
+      <c r="L32" s="39"/>
+      <c r="M32" s="82"/>
+      <c r="N32" s="82"/>
+      <c r="O32" s="82"/>
+      <c r="P32" s="82"/>
+      <c r="Q32" s="82"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="81" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33" s="82" t="s">
-        <v>50</v>
-      </c>
-      <c r="C33" s="82"/>
-      <c r="D33" s="83" t="s">
+      <c r="A33" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="E33" s="83"/>
-      <c r="F33" s="83" t="s">
+      <c r="B33" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="G33" s="83"/>
-      <c r="H33" s="84" t="s">
+      <c r="C33" s="86"/>
+      <c r="D33" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="I33" s="84"/>
-      <c r="J33" s="85" t="s">
+      <c r="E33" s="87"/>
+      <c r="F33" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="K33" s="85"/>
-      <c r="L33" s="80"/>
-      <c r="M33" s="77"/>
-      <c r="N33" s="77"/>
-      <c r="O33" s="77"/>
-      <c r="P33" s="77"/>
-      <c r="Q33" s="77"/>
+      <c r="G33" s="87"/>
+      <c r="H33" s="88" t="s">
+        <v>55</v>
+      </c>
+      <c r="I33" s="88"/>
+      <c r="J33" s="89" t="s">
+        <v>56</v>
+      </c>
+      <c r="K33" s="89"/>
+      <c r="L33" s="39"/>
+      <c r="M33" s="82"/>
+      <c r="N33" s="82"/>
+      <c r="O33" s="82"/>
+      <c r="P33" s="82"/>
+      <c r="Q33" s="82"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="86" t="s">
+      <c r="A34" s="90" t="s">
         <v>17</v>
       </c>
       <c r="B34" s="24" t="s">
@@ -6444,10 +6584,10 @@
       <c r="K34" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="L34" s="80"/>
+      <c r="L34" s="39"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="86" t="s">
+      <c r="A35" s="90" t="s">
         <v>20</v>
       </c>
       <c r="B35" s="26" t="n">
@@ -6480,7 +6620,7 @@
       <c r="K35" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="L35" s="80"/>
+      <c r="L35" s="39"/>
       <c r="M35" s="19"/>
       <c r="N35" s="19"/>
       <c r="O35" s="19"/>
@@ -6488,7 +6628,7 @@
       <c r="Q35" s="19"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="86" t="s">
+      <c r="A36" s="90" t="s">
         <v>21</v>
       </c>
       <c r="B36" s="26" t="n">
@@ -6521,62 +6661,62 @@
       <c r="K36" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="L36" s="80"/>
-      <c r="O36" s="41"/>
-      <c r="P36" s="41"/>
-      <c r="Q36" s="41"/>
-      <c r="R36" s="87"/>
+      <c r="L36" s="39"/>
+      <c r="O36" s="42"/>
+      <c r="P36" s="42"/>
+      <c r="Q36" s="42"/>
+      <c r="R36" s="91"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="88" t="s">
+      <c r="A37" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="89" t="n">
+      <c r="B37" s="93" t="n">
         <f aca="false">IFERROR(B36 / B35,0)</f>
         <v>0</v>
       </c>
-      <c r="C37" s="90" t="n">
+      <c r="C37" s="94" t="n">
         <f aca="false">IFERROR(C36 / C35,0)</f>
         <v>0</v>
       </c>
-      <c r="D37" s="89" t="n">
+      <c r="D37" s="93" t="n">
         <f aca="false">IFERROR(D36 / D35,0)</f>
         <v>0</v>
       </c>
-      <c r="E37" s="91" t="n">
+      <c r="E37" s="95" t="n">
         <f aca="false">IFERROR(E36 / E35,0)</f>
         <v>0</v>
       </c>
-      <c r="F37" s="90" t="n">
+      <c r="F37" s="94" t="n">
         <f aca="false">IFERROR(F36 / F35,0)</f>
         <v>0</v>
       </c>
-      <c r="G37" s="90" t="n">
+      <c r="G37" s="94" t="n">
         <f aca="false">IFERROR(G36 / G35,0)</f>
         <v>0</v>
       </c>
-      <c r="H37" s="89" t="n">
+      <c r="H37" s="93" t="n">
         <f aca="false">IFERROR(H36 / H35,0)</f>
         <v>0</v>
       </c>
-      <c r="I37" s="91" t="n">
+      <c r="I37" s="95" t="n">
         <f aca="false">IFERROR(I36 / I35,0)</f>
         <v>0</v>
       </c>
-      <c r="J37" s="90" t="n">
+      <c r="J37" s="94" t="n">
         <f aca="false">IFERROR(J36 / J35,0)</f>
         <v>0</v>
       </c>
-      <c r="K37" s="91" t="n">
+      <c r="K37" s="95" t="n">
         <f aca="false">IFERROR(K36 / K35,0)</f>
         <v>0</v>
       </c>
-      <c r="L37" s="80"/>
-      <c r="M37" s="78"/>
-      <c r="N37" s="77"/>
-      <c r="O37" s="77"/>
-      <c r="P37" s="78"/>
-      <c r="Q37" s="77"/>
+      <c r="L37" s="39"/>
+      <c r="M37" s="83"/>
+      <c r="N37" s="82"/>
+      <c r="O37" s="82"/>
+      <c r="P37" s="83"/>
+      <c r="Q37" s="82"/>
       <c r="R37" s="19"/>
       <c r="S37" s="19"/>
       <c r="T37" s="19"/>
@@ -6606,18 +6746,18 @@
       <c r="AR37" s="19"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="81" t="s">
-        <v>55</v>
+      <c r="A38" s="85" t="s">
+        <v>57</v>
       </c>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
-      <c r="D38" s="92" t="n">
+      <c r="D38" s="96" t="n">
         <f aca="false">O1</f>
         <v>0</v>
       </c>
       <c r="E38" s="14"/>
       <c r="F38" s="14"/>
-      <c r="G38" s="92" t="n">
+      <c r="G38" s="96" t="n">
         <f aca="false">Q1</f>
         <v>0</v>
       </c>
@@ -6625,12 +6765,12 @@
       <c r="I38" s="14"/>
       <c r="J38" s="14"/>
       <c r="K38" s="14"/>
-      <c r="L38" s="80"/>
-      <c r="M38" s="77"/>
-      <c r="N38" s="77"/>
-      <c r="O38" s="77"/>
-      <c r="P38" s="77"/>
-      <c r="Q38" s="77"/>
+      <c r="L38" s="39"/>
+      <c r="M38" s="82"/>
+      <c r="N38" s="82"/>
+      <c r="O38" s="82"/>
+      <c r="P38" s="82"/>
+      <c r="Q38" s="82"/>
       <c r="R38" s="19"/>
       <c r="S38" s="19"/>
       <c r="T38" s="19"/>
@@ -6660,30 +6800,30 @@
       <c r="AR38" s="19"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="88" t="s">
-        <v>56</v>
+      <c r="A39" s="92" t="s">
+        <v>58</v>
       </c>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
-      <c r="D39" s="93" t="n">
+      <c r="D39" s="97" t="n">
         <f aca="false">IFERROR(D35 / D38,0)</f>
         <v>0</v>
       </c>
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
-      <c r="G39" s="93" t="n">
+      <c r="G39" s="97" t="n">
         <f aca="false">IFERROR(G35 / G38,0)</f>
         <v>0</v>
       </c>
       <c r="H39" s="13"/>
-      <c r="I39" s="94"/>
-      <c r="J39" s="94"/>
+      <c r="I39" s="98"/>
+      <c r="J39" s="98"/>
       <c r="K39" s="13"/>
-      <c r="M39" s="77"/>
-      <c r="N39" s="77"/>
-      <c r="O39" s="77"/>
-      <c r="P39" s="77"/>
-      <c r="Q39" s="77"/>
+      <c r="M39" s="82"/>
+      <c r="N39" s="82"/>
+      <c r="O39" s="82"/>
+      <c r="P39" s="82"/>
+      <c r="Q39" s="82"/>
       <c r="R39" s="19"/>
       <c r="S39" s="19"/>
       <c r="T39" s="19"/>
@@ -6748,31 +6888,31 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="S41" s="19"/>
-      <c r="T41" s="95"/>
-      <c r="U41" s="95"/>
-      <c r="V41" s="95"/>
-      <c r="W41" s="95"/>
-      <c r="X41" s="95"/>
-      <c r="Y41" s="95"/>
-      <c r="Z41" s="95"/>
-      <c r="AA41" s="95"/>
-      <c r="AB41" s="95"/>
-      <c r="AC41" s="95"/>
-      <c r="AD41" s="95"/>
-      <c r="AE41" s="95"/>
+      <c r="T41" s="99"/>
+      <c r="U41" s="99"/>
+      <c r="V41" s="99"/>
+      <c r="W41" s="99"/>
+      <c r="X41" s="99"/>
+      <c r="Y41" s="99"/>
+      <c r="Z41" s="99"/>
+      <c r="AA41" s="99"/>
+      <c r="AB41" s="99"/>
+      <c r="AC41" s="99"/>
+      <c r="AD41" s="99"/>
+      <c r="AE41" s="99"/>
       <c r="AF41" s="19"/>
-      <c r="AG41" s="95"/>
-      <c r="AH41" s="95"/>
-      <c r="AI41" s="95"/>
-      <c r="AJ41" s="95"/>
-      <c r="AK41" s="95"/>
-      <c r="AL41" s="95"/>
-      <c r="AM41" s="95"/>
-      <c r="AN41" s="95"/>
-      <c r="AO41" s="95"/>
-      <c r="AP41" s="95"/>
-      <c r="AQ41" s="95"/>
-      <c r="AR41" s="95"/>
+      <c r="AG41" s="99"/>
+      <c r="AH41" s="99"/>
+      <c r="AI41" s="99"/>
+      <c r="AJ41" s="99"/>
+      <c r="AK41" s="99"/>
+      <c r="AL41" s="99"/>
+      <c r="AM41" s="99"/>
+      <c r="AN41" s="99"/>
+      <c r="AO41" s="99"/>
+      <c r="AP41" s="99"/>
+      <c r="AQ41" s="99"/>
+      <c r="AR41" s="99"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="18"/>
@@ -7618,7 +7758,7 @@
       <c r="A66" s="19"/>
       <c r="C66" s="19"/>
       <c r="D66" s="19"/>
-      <c r="E66" s="96" t="str">
+      <c r="E66" s="100" t="str">
         <f aca="false">IFERROR(C66 / D66, "")</f>
         <v/>
       </c>
@@ -7626,7 +7766,7 @@
       <c r="G66" s="19"/>
       <c r="I66" s="19"/>
       <c r="J66" s="19"/>
-      <c r="K66" s="96" t="str">
+      <c r="K66" s="100" t="str">
         <f aca="false">IFERROR(I66 / J66, "")</f>
         <v/>
       </c>
@@ -7634,7 +7774,7 @@
       <c r="M66" s="19"/>
       <c r="O66" s="19"/>
       <c r="P66" s="19"/>
-      <c r="Q66" s="96" t="str">
+      <c r="Q66" s="100" t="str">
         <f aca="false">IFERROR(O66 / P66, "")</f>
         <v/>
       </c>
@@ -7642,35 +7782,35 @@
       <c r="S66" s="19"/>
       <c r="U66" s="19"/>
       <c r="V66" s="19"/>
-      <c r="W66" s="96" t="str">
+      <c r="W66" s="100" t="str">
         <f aca="false">IFERROR(U66 / V66, "")</f>
         <v/>
       </c>
       <c r="X66" s="19"/>
       <c r="Z66" s="19"/>
       <c r="AA66" s="19"/>
-      <c r="AB66" s="96" t="str">
+      <c r="AB66" s="100" t="str">
         <f aca="false">IFERROR(Z66 / AA66, "")</f>
         <v/>
       </c>
       <c r="AC66" s="19"/>
       <c r="AE66" s="19"/>
       <c r="AF66" s="19"/>
-      <c r="AG66" s="96" t="str">
+      <c r="AG66" s="100" t="str">
         <f aca="false">IFERROR(AE66 / AF66, "")</f>
         <v/>
       </c>
       <c r="AH66" s="19"/>
       <c r="AJ66" s="19"/>
       <c r="AK66" s="19"/>
-      <c r="AL66" s="96" t="str">
+      <c r="AL66" s="100" t="str">
         <f aca="false">IFERROR(AJ66 / AK66, "")</f>
         <v/>
       </c>
       <c r="AM66" s="19"/>
       <c r="AO66" s="19"/>
       <c r="AP66" s="19"/>
-      <c r="AQ66" s="96" t="str">
+      <c r="AQ66" s="100" t="str">
         <f aca="false">IFERROR(AO66 / AP66, "")</f>
         <v/>
       </c>
@@ -9086,7 +9226,7 @@
       <c r="E114" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="45">
+  <mergeCells count="49">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="J1:L1"/>
@@ -9114,6 +9254,10 @@
     <mergeCell ref="H17:J17"/>
     <mergeCell ref="M17:O17"/>
     <mergeCell ref="Q18:S19"/>
+    <mergeCell ref="T18:W19"/>
+    <mergeCell ref="X18:Y18"/>
+    <mergeCell ref="Z18:AC19"/>
+    <mergeCell ref="X19:Y19"/>
     <mergeCell ref="Q20:R20"/>
     <mergeCell ref="Q21:R21"/>
     <mergeCell ref="Q22:R22"/>

</xml_diff>

<commit_message>
Added penaltyshots as a shot type for player statstics. 1. Add PENALTY_SHOT to the ShotTypeTypes enum, and add this directly to postgresql db. 2. Add "Rangaistuslaukaus" as an answer option to player_stats_questions.json. 3. Updated the game stat and player summary excels to have a field for this. 4. Updated excel writing functionality to also calculate and write the penaltyshot values.
</commit_message>
<xml_diff>
--- a/backend/excels/game_stats_template.xlsx
+++ b/backend/excels/game_stats_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Game_Template" sheetId="1" state="visible" r:id="rId3"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="60">
   <si>
     <t xml:space="preserve">PVM:</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t xml:space="preserve">Ohjaus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rangaistuslaukaus</t>
   </si>
   <si>
     <t xml:space="preserve">MIHIN?</t>
@@ -1125,8 +1128,8 @@
   </sheetPr>
   <dimension ref="A1:AR114"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X20" activeCellId="0" sqref="X20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V10" activeCellId="0" sqref="V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1593,6 +1596,10 @@
         <v>34</v>
       </c>
       <c r="U10" s="22"/>
+      <c r="V10" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="W10" s="22"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="34" t="s">
@@ -1658,6 +1665,12 @@
       <c r="U11" s="36" t="s">
         <v>19</v>
       </c>
+      <c r="V11" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="W11" s="36" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="23" t="s">
@@ -1723,6 +1736,12 @@
       <c r="U12" s="27" t="n">
         <v>0</v>
       </c>
+      <c r="V12" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" s="27" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="38" t="s">
@@ -1788,8 +1807,12 @@
       <c r="U13" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="V13" s="39"/>
-      <c r="W13" s="39"/>
+      <c r="V13" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="W13" s="27" t="n">
+        <v>0</v>
+      </c>
       <c r="X13" s="39"/>
       <c r="Y13" s="39"/>
       <c r="Z13" s="39"/>
@@ -1881,8 +1904,14 @@
         <f aca="false">IFERROR(U13 / U12,0)</f>
         <v>0</v>
       </c>
-      <c r="V14" s="39"/>
-      <c r="W14" s="39"/>
+      <c r="V14" s="40" t="n">
+        <f aca="false">IFERROR(V13 / V12,0)</f>
+        <v>0</v>
+      </c>
+      <c r="W14" s="30" t="n">
+        <f aca="false">IFERROR(W13 / W12,0)</f>
+        <v>0</v>
+      </c>
       <c r="X14" s="39"/>
       <c r="Y14" s="39"/>
       <c r="Z14" s="39"/>
@@ -1928,25 +1957,25 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="41" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="42" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D17" s="42"/>
       <c r="E17" s="42"/>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
       <c r="H17" s="43" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I17" s="43"/>
       <c r="J17" s="43"/>
       <c r="K17" s="19"/>
       <c r="L17" s="19"/>
       <c r="M17" s="42" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N17" s="42"/>
       <c r="O17" s="42"/>
@@ -1959,7 +1988,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="44" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B18" s="45"/>
       <c r="C18" s="46"/>
@@ -1977,7 +2006,7 @@
       <c r="O18" s="46"/>
       <c r="P18" s="51"/>
       <c r="Q18" s="52" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="R18" s="52"/>
       <c r="S18" s="52"/>
@@ -1988,7 +2017,7 @@
       <c r="V18" s="53"/>
       <c r="W18" s="53"/>
       <c r="X18" s="54" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y18" s="54"/>
       <c r="Z18" s="55" t="s">
@@ -2046,7 +2075,7 @@
       <c r="V19" s="53"/>
       <c r="W19" s="53"/>
       <c r="X19" s="67" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Y19" s="67"/>
       <c r="Z19" s="55"/>
@@ -2095,7 +2124,7 @@
       </c>
       <c r="P20" s="63"/>
       <c r="Q20" s="74" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="R20" s="74"/>
       <c r="S20" s="75" t="n">
@@ -2144,7 +2173,7 @@
       </c>
       <c r="P21" s="63"/>
       <c r="Q21" s="74" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="R21" s="74"/>
       <c r="S21" s="75" t="n">
@@ -2170,7 +2199,7 @@
       <c r="O22" s="79"/>
       <c r="P22" s="80"/>
       <c r="Q22" s="74" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="R22" s="74"/>
       <c r="S22" s="81" t="n">
@@ -2189,21 +2218,21 @@
       <c r="A24" s="18"/>
       <c r="B24" s="19"/>
       <c r="C24" s="42" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D24" s="42"/>
       <c r="E24" s="42"/>
       <c r="F24" s="19"/>
       <c r="G24" s="18"/>
       <c r="H24" s="43" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I24" s="43"/>
       <c r="J24" s="43"/>
       <c r="K24" s="19"/>
       <c r="L24" s="19"/>
       <c r="M24" s="42" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N24" s="42"/>
       <c r="O24" s="42"/>
@@ -2214,7 +2243,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="44" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B25" s="49"/>
       <c r="C25" s="50"/>
@@ -2232,7 +2261,7 @@
       <c r="O25" s="46"/>
       <c r="P25" s="51"/>
       <c r="Q25" s="52" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="R25" s="52"/>
       <c r="S25" s="52"/>
@@ -2318,7 +2347,7 @@
       </c>
       <c r="P27" s="63"/>
       <c r="Q27" s="74" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="R27" s="74"/>
       <c r="S27" s="75" t="n">
@@ -2365,7 +2394,7 @@
       </c>
       <c r="P28" s="63"/>
       <c r="Q28" s="74" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="R28" s="74"/>
       <c r="S28" s="75" t="n">
@@ -2391,7 +2420,7 @@
       <c r="O29" s="79"/>
       <c r="P29" s="80"/>
       <c r="Q29" s="74" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="R29" s="74"/>
       <c r="S29" s="81" t="n">
@@ -2422,7 +2451,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="84" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B32" s="39"/>
       <c r="C32" s="39"/>
@@ -2443,26 +2472,26 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="85" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B33" s="86" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C33" s="86"/>
       <c r="D33" s="87" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E33" s="87"/>
       <c r="F33" s="87" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G33" s="87"/>
       <c r="H33" s="88" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I33" s="88"/>
       <c r="J33" s="89" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K33" s="89"/>
       <c r="L33" s="39"/>
@@ -2669,7 +2698,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="85" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
@@ -2723,7 +2752,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="92" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
@@ -5148,7 +5177,7 @@
       <c r="E114" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="50">
+  <mergeCells count="51">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="J1:L1"/>
@@ -5173,6 +5202,7 @@
     <mergeCell ref="P10:Q10"/>
     <mergeCell ref="R10:S10"/>
     <mergeCell ref="T10:U10"/>
+    <mergeCell ref="V10:W10"/>
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="H17:J17"/>
     <mergeCell ref="M17:O17"/>
@@ -5217,8 +5247,8 @@
   </sheetPr>
   <dimension ref="A1:AR114"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X20" activeCellId="0" sqref="X20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Z9" activeCellId="0" sqref="Z9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5667,6 +5697,10 @@
         <v>34</v>
       </c>
       <c r="U10" s="22"/>
+      <c r="V10" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="W10" s="22"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="34" t="s">
@@ -5732,6 +5766,12 @@
       <c r="U11" s="36" t="s">
         <v>19</v>
       </c>
+      <c r="V11" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="W11" s="36" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="23" t="s">
@@ -5797,6 +5837,12 @@
       <c r="U12" s="27" t="n">
         <v>0</v>
       </c>
+      <c r="V12" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" s="27" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="38" t="s">
@@ -5862,8 +5908,12 @@
       <c r="U13" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="V13" s="39"/>
-      <c r="W13" s="39"/>
+      <c r="V13" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="W13" s="27" t="n">
+        <v>0</v>
+      </c>
       <c r="X13" s="39"/>
       <c r="Y13" s="39"/>
       <c r="Z13" s="39"/>
@@ -5955,8 +6005,14 @@
         <f aca="false">IFERROR(U13 / U12,0)</f>
         <v>0</v>
       </c>
-      <c r="V14" s="39"/>
-      <c r="W14" s="39"/>
+      <c r="V14" s="40" t="n">
+        <f aca="false">IFERROR(V13 / V12,0)</f>
+        <v>0</v>
+      </c>
+      <c r="W14" s="30" t="n">
+        <f aca="false">IFERROR(W13 / W12,0)</f>
+        <v>0</v>
+      </c>
       <c r="X14" s="39"/>
       <c r="Y14" s="39"/>
       <c r="Z14" s="39"/>
@@ -6002,25 +6058,25 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="41" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="42" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D17" s="42"/>
       <c r="E17" s="42"/>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
       <c r="H17" s="43" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I17" s="43"/>
       <c r="J17" s="43"/>
       <c r="K17" s="19"/>
       <c r="L17" s="19"/>
       <c r="M17" s="42" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N17" s="42"/>
       <c r="O17" s="42"/>
@@ -6033,7 +6089,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="44" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B18" s="45"/>
       <c r="C18" s="46"/>
@@ -6051,7 +6107,7 @@
       <c r="O18" s="46"/>
       <c r="P18" s="51"/>
       <c r="Q18" s="52" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="R18" s="52"/>
       <c r="S18" s="52"/>
@@ -6062,7 +6118,7 @@
       <c r="V18" s="53"/>
       <c r="W18" s="53"/>
       <c r="X18" s="54" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y18" s="54"/>
       <c r="Z18" s="55" t="s">
@@ -6122,7 +6178,7 @@
       <c r="V19" s="53"/>
       <c r="W19" s="53"/>
       <c r="X19" s="67" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Y19" s="67"/>
       <c r="Z19" s="55"/>
@@ -6173,7 +6229,7 @@
       </c>
       <c r="P20" s="63"/>
       <c r="Q20" s="74" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="R20" s="74"/>
       <c r="S20" s="75" t="n">
@@ -6222,7 +6278,7 @@
       </c>
       <c r="P21" s="63"/>
       <c r="Q21" s="74" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="R21" s="74"/>
       <c r="S21" s="75" t="n">
@@ -6248,7 +6304,7 @@
       <c r="O22" s="79"/>
       <c r="P22" s="80"/>
       <c r="Q22" s="74" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="R22" s="74"/>
       <c r="S22" s="81" t="n">
@@ -6267,21 +6323,21 @@
       <c r="A24" s="18"/>
       <c r="B24" s="19"/>
       <c r="C24" s="42" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D24" s="42"/>
       <c r="E24" s="42"/>
       <c r="F24" s="19"/>
       <c r="G24" s="18"/>
       <c r="H24" s="43" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I24" s="43"/>
       <c r="J24" s="43"/>
       <c r="K24" s="19"/>
       <c r="L24" s="19"/>
       <c r="M24" s="42" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N24" s="42"/>
       <c r="O24" s="42"/>
@@ -6292,7 +6348,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="44" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B25" s="49"/>
       <c r="C25" s="50"/>
@@ -6310,7 +6366,7 @@
       <c r="O25" s="46"/>
       <c r="P25" s="51"/>
       <c r="Q25" s="52" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="R25" s="52"/>
       <c r="S25" s="52"/>
@@ -6396,7 +6452,7 @@
       </c>
       <c r="P27" s="63"/>
       <c r="Q27" s="74" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="R27" s="74"/>
       <c r="S27" s="75" t="n">
@@ -6443,7 +6499,7 @@
       </c>
       <c r="P28" s="63"/>
       <c r="Q28" s="74" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="R28" s="74"/>
       <c r="S28" s="75" t="n">
@@ -6469,7 +6525,7 @@
       <c r="O29" s="79"/>
       <c r="P29" s="80"/>
       <c r="Q29" s="74" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="R29" s="74"/>
       <c r="S29" s="81" t="n">
@@ -6500,7 +6556,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="84" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B32" s="39"/>
       <c r="C32" s="39"/>
@@ -6521,26 +6577,26 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="85" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B33" s="86" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C33" s="86"/>
       <c r="D33" s="87" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E33" s="87"/>
       <c r="F33" s="87" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G33" s="87"/>
       <c r="H33" s="88" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I33" s="88"/>
       <c r="J33" s="89" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K33" s="89"/>
       <c r="L33" s="39"/>
@@ -6747,7 +6803,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="85" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
@@ -6801,7 +6857,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="92" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
@@ -9226,7 +9282,7 @@
       <c r="E114" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="49">
+  <mergeCells count="50">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="J1:L1"/>
@@ -9250,6 +9306,7 @@
     <mergeCell ref="P10:Q10"/>
     <mergeCell ref="R10:S10"/>
     <mergeCell ref="T10:U10"/>
+    <mergeCell ref="V10:W10"/>
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="H17:J17"/>
     <mergeCell ref="M17:O17"/>

</xml_diff>

<commit_message>
Added Redis Cache to speed up /players routes (#49)
* Refactor and implement redis cache for the /players routes

* Add redis to requirements.txt
</commit_message>
<xml_diff>
--- a/backend/excels/game_stats_template.xlsx
+++ b/backend/excels/game_stats_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Game_Template" sheetId="1" state="visible" r:id="rId3"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="60">
   <si>
     <t xml:space="preserve">PVM:</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t xml:space="preserve">Ohjaus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rangaistuslaukaus</t>
   </si>
   <si>
     <t xml:space="preserve">MIHIN?</t>
@@ -1125,8 +1128,8 @@
   </sheetPr>
   <dimension ref="A1:AR114"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X20" activeCellId="0" sqref="X20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V10" activeCellId="0" sqref="V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1593,6 +1596,10 @@
         <v>34</v>
       </c>
       <c r="U10" s="22"/>
+      <c r="V10" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="W10" s="22"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="34" t="s">
@@ -1658,6 +1665,12 @@
       <c r="U11" s="36" t="s">
         <v>19</v>
       </c>
+      <c r="V11" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="W11" s="36" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="23" t="s">
@@ -1723,6 +1736,12 @@
       <c r="U12" s="27" t="n">
         <v>0</v>
       </c>
+      <c r="V12" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" s="27" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="38" t="s">
@@ -1788,8 +1807,12 @@
       <c r="U13" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="V13" s="39"/>
-      <c r="W13" s="39"/>
+      <c r="V13" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="W13" s="27" t="n">
+        <v>0</v>
+      </c>
       <c r="X13" s="39"/>
       <c r="Y13" s="39"/>
       <c r="Z13" s="39"/>
@@ -1881,8 +1904,14 @@
         <f aca="false">IFERROR(U13 / U12,0)</f>
         <v>0</v>
       </c>
-      <c r="V14" s="39"/>
-      <c r="W14" s="39"/>
+      <c r="V14" s="40" t="n">
+        <f aca="false">IFERROR(V13 / V12,0)</f>
+        <v>0</v>
+      </c>
+      <c r="W14" s="30" t="n">
+        <f aca="false">IFERROR(W13 / W12,0)</f>
+        <v>0</v>
+      </c>
       <c r="X14" s="39"/>
       <c r="Y14" s="39"/>
       <c r="Z14" s="39"/>
@@ -1928,25 +1957,25 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="41" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="42" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D17" s="42"/>
       <c r="E17" s="42"/>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
       <c r="H17" s="43" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I17" s="43"/>
       <c r="J17" s="43"/>
       <c r="K17" s="19"/>
       <c r="L17" s="19"/>
       <c r="M17" s="42" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N17" s="42"/>
       <c r="O17" s="42"/>
@@ -1959,7 +1988,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="44" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B18" s="45"/>
       <c r="C18" s="46"/>
@@ -1977,7 +2006,7 @@
       <c r="O18" s="46"/>
       <c r="P18" s="51"/>
       <c r="Q18" s="52" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="R18" s="52"/>
       <c r="S18" s="52"/>
@@ -1988,7 +2017,7 @@
       <c r="V18" s="53"/>
       <c r="W18" s="53"/>
       <c r="X18" s="54" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y18" s="54"/>
       <c r="Z18" s="55" t="s">
@@ -2046,7 +2075,7 @@
       <c r="V19" s="53"/>
       <c r="W19" s="53"/>
       <c r="X19" s="67" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Y19" s="67"/>
       <c r="Z19" s="55"/>
@@ -2095,7 +2124,7 @@
       </c>
       <c r="P20" s="63"/>
       <c r="Q20" s="74" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="R20" s="74"/>
       <c r="S20" s="75" t="n">
@@ -2144,7 +2173,7 @@
       </c>
       <c r="P21" s="63"/>
       <c r="Q21" s="74" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="R21" s="74"/>
       <c r="S21" s="75" t="n">
@@ -2170,7 +2199,7 @@
       <c r="O22" s="79"/>
       <c r="P22" s="80"/>
       <c r="Q22" s="74" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="R22" s="74"/>
       <c r="S22" s="81" t="n">
@@ -2189,21 +2218,21 @@
       <c r="A24" s="18"/>
       <c r="B24" s="19"/>
       <c r="C24" s="42" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D24" s="42"/>
       <c r="E24" s="42"/>
       <c r="F24" s="19"/>
       <c r="G24" s="18"/>
       <c r="H24" s="43" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I24" s="43"/>
       <c r="J24" s="43"/>
       <c r="K24" s="19"/>
       <c r="L24" s="19"/>
       <c r="M24" s="42" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N24" s="42"/>
       <c r="O24" s="42"/>
@@ -2214,7 +2243,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="44" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B25" s="49"/>
       <c r="C25" s="50"/>
@@ -2232,7 +2261,7 @@
       <c r="O25" s="46"/>
       <c r="P25" s="51"/>
       <c r="Q25" s="52" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="R25" s="52"/>
       <c r="S25" s="52"/>
@@ -2318,7 +2347,7 @@
       </c>
       <c r="P27" s="63"/>
       <c r="Q27" s="74" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="R27" s="74"/>
       <c r="S27" s="75" t="n">
@@ -2365,7 +2394,7 @@
       </c>
       <c r="P28" s="63"/>
       <c r="Q28" s="74" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="R28" s="74"/>
       <c r="S28" s="75" t="n">
@@ -2391,7 +2420,7 @@
       <c r="O29" s="79"/>
       <c r="P29" s="80"/>
       <c r="Q29" s="74" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="R29" s="74"/>
       <c r="S29" s="81" t="n">
@@ -2422,7 +2451,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="84" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B32" s="39"/>
       <c r="C32" s="39"/>
@@ -2443,26 +2472,26 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="85" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B33" s="86" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C33" s="86"/>
       <c r="D33" s="87" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E33" s="87"/>
       <c r="F33" s="87" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G33" s="87"/>
       <c r="H33" s="88" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I33" s="88"/>
       <c r="J33" s="89" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K33" s="89"/>
       <c r="L33" s="39"/>
@@ -2669,7 +2698,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="85" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
@@ -2723,7 +2752,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="92" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
@@ -5148,7 +5177,7 @@
       <c r="E114" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="50">
+  <mergeCells count="51">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="J1:L1"/>
@@ -5173,6 +5202,7 @@
     <mergeCell ref="P10:Q10"/>
     <mergeCell ref="R10:S10"/>
     <mergeCell ref="T10:U10"/>
+    <mergeCell ref="V10:W10"/>
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="H17:J17"/>
     <mergeCell ref="M17:O17"/>
@@ -5217,8 +5247,8 @@
   </sheetPr>
   <dimension ref="A1:AR114"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X20" activeCellId="0" sqref="X20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Z9" activeCellId="0" sqref="Z9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5667,6 +5697,10 @@
         <v>34</v>
       </c>
       <c r="U10" s="22"/>
+      <c r="V10" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="W10" s="22"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="34" t="s">
@@ -5732,6 +5766,12 @@
       <c r="U11" s="36" t="s">
         <v>19</v>
       </c>
+      <c r="V11" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="W11" s="36" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="23" t="s">
@@ -5797,6 +5837,12 @@
       <c r="U12" s="27" t="n">
         <v>0</v>
       </c>
+      <c r="V12" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" s="27" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="38" t="s">
@@ -5862,8 +5908,12 @@
       <c r="U13" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="V13" s="39"/>
-      <c r="W13" s="39"/>
+      <c r="V13" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="W13" s="27" t="n">
+        <v>0</v>
+      </c>
       <c r="X13" s="39"/>
       <c r="Y13" s="39"/>
       <c r="Z13" s="39"/>
@@ -5955,8 +6005,14 @@
         <f aca="false">IFERROR(U13 / U12,0)</f>
         <v>0</v>
       </c>
-      <c r="V14" s="39"/>
-      <c r="W14" s="39"/>
+      <c r="V14" s="40" t="n">
+        <f aca="false">IFERROR(V13 / V12,0)</f>
+        <v>0</v>
+      </c>
+      <c r="W14" s="30" t="n">
+        <f aca="false">IFERROR(W13 / W12,0)</f>
+        <v>0</v>
+      </c>
       <c r="X14" s="39"/>
       <c r="Y14" s="39"/>
       <c r="Z14" s="39"/>
@@ -6002,25 +6058,25 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="41" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="42" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D17" s="42"/>
       <c r="E17" s="42"/>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
       <c r="H17" s="43" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I17" s="43"/>
       <c r="J17" s="43"/>
       <c r="K17" s="19"/>
       <c r="L17" s="19"/>
       <c r="M17" s="42" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N17" s="42"/>
       <c r="O17" s="42"/>
@@ -6033,7 +6089,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="44" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B18" s="45"/>
       <c r="C18" s="46"/>
@@ -6051,7 +6107,7 @@
       <c r="O18" s="46"/>
       <c r="P18" s="51"/>
       <c r="Q18" s="52" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="R18" s="52"/>
       <c r="S18" s="52"/>
@@ -6062,7 +6118,7 @@
       <c r="V18" s="53"/>
       <c r="W18" s="53"/>
       <c r="X18" s="54" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y18" s="54"/>
       <c r="Z18" s="55" t="s">
@@ -6122,7 +6178,7 @@
       <c r="V19" s="53"/>
       <c r="W19" s="53"/>
       <c r="X19" s="67" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Y19" s="67"/>
       <c r="Z19" s="55"/>
@@ -6173,7 +6229,7 @@
       </c>
       <c r="P20" s="63"/>
       <c r="Q20" s="74" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="R20" s="74"/>
       <c r="S20" s="75" t="n">
@@ -6222,7 +6278,7 @@
       </c>
       <c r="P21" s="63"/>
       <c r="Q21" s="74" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="R21" s="74"/>
       <c r="S21" s="75" t="n">
@@ -6248,7 +6304,7 @@
       <c r="O22" s="79"/>
       <c r="P22" s="80"/>
       <c r="Q22" s="74" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="R22" s="74"/>
       <c r="S22" s="81" t="n">
@@ -6267,21 +6323,21 @@
       <c r="A24" s="18"/>
       <c r="B24" s="19"/>
       <c r="C24" s="42" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D24" s="42"/>
       <c r="E24" s="42"/>
       <c r="F24" s="19"/>
       <c r="G24" s="18"/>
       <c r="H24" s="43" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I24" s="43"/>
       <c r="J24" s="43"/>
       <c r="K24" s="19"/>
       <c r="L24" s="19"/>
       <c r="M24" s="42" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N24" s="42"/>
       <c r="O24" s="42"/>
@@ -6292,7 +6348,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="44" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B25" s="49"/>
       <c r="C25" s="50"/>
@@ -6310,7 +6366,7 @@
       <c r="O25" s="46"/>
       <c r="P25" s="51"/>
       <c r="Q25" s="52" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="R25" s="52"/>
       <c r="S25" s="52"/>
@@ -6396,7 +6452,7 @@
       </c>
       <c r="P27" s="63"/>
       <c r="Q27" s="74" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="R27" s="74"/>
       <c r="S27" s="75" t="n">
@@ -6443,7 +6499,7 @@
       </c>
       <c r="P28" s="63"/>
       <c r="Q28" s="74" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="R28" s="74"/>
       <c r="S28" s="75" t="n">
@@ -6469,7 +6525,7 @@
       <c r="O29" s="79"/>
       <c r="P29" s="80"/>
       <c r="Q29" s="74" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="R29" s="74"/>
       <c r="S29" s="81" t="n">
@@ -6500,7 +6556,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="84" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B32" s="39"/>
       <c r="C32" s="39"/>
@@ -6521,26 +6577,26 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="85" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B33" s="86" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C33" s="86"/>
       <c r="D33" s="87" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E33" s="87"/>
       <c r="F33" s="87" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G33" s="87"/>
       <c r="H33" s="88" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I33" s="88"/>
       <c r="J33" s="89" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K33" s="89"/>
       <c r="L33" s="39"/>
@@ -6747,7 +6803,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="85" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
@@ -6801,7 +6857,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="92" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
@@ -9226,7 +9282,7 @@
       <c r="E114" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="49">
+  <mergeCells count="50">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="J1:L1"/>
@@ -9250,6 +9306,7 @@
     <mergeCell ref="P10:Q10"/>
     <mergeCell ref="R10:S10"/>
     <mergeCell ref="T10:U10"/>
+    <mergeCell ref="V10:W10"/>
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="H17:J17"/>
     <mergeCell ref="M17:O17"/>

</xml_diff>